<commit_message>
Updated on 2018-11-11 at 19:11:14
</commit_message>
<xml_diff>
--- a/index.xlsx
+++ b/index.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Songs" sheetId="1" r:id="rId1"/>
+    <sheet name="Songs-Index" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -655,6 +655,11 @@
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="21.7109375" customWidth="1"/>
+    <col min="2" max="2" width="32.7109375" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="B1" s="1" t="s">

</xml_diff>

<commit_message>
Updated on 2018-11-11 at 19:44:46
</commit_message>
<xml_diff>
--- a/index.xlsx
+++ b/index.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="97">
   <si>
     <t>Song Title</t>
   </si>
@@ -148,6 +148,12 @@
     <t>Without You</t>
   </si>
   <si>
+    <t>Baby</t>
+  </si>
+  <si>
+    <t>Bad Liar</t>
+  </si>
+  <si>
     <t>Kodaline</t>
   </si>
   <si>
@@ -269,6 +275,12 @@
   </si>
   <si>
     <t>Unknown</t>
+  </si>
+  <si>
+    <t>Clean Bandit, Marina And The Diam</t>
+  </si>
+  <si>
+    <t>Selena Gomez</t>
   </si>
   <si>
     <t>29-9-2018</t>
@@ -650,14 +662,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D42"/>
+  <dimension ref="A1:D44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="21.7109375" customWidth="1"/>
-    <col min="2" max="2" width="32.7109375" customWidth="1"/>
+    <col min="2" max="2" width="34.7109375" customWidth="1"/>
     <col min="3" max="3" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -680,10 +692,10 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D2" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -694,10 +706,10 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D3" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -708,10 +720,10 @@
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D4" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -722,10 +734,10 @@
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D5" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -736,10 +748,10 @@
         <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D6" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -750,10 +762,10 @@
         <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D7" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -764,10 +776,10 @@
         <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D8" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -778,10 +790,10 @@
         <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D9" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -792,10 +804,10 @@
         <v>11</v>
       </c>
       <c r="C10" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D10" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -806,10 +818,10 @@
         <v>12</v>
       </c>
       <c r="C11" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D11" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -820,10 +832,10 @@
         <v>13</v>
       </c>
       <c r="C12" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D12" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -834,10 +846,10 @@
         <v>14</v>
       </c>
       <c r="C13" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D13" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -848,10 +860,10 @@
         <v>15</v>
       </c>
       <c r="C14" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D14" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -862,10 +874,10 @@
         <v>16</v>
       </c>
       <c r="C15" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D15" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -876,10 +888,10 @@
         <v>17</v>
       </c>
       <c r="C16" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D16" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -890,10 +902,10 @@
         <v>18</v>
       </c>
       <c r="C17" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D17" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -904,10 +916,10 @@
         <v>19</v>
       </c>
       <c r="C18" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D18" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -918,10 +930,10 @@
         <v>20</v>
       </c>
       <c r="C19" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D19" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -932,10 +944,10 @@
         <v>21</v>
       </c>
       <c r="C20" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D20" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -946,10 +958,10 @@
         <v>22</v>
       </c>
       <c r="C21" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D21" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -960,10 +972,10 @@
         <v>23</v>
       </c>
       <c r="C22" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D22" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -974,10 +986,10 @@
         <v>24</v>
       </c>
       <c r="C23" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D23" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -988,10 +1000,10 @@
         <v>25</v>
       </c>
       <c r="C24" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D24" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -1002,10 +1014,10 @@
         <v>26</v>
       </c>
       <c r="C25" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D25" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -1016,10 +1028,10 @@
         <v>27</v>
       </c>
       <c r="C26" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D26" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -1030,10 +1042,10 @@
         <v>28</v>
       </c>
       <c r="C27" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D27" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -1044,10 +1056,10 @@
         <v>29</v>
       </c>
       <c r="C28" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D28" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -1058,10 +1070,10 @@
         <v>30</v>
       </c>
       <c r="C29" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="D29" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -1072,10 +1084,10 @@
         <v>31</v>
       </c>
       <c r="C30" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D30" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -1086,10 +1098,10 @@
         <v>32</v>
       </c>
       <c r="C31" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="D31" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -1100,10 +1112,10 @@
         <v>33</v>
       </c>
       <c r="C32" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D32" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -1114,10 +1126,10 @@
         <v>34</v>
       </c>
       <c r="C33" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D33" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -1128,10 +1140,10 @@
         <v>35</v>
       </c>
       <c r="C34" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D34" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -1142,10 +1154,10 @@
         <v>36</v>
       </c>
       <c r="C35" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D35" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -1156,10 +1168,10 @@
         <v>37</v>
       </c>
       <c r="C36" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="D36" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -1170,10 +1182,10 @@
         <v>38</v>
       </c>
       <c r="C37" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="D37" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -1184,10 +1196,10 @@
         <v>39</v>
       </c>
       <c r="C38" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="D38" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -1198,10 +1210,10 @@
         <v>40</v>
       </c>
       <c r="C39" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D39" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -1212,10 +1224,10 @@
         <v>41</v>
       </c>
       <c r="C40" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D40" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -1226,10 +1238,10 @@
         <v>42</v>
       </c>
       <c r="C41" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="D41" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -1240,10 +1252,38 @@
         <v>43</v>
       </c>
       <c r="C42" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D42" t="s">
-        <v>92</v>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" s="1">
+        <v>41</v>
+      </c>
+      <c r="B43" t="s">
+        <v>44</v>
+      </c>
+      <c r="C43" t="s">
+        <v>87</v>
+      </c>
+      <c r="D43" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" s="1">
+        <v>42</v>
+      </c>
+      <c r="B44" t="s">
+        <v>45</v>
+      </c>
+      <c r="C44" t="s">
+        <v>88</v>
+      </c>
+      <c r="D44" t="s">
+        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated on 2018-11-12 at 15:01:22
</commit_message>
<xml_diff>
--- a/index.xlsx
+++ b/index.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="100">
   <si>
     <t>Song Title</t>
   </si>
@@ -154,6 +154,9 @@
     <t>Bad Liar</t>
   </si>
   <si>
+    <t>Wolves</t>
+  </si>
+  <si>
     <t>Kodaline</t>
   </si>
   <si>
@@ -283,6 +286,9 @@
     <t>Selena Gomez</t>
   </si>
   <si>
+    <t>Selena Gomez, Marshmello</t>
+  </si>
+  <si>
     <t>29-9-2018</t>
   </si>
   <si>
@@ -305,6 +311,9 @@
   </si>
   <si>
     <t>11-11-2018</t>
+  </si>
+  <si>
+    <t>12-11-2018</t>
   </si>
 </sst>
 </file>
@@ -662,7 +671,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D44"/>
+  <dimension ref="A1:D45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -692,10 +701,10 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -706,10 +715,10 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D3" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -720,10 +729,10 @@
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D4" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -734,10 +743,10 @@
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D5" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -748,10 +757,10 @@
         <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D6" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -762,10 +771,10 @@
         <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D7" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -776,10 +785,10 @@
         <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D8" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -790,10 +799,10 @@
         <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D9" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -804,10 +813,10 @@
         <v>11</v>
       </c>
       <c r="C10" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D10" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -818,10 +827,10 @@
         <v>12</v>
       </c>
       <c r="C11" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D11" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -832,10 +841,10 @@
         <v>13</v>
       </c>
       <c r="C12" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D12" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -846,10 +855,10 @@
         <v>14</v>
       </c>
       <c r="C13" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D13" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -860,10 +869,10 @@
         <v>15</v>
       </c>
       <c r="C14" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D14" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -874,10 +883,10 @@
         <v>16</v>
       </c>
       <c r="C15" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D15" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -888,10 +897,10 @@
         <v>17</v>
       </c>
       <c r="C16" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D16" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -902,10 +911,10 @@
         <v>18</v>
       </c>
       <c r="C17" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D17" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -916,10 +925,10 @@
         <v>19</v>
       </c>
       <c r="C18" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D18" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -930,10 +939,10 @@
         <v>20</v>
       </c>
       <c r="C19" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D19" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -944,10 +953,10 @@
         <v>21</v>
       </c>
       <c r="C20" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D20" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -958,10 +967,10 @@
         <v>22</v>
       </c>
       <c r="C21" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D21" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -972,10 +981,10 @@
         <v>23</v>
       </c>
       <c r="C22" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D22" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -986,10 +995,10 @@
         <v>24</v>
       </c>
       <c r="C23" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D23" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -1000,10 +1009,10 @@
         <v>25</v>
       </c>
       <c r="C24" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D24" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -1014,10 +1023,10 @@
         <v>26</v>
       </c>
       <c r="C25" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D25" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -1028,10 +1037,10 @@
         <v>27</v>
       </c>
       <c r="C26" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D26" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -1042,10 +1051,10 @@
         <v>28</v>
       </c>
       <c r="C27" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D27" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -1056,10 +1065,10 @@
         <v>29</v>
       </c>
       <c r="C28" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D28" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -1070,10 +1079,10 @@
         <v>30</v>
       </c>
       <c r="C29" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D29" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -1084,10 +1093,10 @@
         <v>31</v>
       </c>
       <c r="C30" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D30" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -1098,10 +1107,10 @@
         <v>32</v>
       </c>
       <c r="C31" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D31" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -1112,10 +1121,10 @@
         <v>33</v>
       </c>
       <c r="C32" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D32" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -1126,10 +1135,10 @@
         <v>34</v>
       </c>
       <c r="C33" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D33" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -1140,10 +1149,10 @@
         <v>35</v>
       </c>
       <c r="C34" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D34" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -1154,10 +1163,10 @@
         <v>36</v>
       </c>
       <c r="C35" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D35" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -1168,10 +1177,10 @@
         <v>37</v>
       </c>
       <c r="C36" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D36" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -1182,10 +1191,10 @@
         <v>38</v>
       </c>
       <c r="C37" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D37" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -1196,10 +1205,10 @@
         <v>39</v>
       </c>
       <c r="C38" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D38" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -1210,10 +1219,10 @@
         <v>40</v>
       </c>
       <c r="C39" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D39" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -1224,10 +1233,10 @@
         <v>41</v>
       </c>
       <c r="C40" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D40" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -1238,10 +1247,10 @@
         <v>42</v>
       </c>
       <c r="C41" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D41" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -1252,10 +1261,10 @@
         <v>43</v>
       </c>
       <c r="C42" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D42" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -1266,10 +1275,10 @@
         <v>44</v>
       </c>
       <c r="C43" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D43" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -1280,10 +1289,24 @@
         <v>45</v>
       </c>
       <c r="C44" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D44" t="s">
-        <v>96</v>
+        <v>98</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" s="1">
+        <v>43</v>
+      </c>
+      <c r="B45" t="s">
+        <v>46</v>
+      </c>
+      <c r="C45" t="s">
+        <v>90</v>
+      </c>
+      <c r="D45" t="s">
+        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated on 2018-11-16 at 02:10:26
</commit_message>
<xml_diff>
--- a/index.xlsx
+++ b/index.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="105">
   <si>
     <t>Song Title</t>
   </si>
@@ -157,6 +157,12 @@
     <t>Wolves</t>
   </si>
   <si>
+    <t>Sad_</t>
+  </si>
+  <si>
+    <t>No Brainer</t>
+  </si>
+  <si>
     <t>Kodaline</t>
   </si>
   <si>
@@ -289,6 +295,12 @@
     <t>Selena Gomez, Marshmello</t>
   </si>
   <si>
+    <t>XXXTENTACION</t>
+  </si>
+  <si>
+    <t>DJ Khaled, Justin Bieber, C</t>
+  </si>
+  <si>
     <t>29-9-2018</t>
   </si>
   <si>
@@ -314,6 +326,9 @@
   </si>
   <si>
     <t>12-11-2018</t>
+  </si>
+  <si>
+    <t>16-11-2018</t>
   </si>
 </sst>
 </file>
@@ -671,7 +686,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D45"/>
+  <dimension ref="A1:D47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -701,10 +716,10 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D2" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -715,10 +730,10 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D3" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -729,10 +744,10 @@
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D4" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -743,10 +758,10 @@
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D5" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -757,10 +772,10 @@
         <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D6" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -771,10 +786,10 @@
         <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D7" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -785,10 +800,10 @@
         <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D8" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -799,10 +814,10 @@
         <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D9" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -813,10 +828,10 @@
         <v>11</v>
       </c>
       <c r="C10" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D10" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -827,10 +842,10 @@
         <v>12</v>
       </c>
       <c r="C11" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D11" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -841,10 +856,10 @@
         <v>13</v>
       </c>
       <c r="C12" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D12" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -855,10 +870,10 @@
         <v>14</v>
       </c>
       <c r="C13" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D13" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -869,10 +884,10 @@
         <v>15</v>
       </c>
       <c r="C14" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D14" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -883,10 +898,10 @@
         <v>16</v>
       </c>
       <c r="C15" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D15" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -897,10 +912,10 @@
         <v>17</v>
       </c>
       <c r="C16" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D16" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -911,10 +926,10 @@
         <v>18</v>
       </c>
       <c r="C17" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D17" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -925,10 +940,10 @@
         <v>19</v>
       </c>
       <c r="C18" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D18" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -939,10 +954,10 @@
         <v>20</v>
       </c>
       <c r="C19" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D19" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -953,10 +968,10 @@
         <v>21</v>
       </c>
       <c r="C20" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D20" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -967,10 +982,10 @@
         <v>22</v>
       </c>
       <c r="C21" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D21" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -981,10 +996,10 @@
         <v>23</v>
       </c>
       <c r="C22" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D22" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -995,10 +1010,10 @@
         <v>24</v>
       </c>
       <c r="C23" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D23" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -1009,10 +1024,10 @@
         <v>25</v>
       </c>
       <c r="C24" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D24" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -1023,10 +1038,10 @@
         <v>26</v>
       </c>
       <c r="C25" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D25" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -1037,10 +1052,10 @@
         <v>27</v>
       </c>
       <c r="C26" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="D26" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -1051,10 +1066,10 @@
         <v>28</v>
       </c>
       <c r="C27" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D27" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -1065,10 +1080,10 @@
         <v>29</v>
       </c>
       <c r="C28" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="D28" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -1079,10 +1094,10 @@
         <v>30</v>
       </c>
       <c r="C29" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D29" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -1093,10 +1108,10 @@
         <v>31</v>
       </c>
       <c r="C30" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D30" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -1107,10 +1122,10 @@
         <v>32</v>
       </c>
       <c r="C31" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D31" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -1121,10 +1136,10 @@
         <v>33</v>
       </c>
       <c r="C32" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D32" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -1135,10 +1150,10 @@
         <v>34</v>
       </c>
       <c r="C33" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="D33" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -1149,10 +1164,10 @@
         <v>35</v>
       </c>
       <c r="C34" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="D34" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -1163,10 +1178,10 @@
         <v>36</v>
       </c>
       <c r="C35" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="D35" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -1177,10 +1192,10 @@
         <v>37</v>
       </c>
       <c r="C36" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D36" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -1191,10 +1206,10 @@
         <v>38</v>
       </c>
       <c r="C37" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D37" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -1205,10 +1220,10 @@
         <v>39</v>
       </c>
       <c r="C38" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="D38" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -1219,10 +1234,10 @@
         <v>40</v>
       </c>
       <c r="C39" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D39" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -1233,10 +1248,10 @@
         <v>41</v>
       </c>
       <c r="C40" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="D40" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -1247,10 +1262,10 @@
         <v>42</v>
       </c>
       <c r="C41" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D41" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -1261,10 +1276,10 @@
         <v>43</v>
       </c>
       <c r="C42" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D42" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -1275,10 +1290,10 @@
         <v>44</v>
       </c>
       <c r="C43" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="D43" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -1289,10 +1304,10 @@
         <v>45</v>
       </c>
       <c r="C44" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="D44" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -1303,10 +1318,38 @@
         <v>46</v>
       </c>
       <c r="C45" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D45" t="s">
-        <v>99</v>
+        <v>103</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" s="1">
+        <v>44</v>
+      </c>
+      <c r="B46" t="s">
+        <v>47</v>
+      </c>
+      <c r="C46" t="s">
+        <v>93</v>
+      </c>
+      <c r="D46" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" s="1">
+        <v>45</v>
+      </c>
+      <c r="B47" t="s">
+        <v>48</v>
+      </c>
+      <c r="C47" t="s">
+        <v>94</v>
+      </c>
+      <c r="D47" t="s">
+        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated on 2018-11-18 at 10:36:29
</commit_message>
<xml_diff>
--- a/index.xlsx
+++ b/index.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="115">
   <si>
     <t>Song Title</t>
   </si>
@@ -163,6 +163,21 @@
     <t>No Brainer</t>
   </si>
   <si>
+    <t>It Ain_t Me</t>
+  </si>
+  <si>
+    <t>Don_t Let Me Down</t>
+  </si>
+  <si>
+    <t>Complicated_Dimitri_Vegas_Like_Mike_D_[500kbps_M4A]</t>
+  </si>
+  <si>
+    <t>2U</t>
+  </si>
+  <si>
+    <t>Attention</t>
+  </si>
+  <si>
     <t>Kodaline</t>
   </si>
   <si>
@@ -301,6 +316,18 @@
     <t>DJ Khaled, Justin Bieber, C</t>
   </si>
   <si>
+    <t>Kygo, Selena Gomez</t>
+  </si>
+  <si>
+    <t>The Chainsmokers, Da</t>
+  </si>
+  <si>
+    <t>David Guetta, Justin Bieber</t>
+  </si>
+  <si>
+    <t>Charlie Puth</t>
+  </si>
+  <si>
     <t>29-9-2018</t>
   </si>
   <si>
@@ -329,6 +356,9 @@
   </si>
   <si>
     <t>16-11-2018</t>
+  </si>
+  <si>
+    <t>18-11-2018</t>
   </si>
 </sst>
 </file>
@@ -686,13 +716,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D47"/>
+  <dimension ref="A1:D52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.7109375" customWidth="1"/>
+    <col min="1" max="1" width="52.7109375" customWidth="1"/>
     <col min="2" max="2" width="34.7109375" customWidth="1"/>
     <col min="3" max="3" width="14.7109375" customWidth="1"/>
   </cols>
@@ -716,10 +746,10 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="D2" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -730,10 +760,10 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="D3" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -744,10 +774,10 @@
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="D4" t="s">
-        <v>96</v>
+        <v>105</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -758,10 +788,10 @@
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="D5" t="s">
-        <v>97</v>
+        <v>106</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -772,10 +802,10 @@
         <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="D6" t="s">
-        <v>97</v>
+        <v>106</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -786,10 +816,10 @@
         <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="D7" t="s">
-        <v>97</v>
+        <v>106</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -800,10 +830,10 @@
         <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="D8" t="s">
-        <v>97</v>
+        <v>106</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -814,10 +844,10 @@
         <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="D9" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -828,10 +858,10 @@
         <v>11</v>
       </c>
       <c r="C10" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="D10" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -842,10 +872,10 @@
         <v>12</v>
       </c>
       <c r="C11" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="D11" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -856,10 +886,10 @@
         <v>13</v>
       </c>
       <c r="C12" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="D12" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -870,10 +900,10 @@
         <v>14</v>
       </c>
       <c r="C13" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="D13" t="s">
-        <v>99</v>
+        <v>108</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -884,10 +914,10 @@
         <v>15</v>
       </c>
       <c r="C14" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="D14" t="s">
-        <v>99</v>
+        <v>108</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -898,10 +928,10 @@
         <v>16</v>
       </c>
       <c r="C15" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="D15" t="s">
-        <v>100</v>
+        <v>109</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -912,10 +942,10 @@
         <v>17</v>
       </c>
       <c r="C16" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="D16" t="s">
-        <v>100</v>
+        <v>109</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -926,10 +956,10 @@
         <v>18</v>
       </c>
       <c r="C17" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="D17" t="s">
-        <v>101</v>
+        <v>110</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -940,10 +970,10 @@
         <v>19</v>
       </c>
       <c r="C18" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="D18" t="s">
-        <v>101</v>
+        <v>110</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -954,10 +984,10 @@
         <v>20</v>
       </c>
       <c r="C19" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="D19" t="s">
-        <v>101</v>
+        <v>110</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -968,10 +998,10 @@
         <v>21</v>
       </c>
       <c r="C20" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="D20" t="s">
-        <v>101</v>
+        <v>110</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -982,10 +1012,10 @@
         <v>22</v>
       </c>
       <c r="C21" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="D21" t="s">
-        <v>101</v>
+        <v>110</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -996,10 +1026,10 @@
         <v>23</v>
       </c>
       <c r="C22" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="D22" t="s">
-        <v>101</v>
+        <v>110</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -1010,10 +1040,10 @@
         <v>24</v>
       </c>
       <c r="C23" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="D23" t="s">
-        <v>101</v>
+        <v>110</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -1024,10 +1054,10 @@
         <v>25</v>
       </c>
       <c r="C24" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="D24" t="s">
-        <v>101</v>
+        <v>110</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -1038,10 +1068,10 @@
         <v>26</v>
       </c>
       <c r="C25" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="D25" t="s">
-        <v>101</v>
+        <v>110</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -1052,10 +1082,10 @@
         <v>27</v>
       </c>
       <c r="C26" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="D26" t="s">
-        <v>101</v>
+        <v>110</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -1066,10 +1096,10 @@
         <v>28</v>
       </c>
       <c r="C27" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="D27" t="s">
-        <v>101</v>
+        <v>110</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -1080,10 +1110,10 @@
         <v>29</v>
       </c>
       <c r="C28" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="D28" t="s">
-        <v>101</v>
+        <v>110</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -1094,10 +1124,10 @@
         <v>30</v>
       </c>
       <c r="C29" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="D29" t="s">
-        <v>101</v>
+        <v>110</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -1108,10 +1138,10 @@
         <v>31</v>
       </c>
       <c r="C30" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="D30" t="s">
-        <v>101</v>
+        <v>110</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -1122,10 +1152,10 @@
         <v>32</v>
       </c>
       <c r="C31" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="D31" t="s">
-        <v>101</v>
+        <v>110</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -1136,10 +1166,10 @@
         <v>33</v>
       </c>
       <c r="C32" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="D32" t="s">
-        <v>101</v>
+        <v>110</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -1150,10 +1180,10 @@
         <v>34</v>
       </c>
       <c r="C33" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="D33" t="s">
-        <v>101</v>
+        <v>110</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -1164,10 +1194,10 @@
         <v>35</v>
       </c>
       <c r="C34" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="D34" t="s">
-        <v>101</v>
+        <v>110</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -1178,10 +1208,10 @@
         <v>36</v>
       </c>
       <c r="C35" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="D35" t="s">
-        <v>102</v>
+        <v>111</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -1192,10 +1222,10 @@
         <v>37</v>
       </c>
       <c r="C36" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="D36" t="s">
-        <v>102</v>
+        <v>111</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -1206,10 +1236,10 @@
         <v>38</v>
       </c>
       <c r="C37" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="D37" t="s">
-        <v>102</v>
+        <v>111</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -1220,10 +1250,10 @@
         <v>39</v>
       </c>
       <c r="C38" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="D38" t="s">
-        <v>102</v>
+        <v>111</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -1234,10 +1264,10 @@
         <v>40</v>
       </c>
       <c r="C39" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="D39" t="s">
-        <v>102</v>
+        <v>111</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -1248,10 +1278,10 @@
         <v>41</v>
       </c>
       <c r="C40" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="D40" t="s">
-        <v>102</v>
+        <v>111</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -1262,10 +1292,10 @@
         <v>42</v>
       </c>
       <c r="C41" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="D41" t="s">
-        <v>102</v>
+        <v>111</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -1276,10 +1306,10 @@
         <v>43</v>
       </c>
       <c r="C42" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="D42" t="s">
-        <v>102</v>
+        <v>111</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -1290,10 +1320,10 @@
         <v>44</v>
       </c>
       <c r="C43" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="D43" t="s">
-        <v>102</v>
+        <v>111</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -1304,10 +1334,10 @@
         <v>45</v>
       </c>
       <c r="C44" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="D44" t="s">
-        <v>102</v>
+        <v>111</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -1318,10 +1348,10 @@
         <v>46</v>
       </c>
       <c r="C45" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="D45" t="s">
-        <v>103</v>
+        <v>112</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -1332,10 +1362,10 @@
         <v>47</v>
       </c>
       <c r="C46" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="D46" t="s">
-        <v>104</v>
+        <v>113</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -1346,10 +1376,80 @@
         <v>48</v>
       </c>
       <c r="C47" t="s">
+        <v>99</v>
+      </c>
+      <c r="D47" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" s="1">
+        <v>46</v>
+      </c>
+      <c r="B48" t="s">
+        <v>49</v>
+      </c>
+      <c r="C48" t="s">
+        <v>100</v>
+      </c>
+      <c r="D48" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49" s="1">
+        <v>47</v>
+      </c>
+      <c r="B49" t="s">
+        <v>50</v>
+      </c>
+      <c r="C49" t="s">
+        <v>101</v>
+      </c>
+      <c r="D49" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50" s="1">
+        <v>48</v>
+      </c>
+      <c r="B50" t="s">
+        <v>51</v>
+      </c>
+      <c r="C50" t="s">
         <v>94</v>
       </c>
-      <c r="D47" t="s">
-        <v>104</v>
+      <c r="D50" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="A51" s="1">
+        <v>49</v>
+      </c>
+      <c r="B51" t="s">
+        <v>52</v>
+      </c>
+      <c r="C51" t="s">
+        <v>102</v>
+      </c>
+      <c r="D51" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="A52" s="1">
+        <v>50</v>
+      </c>
+      <c r="B52" t="s">
+        <v>53</v>
+      </c>
+      <c r="C52" t="s">
+        <v>103</v>
+      </c>
+      <c r="D52" t="s">
+        <v>114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated on 2018-11-18 at 10:37:19
</commit_message>
<xml_diff>
--- a/index.xlsx
+++ b/index.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="116">
   <si>
     <t>Song Title</t>
   </si>
@@ -169,7 +169,7 @@
     <t>Don_t Let Me Down</t>
   </si>
   <si>
-    <t>Complicated_Dimitri_Vegas_Like_Mike_D_[500kbps_M4A]</t>
+    <t>Complicated</t>
   </si>
   <si>
     <t>2U</t>
@@ -320,6 +320,9 @@
   </si>
   <si>
     <t>The Chainsmokers, Da</t>
+  </si>
+  <si>
+    <t>Dimitri Vegas, Like_Mike, D_</t>
   </si>
   <si>
     <t>David Guetta, Justin Bieber</t>
@@ -722,7 +725,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="52.7109375" customWidth="1"/>
+    <col min="1" max="1" width="21.7109375" customWidth="1"/>
     <col min="2" max="2" width="34.7109375" customWidth="1"/>
     <col min="3" max="3" width="14.7109375" customWidth="1"/>
   </cols>
@@ -749,7 +752,7 @@
         <v>54</v>
       </c>
       <c r="D2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -763,7 +766,7 @@
         <v>55</v>
       </c>
       <c r="D3" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -777,7 +780,7 @@
         <v>56</v>
       </c>
       <c r="D4" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -791,7 +794,7 @@
         <v>57</v>
       </c>
       <c r="D5" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -805,7 +808,7 @@
         <v>58</v>
       </c>
       <c r="D6" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -819,7 +822,7 @@
         <v>59</v>
       </c>
       <c r="D7" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -833,7 +836,7 @@
         <v>60</v>
       </c>
       <c r="D8" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -847,7 +850,7 @@
         <v>61</v>
       </c>
       <c r="D9" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -861,7 +864,7 @@
         <v>62</v>
       </c>
       <c r="D10" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -875,7 +878,7 @@
         <v>63</v>
       </c>
       <c r="D11" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -889,7 +892,7 @@
         <v>64</v>
       </c>
       <c r="D12" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -903,7 +906,7 @@
         <v>65</v>
       </c>
       <c r="D13" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -917,7 +920,7 @@
         <v>66</v>
       </c>
       <c r="D14" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -931,7 +934,7 @@
         <v>67</v>
       </c>
       <c r="D15" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -945,7 +948,7 @@
         <v>68</v>
       </c>
       <c r="D16" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -959,7 +962,7 @@
         <v>69</v>
       </c>
       <c r="D17" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -973,7 +976,7 @@
         <v>70</v>
       </c>
       <c r="D18" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -987,7 +990,7 @@
         <v>71</v>
       </c>
       <c r="D19" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -1001,7 +1004,7 @@
         <v>72</v>
       </c>
       <c r="D20" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -1015,7 +1018,7 @@
         <v>73</v>
       </c>
       <c r="D21" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -1029,7 +1032,7 @@
         <v>74</v>
       </c>
       <c r="D22" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -1043,7 +1046,7 @@
         <v>75</v>
       </c>
       <c r="D23" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -1057,7 +1060,7 @@
         <v>76</v>
       </c>
       <c r="D24" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -1071,7 +1074,7 @@
         <v>77</v>
       </c>
       <c r="D25" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -1085,7 +1088,7 @@
         <v>78</v>
       </c>
       <c r="D26" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -1099,7 +1102,7 @@
         <v>79</v>
       </c>
       <c r="D27" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -1113,7 +1116,7 @@
         <v>80</v>
       </c>
       <c r="D28" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -1127,7 +1130,7 @@
         <v>81</v>
       </c>
       <c r="D29" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -1141,7 +1144,7 @@
         <v>82</v>
       </c>
       <c r="D30" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -1155,7 +1158,7 @@
         <v>83</v>
       </c>
       <c r="D31" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -1169,7 +1172,7 @@
         <v>84</v>
       </c>
       <c r="D32" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -1183,7 +1186,7 @@
         <v>85</v>
       </c>
       <c r="D33" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -1197,7 +1200,7 @@
         <v>86</v>
       </c>
       <c r="D34" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -1211,7 +1214,7 @@
         <v>87</v>
       </c>
       <c r="D35" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -1225,7 +1228,7 @@
         <v>88</v>
       </c>
       <c r="D36" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -1239,7 +1242,7 @@
         <v>89</v>
       </c>
       <c r="D37" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -1253,7 +1256,7 @@
         <v>90</v>
       </c>
       <c r="D38" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -1267,7 +1270,7 @@
         <v>91</v>
       </c>
       <c r="D39" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -1281,7 +1284,7 @@
         <v>92</v>
       </c>
       <c r="D40" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -1295,7 +1298,7 @@
         <v>93</v>
       </c>
       <c r="D41" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -1309,7 +1312,7 @@
         <v>94</v>
       </c>
       <c r="D42" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -1323,7 +1326,7 @@
         <v>95</v>
       </c>
       <c r="D43" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -1337,7 +1340,7 @@
         <v>96</v>
       </c>
       <c r="D44" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -1351,7 +1354,7 @@
         <v>97</v>
       </c>
       <c r="D45" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -1365,7 +1368,7 @@
         <v>98</v>
       </c>
       <c r="D46" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -1379,7 +1382,7 @@
         <v>99</v>
       </c>
       <c r="D47" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -1393,7 +1396,7 @@
         <v>100</v>
       </c>
       <c r="D48" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -1407,7 +1410,7 @@
         <v>101</v>
       </c>
       <c r="D49" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -1418,10 +1421,10 @@
         <v>51</v>
       </c>
       <c r="C50" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="D50" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="51" spans="1:4">
@@ -1432,10 +1435,10 @@
         <v>52</v>
       </c>
       <c r="C51" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D51" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="52" spans="1:4">
@@ -1446,10 +1449,10 @@
         <v>53</v>
       </c>
       <c r="C52" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D52" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated on 2018-11-18 at 10:39:38
</commit_message>
<xml_diff>
--- a/index.xlsx
+++ b/index.xlsx
@@ -25,343 +25,343 @@
     <t>Date Modified</t>
   </si>
   <si>
+    <t>2U</t>
+  </si>
+  <si>
+    <t>All Falls Down</t>
+  </si>
+  <si>
+    <t>Astronomia</t>
+  </si>
+  <si>
+    <t>Attention</t>
+  </si>
+  <si>
+    <t>Baby</t>
+  </si>
+  <si>
+    <t>Bad Liar</t>
+  </si>
+  <si>
+    <t>Battle Symphony</t>
+  </si>
+  <si>
+    <t>Complicated</t>
+  </si>
+  <si>
+    <t>Connection</t>
+  </si>
+  <si>
+    <t>Count On Me</t>
+  </si>
+  <si>
+    <t>Darkside</t>
+  </si>
+  <si>
+    <t>Diamond Heart</t>
+  </si>
+  <si>
+    <t>Don_t Leave Me Alone</t>
+  </si>
+  <si>
+    <t>Don_t Let Me Down</t>
+  </si>
+  <si>
+    <t>Dusk Till Dawn</t>
+  </si>
+  <si>
+    <t>Eastside</t>
+  </si>
+  <si>
+    <t>Finest Hour</t>
+  </si>
+  <si>
     <t>Follow Your Fire</t>
   </si>
   <si>
+    <t>Friend Of Mine</t>
+  </si>
+  <si>
+    <t>Girls Like You</t>
+  </si>
+  <si>
+    <t>Happier</t>
+  </si>
+  <si>
+    <t>Happy Now</t>
+  </si>
+  <si>
+    <t>Havana</t>
+  </si>
+  <si>
+    <t>High On Life</t>
+  </si>
+  <si>
+    <t>Ignite</t>
+  </si>
+  <si>
+    <t>It Ain_t Me</t>
+  </si>
+  <si>
     <t>Jackie Chan</t>
   </si>
   <si>
+    <t>Like I Do</t>
+  </si>
+  <si>
+    <t>Love Me Like You Do</t>
+  </si>
+  <si>
+    <t>Lovers On The Sun</t>
+  </si>
+  <si>
+    <t>Lullaby</t>
+  </si>
+  <si>
+    <t>Mockingbird</t>
+  </si>
+  <si>
+    <t>Natural</t>
+  </si>
+  <si>
+    <t>No Brainer</t>
+  </si>
+  <si>
+    <t>Ocean</t>
+  </si>
+  <si>
+    <t>Over You</t>
+  </si>
+  <si>
+    <t>Rain</t>
+  </si>
+  <si>
+    <t>Remind Me To Forget</t>
+  </si>
+  <si>
+    <t>Right Now</t>
+  </si>
+  <si>
+    <t>Sad_</t>
+  </si>
+  <si>
+    <t>Solo</t>
+  </si>
+  <si>
+    <t>Symphony</t>
+  </si>
+  <si>
     <t>The Nights</t>
   </si>
   <si>
-    <t>Love Me Like You Do</t>
-  </si>
-  <si>
-    <t>Rain</t>
-  </si>
-  <si>
-    <t>Like I Do</t>
+    <t>The Wave</t>
+  </si>
+  <si>
+    <t>This Feeling</t>
   </si>
   <si>
     <t>Thunderclouds</t>
   </si>
   <si>
-    <t>Right Now</t>
-  </si>
-  <si>
-    <t>All Falls Down</t>
-  </si>
-  <si>
-    <t>Girls Like You</t>
-  </si>
-  <si>
-    <t>Astronomia</t>
-  </si>
-  <si>
-    <t>Dusk Till Dawn</t>
-  </si>
-  <si>
-    <t>Havana</t>
+    <t>Wake Me Up</t>
+  </si>
+  <si>
+    <t>Want To</t>
   </si>
   <si>
     <t>Without Me</t>
   </si>
   <si>
-    <t>This Feeling</t>
-  </si>
-  <si>
-    <t>Ocean</t>
-  </si>
-  <si>
-    <t>The Wave</t>
-  </si>
-  <si>
-    <t>Happy Now</t>
-  </si>
-  <si>
-    <t>Lullaby</t>
-  </si>
-  <si>
-    <t>Natural</t>
-  </si>
-  <si>
-    <t>Don_t Leave Me Alone</t>
-  </si>
-  <si>
-    <t>Lovers On The Sun</t>
-  </si>
-  <si>
-    <t>Connection</t>
-  </si>
-  <si>
-    <t>Symphony</t>
-  </si>
-  <si>
-    <t>Darkside</t>
-  </si>
-  <si>
-    <t>Count On Me</t>
-  </si>
-  <si>
-    <t>Mockingbird</t>
-  </si>
-  <si>
-    <t>Happier</t>
-  </si>
-  <si>
-    <t>Over You</t>
-  </si>
-  <si>
-    <t>Wake Me Up</t>
-  </si>
-  <si>
-    <t>Finest Hour</t>
-  </si>
-  <si>
-    <t>Friend Of Mine</t>
-  </si>
-  <si>
-    <t>Remind Me To Forget</t>
-  </si>
-  <si>
-    <t>High On Life</t>
-  </si>
-  <si>
-    <t>Solo</t>
-  </si>
-  <si>
-    <t>Ignite</t>
-  </si>
-  <si>
-    <t>Eastside</t>
-  </si>
-  <si>
-    <t>Diamond Heart</t>
-  </si>
-  <si>
-    <t>Want To</t>
-  </si>
-  <si>
-    <t>Battle Symphony</t>
-  </si>
-  <si>
     <t>Without You</t>
   </si>
   <si>
-    <t>Baby</t>
-  </si>
-  <si>
-    <t>Bad Liar</t>
-  </si>
-  <si>
     <t>Wolves</t>
   </si>
   <si>
-    <t>Sad_</t>
-  </si>
-  <si>
-    <t>No Brainer</t>
-  </si>
-  <si>
-    <t>It Ain_t Me</t>
-  </si>
-  <si>
-    <t>Don_t Let Me Down</t>
-  </si>
-  <si>
-    <t>Complicated</t>
-  </si>
-  <si>
-    <t>2U</t>
-  </si>
-  <si>
-    <t>Attention</t>
+    <t>David Guetta, Justin Bieber</t>
+  </si>
+  <si>
+    <t>Alan Walker, Noah Cyrus</t>
+  </si>
+  <si>
+    <t>Tony Igy</t>
+  </si>
+  <si>
+    <t>Charlie Puth</t>
+  </si>
+  <si>
+    <t>Clean Bandit, Marina And The Diam</t>
+  </si>
+  <si>
+    <t>Selena Gomez</t>
+  </si>
+  <si>
+    <t>Linkin Park</t>
+  </si>
+  <si>
+    <t>Dimitri Vegas, Like_Mike, D_</t>
+  </si>
+  <si>
+    <t>OneRepublic</t>
+  </si>
+  <si>
+    <t>Bruno Mars</t>
+  </si>
+  <si>
+    <t>Alan Walker, Tomine Harket, A</t>
+  </si>
+  <si>
+    <t>Alan Walker, Sophia Soma</t>
+  </si>
+  <si>
+    <t>David Guetta, Ann</t>
+  </si>
+  <si>
+    <t>The Chainsmokers, Da</t>
+  </si>
+  <si>
+    <t>ZAYN, Sia</t>
+  </si>
+  <si>
+    <t>Benny Blanco, Halsey, Khalid</t>
+  </si>
+  <si>
+    <t>Cash Cash, Abir</t>
   </si>
   <si>
     <t>Kodaline</t>
   </si>
   <si>
+    <t>Avicii, Vargas Lagola</t>
+  </si>
+  <si>
+    <t>Maroon 5, Cardi B</t>
+  </si>
+  <si>
+    <t>Marshmello, Bastille</t>
+  </si>
+  <si>
+    <t>Zedd, Elley Duhe</t>
+  </si>
+  <si>
+    <t>Camila Cabello, Young Thug</t>
+  </si>
+  <si>
+    <t>Martin Garrix, Bonn</t>
+  </si>
+  <si>
+    <t>K-391, Alan Walker, Julie Berga</t>
+  </si>
+  <si>
+    <t>Kygo, Selena Gomez</t>
+  </si>
+  <si>
     <t>Ti__sto, Dzeko, Preme, Pos</t>
   </si>
   <si>
+    <t>David Guetta, Martin Garrix_</t>
+  </si>
+  <si>
+    <t>Ellie Goulding</t>
+  </si>
+  <si>
+    <t>David Guetta, Sam Ma</t>
+  </si>
+  <si>
+    <t>R3hab, Mike Williams</t>
+  </si>
+  <si>
+    <t>Eminem</t>
+  </si>
+  <si>
+    <t>Imagine Dragons</t>
+  </si>
+  <si>
+    <t>DJ Khaled, Justin Bieber, C</t>
+  </si>
+  <si>
+    <t>Martin Garrix, Khalid</t>
+  </si>
+  <si>
+    <t>Daughtry</t>
+  </si>
+  <si>
+    <t>The Script</t>
+  </si>
+  <si>
+    <t>Kygo, Miguel</t>
+  </si>
+  <si>
+    <t>Nick Jonas, Robin Schulz</t>
+  </si>
+  <si>
+    <t>XXXTENTACION</t>
+  </si>
+  <si>
+    <t>Clean Bandit, Demi Lovato</t>
+  </si>
+  <si>
+    <t>Clean Bandit, Zara Larsson</t>
+  </si>
+  <si>
     <t>Avicii</t>
   </si>
   <si>
-    <t>Ellie Goulding</t>
-  </si>
-  <si>
-    <t>The Script</t>
-  </si>
-  <si>
-    <t>David Guetta, Martin Garrix_</t>
+    <t>R3hab, Lia Marie Johnson</t>
+  </si>
+  <si>
+    <t>The Chainsmokers, Kelsea</t>
   </si>
   <si>
     <t>LSD</t>
   </si>
   <si>
-    <t>Nick Jonas, Robin Schulz</t>
-  </si>
-  <si>
-    <t>Alan Walker, Noah Cyrus</t>
-  </si>
-  <si>
-    <t>Maroon 5, Cardi B</t>
-  </si>
-  <si>
-    <t>Tony Igy</t>
-  </si>
-  <si>
-    <t>ZAYN, Sia</t>
-  </si>
-  <si>
-    <t>Camila Cabello, Young Thug</t>
+    <t>Avicii, Aloe Blacc</t>
+  </si>
+  <si>
+    <t>Dua Lipa</t>
   </si>
   <si>
     <t>Halsey</t>
   </si>
   <si>
-    <t>The Chainsmokers, Kelsea</t>
-  </si>
-  <si>
-    <t>Martin Garrix, Khalid</t>
-  </si>
-  <si>
-    <t>R3hab, Lia Marie Johnson</t>
-  </si>
-  <si>
-    <t>Zedd, Elley Duhe</t>
-  </si>
-  <si>
-    <t>R3hab, Mike Williams</t>
-  </si>
-  <si>
-    <t>Imagine Dragons</t>
-  </si>
-  <si>
-    <t>David Guetta, Ann</t>
-  </si>
-  <si>
-    <t>David Guetta, Sam Ma</t>
-  </si>
-  <si>
-    <t>OneRepublic</t>
-  </si>
-  <si>
-    <t>Clean Bandit, Zara Larsson</t>
-  </si>
-  <si>
-    <t>Alan Walker, Tomine Harket, A</t>
-  </si>
-  <si>
-    <t>Bruno Mars</t>
-  </si>
-  <si>
-    <t>Eminem</t>
-  </si>
-  <si>
-    <t>Marshmello, Bastille</t>
-  </si>
-  <si>
-    <t>Daughtry</t>
-  </si>
-  <si>
-    <t>Avicii, Aloe Blacc</t>
-  </si>
-  <si>
-    <t>Cash Cash, Abir</t>
-  </si>
-  <si>
-    <t>Avicii, Vargas Lagola</t>
-  </si>
-  <si>
-    <t>Kygo, Miguel</t>
-  </si>
-  <si>
-    <t>Martin Garrix, Bonn</t>
-  </si>
-  <si>
-    <t>Clean Bandit, Demi Lovato</t>
-  </si>
-  <si>
-    <t>K-391, Alan Walker, Julie Berga</t>
-  </si>
-  <si>
-    <t>Benny Blanco, Halsey, Khalid</t>
-  </si>
-  <si>
-    <t>Alan Walker, Sophia Soma</t>
-  </si>
-  <si>
-    <t>Dua Lipa</t>
-  </si>
-  <si>
-    <t>Linkin Park</t>
-  </si>
-  <si>
     <t>Unknown</t>
   </si>
   <si>
-    <t>Clean Bandit, Marina And The Diam</t>
-  </si>
-  <si>
-    <t>Selena Gomez</t>
-  </si>
-  <si>
     <t>Selena Gomez, Marshmello</t>
   </si>
   <si>
-    <t>XXXTENTACION</t>
-  </si>
-  <si>
-    <t>DJ Khaled, Justin Bieber, C</t>
-  </si>
-  <si>
-    <t>Kygo, Selena Gomez</t>
-  </si>
-  <si>
-    <t>The Chainsmokers, Da</t>
-  </si>
-  <si>
-    <t>Dimitri Vegas, Like_Mike, D_</t>
-  </si>
-  <si>
-    <t>David Guetta, Justin Bieber</t>
-  </si>
-  <si>
-    <t>Charlie Puth</t>
+    <t>18-11-2018</t>
+  </si>
+  <si>
+    <t>12-10-2018</t>
+  </si>
+  <si>
+    <t>11-11-2018</t>
+  </si>
+  <si>
+    <t>25-10-2018</t>
+  </si>
+  <si>
+    <t>13-10-2018</t>
   </si>
   <si>
     <t>29-9-2018</t>
   </si>
   <si>
+    <t>11-10-2018</t>
+  </si>
+  <si>
+    <t>16-11-2018</t>
+  </si>
+  <si>
     <t>1-10-2018</t>
   </si>
   <si>
-    <t>11-10-2018</t>
-  </si>
-  <si>
-    <t>12-10-2018</t>
-  </si>
-  <si>
-    <t>13-10-2018</t>
-  </si>
-  <si>
     <t>19-10-2018</t>
   </si>
   <si>
-    <t>25-10-2018</t>
-  </si>
-  <si>
-    <t>11-11-2018</t>
-  </si>
-  <si>
     <t>12-11-2018</t>
-  </si>
-  <si>
-    <t>16-11-2018</t>
-  </si>
-  <si>
-    <t>18-11-2018</t>
   </si>
 </sst>
 </file>
@@ -766,7 +766,7 @@
         <v>55</v>
       </c>
       <c r="D3" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -794,7 +794,7 @@
         <v>57</v>
       </c>
       <c r="D5" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -850,7 +850,7 @@
         <v>61</v>
       </c>
       <c r="D9" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -906,7 +906,7 @@
         <v>65</v>
       </c>
       <c r="D13" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -920,7 +920,7 @@
         <v>66</v>
       </c>
       <c r="D14" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -934,7 +934,7 @@
         <v>67</v>
       </c>
       <c r="D15" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -948,7 +948,7 @@
         <v>68</v>
       </c>
       <c r="D16" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -962,7 +962,7 @@
         <v>69</v>
       </c>
       <c r="D17" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -976,7 +976,7 @@
         <v>70</v>
       </c>
       <c r="D18" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -990,7 +990,7 @@
         <v>71</v>
       </c>
       <c r="D19" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -1004,7 +1004,7 @@
         <v>72</v>
       </c>
       <c r="D20" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -1018,7 +1018,7 @@
         <v>73</v>
       </c>
       <c r="D21" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -1032,7 +1032,7 @@
         <v>74</v>
       </c>
       <c r="D22" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -1046,7 +1046,7 @@
         <v>75</v>
       </c>
       <c r="D23" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -1060,7 +1060,7 @@
         <v>76</v>
       </c>
       <c r="D24" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -1074,7 +1074,7 @@
         <v>77</v>
       </c>
       <c r="D25" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -1088,7 +1088,7 @@
         <v>78</v>
       </c>
       <c r="D26" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -1102,7 +1102,7 @@
         <v>79</v>
       </c>
       <c r="D27" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -1116,7 +1116,7 @@
         <v>80</v>
       </c>
       <c r="D28" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -1158,7 +1158,7 @@
         <v>83</v>
       </c>
       <c r="D31" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -1172,7 +1172,7 @@
         <v>84</v>
       </c>
       <c r="D32" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -1186,7 +1186,7 @@
         <v>85</v>
       </c>
       <c r="D33" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -1200,7 +1200,7 @@
         <v>86</v>
       </c>
       <c r="D34" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -1228,7 +1228,7 @@
         <v>88</v>
       </c>
       <c r="D36" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -1242,7 +1242,7 @@
         <v>89</v>
       </c>
       <c r="D37" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -1256,7 +1256,7 @@
         <v>90</v>
       </c>
       <c r="D38" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -1270,7 +1270,7 @@
         <v>91</v>
       </c>
       <c r="D39" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -1284,7 +1284,7 @@
         <v>92</v>
       </c>
       <c r="D40" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -1312,7 +1312,7 @@
         <v>94</v>
       </c>
       <c r="D42" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -1326,7 +1326,7 @@
         <v>95</v>
       </c>
       <c r="D43" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -1340,7 +1340,7 @@
         <v>96</v>
       </c>
       <c r="D44" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -1354,7 +1354,7 @@
         <v>97</v>
       </c>
       <c r="D45" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -1382,7 +1382,7 @@
         <v>99</v>
       </c>
       <c r="D47" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -1396,7 +1396,7 @@
         <v>100</v>
       </c>
       <c r="D48" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -1410,7 +1410,7 @@
         <v>101</v>
       </c>
       <c r="D49" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -1424,7 +1424,7 @@
         <v>102</v>
       </c>
       <c r="D50" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="51" spans="1:4">
@@ -1438,7 +1438,7 @@
         <v>103</v>
       </c>
       <c r="D51" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
     </row>
     <row r="52" spans="1:4">

</xml_diff>

<commit_message>
Updated on 2018-11-18 at 10:44:22
</commit_message>
<xml_diff>
--- a/index.xlsx
+++ b/index.xlsx
@@ -743,7 +743,7 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
@@ -757,7 +757,7 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
@@ -771,7 +771,7 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
@@ -785,7 +785,7 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
@@ -799,7 +799,7 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
@@ -813,7 +813,7 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
         <v>8</v>
@@ -827,7 +827,7 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
         <v>9</v>
@@ -841,7 +841,7 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
         <v>10</v>
@@ -855,7 +855,7 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B10" t="s">
         <v>11</v>
@@ -869,7 +869,7 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B11" t="s">
         <v>12</v>
@@ -883,7 +883,7 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="1">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B12" t="s">
         <v>13</v>
@@ -897,7 +897,7 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="1">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B13" t="s">
         <v>14</v>
@@ -911,7 +911,7 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="1">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B14" t="s">
         <v>15</v>
@@ -925,7 +925,7 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="1">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B15" t="s">
         <v>16</v>
@@ -939,7 +939,7 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="1">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B16" t="s">
         <v>17</v>
@@ -953,7 +953,7 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="1">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B17" t="s">
         <v>18</v>
@@ -967,7 +967,7 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="1">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B18" t="s">
         <v>19</v>
@@ -981,7 +981,7 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="1">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B19" t="s">
         <v>20</v>
@@ -995,7 +995,7 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="1">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B20" t="s">
         <v>21</v>
@@ -1009,7 +1009,7 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="1">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B21" t="s">
         <v>22</v>
@@ -1023,7 +1023,7 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="1">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B22" t="s">
         <v>23</v>
@@ -1037,7 +1037,7 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="1">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B23" t="s">
         <v>24</v>
@@ -1051,7 +1051,7 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="1">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B24" t="s">
         <v>25</v>
@@ -1065,7 +1065,7 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="1">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B25" t="s">
         <v>26</v>
@@ -1079,7 +1079,7 @@
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="1">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B26" t="s">
         <v>27</v>
@@ -1093,7 +1093,7 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="1">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B27" t="s">
         <v>28</v>
@@ -1107,7 +1107,7 @@
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="1">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B28" t="s">
         <v>29</v>
@@ -1121,7 +1121,7 @@
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="1">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B29" t="s">
         <v>30</v>
@@ -1135,7 +1135,7 @@
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="1">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B30" t="s">
         <v>31</v>
@@ -1149,7 +1149,7 @@
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="1">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B31" t="s">
         <v>32</v>
@@ -1163,7 +1163,7 @@
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="1">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B32" t="s">
         <v>33</v>
@@ -1177,7 +1177,7 @@
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="1">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B33" t="s">
         <v>34</v>
@@ -1191,7 +1191,7 @@
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="1">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B34" t="s">
         <v>35</v>
@@ -1205,7 +1205,7 @@
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="1">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B35" t="s">
         <v>36</v>
@@ -1219,7 +1219,7 @@
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="1">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B36" t="s">
         <v>37</v>
@@ -1233,7 +1233,7 @@
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="1">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B37" t="s">
         <v>38</v>
@@ -1247,7 +1247,7 @@
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="1">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B38" t="s">
         <v>39</v>
@@ -1261,7 +1261,7 @@
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="1">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B39" t="s">
         <v>40</v>
@@ -1275,7 +1275,7 @@
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="1">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B40" t="s">
         <v>41</v>
@@ -1289,7 +1289,7 @@
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="1">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B41" t="s">
         <v>42</v>
@@ -1303,7 +1303,7 @@
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="1">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B42" t="s">
         <v>43</v>
@@ -1317,7 +1317,7 @@
     </row>
     <row r="43" spans="1:4">
       <c r="A43" s="1">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B43" t="s">
         <v>44</v>
@@ -1331,7 +1331,7 @@
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="1">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B44" t="s">
         <v>45</v>
@@ -1345,7 +1345,7 @@
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="1">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B45" t="s">
         <v>46</v>
@@ -1359,7 +1359,7 @@
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="1">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B46" t="s">
         <v>47</v>
@@ -1373,7 +1373,7 @@
     </row>
     <row r="47" spans="1:4">
       <c r="A47" s="1">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B47" t="s">
         <v>48</v>
@@ -1387,7 +1387,7 @@
     </row>
     <row r="48" spans="1:4">
       <c r="A48" s="1">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B48" t="s">
         <v>49</v>
@@ -1401,7 +1401,7 @@
     </row>
     <row r="49" spans="1:4">
       <c r="A49" s="1">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B49" t="s">
         <v>50</v>
@@ -1415,7 +1415,7 @@
     </row>
     <row r="50" spans="1:4">
       <c r="A50" s="1">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B50" t="s">
         <v>51</v>
@@ -1429,7 +1429,7 @@
     </row>
     <row r="51" spans="1:4">
       <c r="A51" s="1">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B51" t="s">
         <v>52</v>
@@ -1443,7 +1443,7 @@
     </row>
     <row r="52" spans="1:4">
       <c r="A52" s="1">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B52" t="s">
         <v>53</v>

</xml_diff>

<commit_message>
Updated on 2018-11-18 at 13:28:35
</commit_message>
<xml_diff>
--- a/index.xlsx
+++ b/index.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="146">
   <si>
     <t>Song Title</t>
   </si>
@@ -31,6 +31,9 @@
     <t>All Falls Down</t>
   </si>
   <si>
+    <t>Alone</t>
+  </si>
+  <si>
     <t>Astronomia</t>
   </si>
   <si>
@@ -73,6 +76,9 @@
     <t>Eastside</t>
   </si>
   <si>
+    <t>Faded</t>
+  </si>
+  <si>
     <t>Finest Hour</t>
   </si>
   <si>
@@ -82,9 +88,15 @@
     <t>Friend Of Mine</t>
   </si>
   <si>
+    <t>Friends</t>
+  </si>
+  <si>
     <t>Girls Like You</t>
   </si>
   <si>
+    <t>God_s Plan</t>
+  </si>
+  <si>
     <t>Happier</t>
   </si>
   <si>
@@ -106,18 +118,27 @@
     <t>Jackie Chan</t>
   </si>
   <si>
+    <t>Let Me Love You</t>
+  </si>
+  <si>
     <t>Like I Do</t>
   </si>
   <si>
     <t>Love Me Like You Do</t>
   </si>
   <si>
+    <t>Love Yourself</t>
+  </si>
+  <si>
     <t>Lovers On The Sun</t>
   </si>
   <si>
     <t>Lullaby</t>
   </si>
   <si>
+    <t>Magenta Riddim</t>
+  </si>
+  <si>
     <t>Mockingbird</t>
   </si>
   <si>
@@ -130,9 +151,15 @@
     <t>Ocean</t>
   </si>
   <si>
+    <t>One Less Lonely Girl</t>
+  </si>
+  <si>
     <t>Over You</t>
   </si>
   <si>
+    <t>Paris</t>
+  </si>
+  <si>
     <t>Rain</t>
   </si>
   <si>
@@ -142,9 +169,18 @@
     <t>Right Now</t>
   </si>
   <si>
+    <t>Rise</t>
+  </si>
+  <si>
+    <t>Rockabye</t>
+  </si>
+  <si>
     <t>Sad_</t>
   </si>
   <si>
+    <t>Sing Me To Sleep</t>
+  </si>
+  <si>
     <t>Solo</t>
   </si>
   <si>
@@ -163,12 +199,18 @@
     <t>Thunderclouds</t>
   </si>
   <si>
+    <t>Tired</t>
+  </si>
+  <si>
     <t>Wake Me Up</t>
   </si>
   <si>
     <t>Want To</t>
   </si>
   <si>
+    <t>We Don_t Talk Anymore</t>
+  </si>
+  <si>
     <t>Without Me</t>
   </si>
   <si>
@@ -178,12 +220,21 @@
     <t>Wolves</t>
   </si>
   <si>
+    <t>You_re No One Til Someone Lets You Down [500kbps_M4A]</t>
+  </si>
+  <si>
+    <t>Young Dumb And Broke</t>
+  </si>
+  <si>
     <t>David Guetta, Justin Bieber</t>
   </si>
   <si>
     <t>Alan Walker, Noah Cyrus</t>
   </si>
   <si>
+    <t>Alan Walker, Noonie Bao</t>
+  </si>
+  <si>
     <t>Tony Igy</t>
   </si>
   <si>
@@ -226,6 +277,9 @@
     <t>Benny Blanco, Halsey, Khalid</t>
   </si>
   <si>
+    <t>Alan Walker</t>
+  </si>
+  <si>
     <t>Cash Cash, Abir</t>
   </si>
   <si>
@@ -235,9 +289,15 @@
     <t>Avicii, Vargas Lagola</t>
   </si>
   <si>
+    <t>Marshmello, Anne-Marie</t>
+  </si>
+  <si>
     <t>Maroon 5, Cardi B</t>
   </si>
   <si>
+    <t>Drake</t>
+  </si>
+  <si>
     <t>Marshmello, Bastille</t>
   </si>
   <si>
@@ -259,18 +319,27 @@
     <t>Ti__sto, Dzeko, Preme, Pos</t>
   </si>
   <si>
+    <t>DJ Snake, Justin Biebe</t>
+  </si>
+  <si>
     <t>David Guetta, Martin Garrix_</t>
   </si>
   <si>
     <t>Ellie Goulding</t>
   </si>
   <si>
+    <t>Justin Bieber</t>
+  </si>
+  <si>
     <t>David Guetta, Sam Ma</t>
   </si>
   <si>
     <t>R3hab, Mike Williams</t>
   </si>
   <si>
+    <t>DJ Snake</t>
+  </si>
+  <si>
     <t>Eminem</t>
   </si>
   <si>
@@ -286,6 +355,9 @@
     <t>Daughtry</t>
   </si>
   <si>
+    <t>The Chainsmokers, Emily Warren</t>
+  </si>
+  <si>
     <t>The Script</t>
   </si>
   <si>
@@ -295,9 +367,18 @@
     <t>Nick Jonas, Robin Schulz</t>
   </si>
   <si>
+    <t>Jonas Blue, Jack Jack</t>
+  </si>
+  <si>
+    <t>Clean Bandit, Sean Paul, Anne</t>
+  </si>
+  <si>
     <t>XXXTENTACION</t>
   </si>
   <si>
+    <t>Alan Walker, Iselin S</t>
+  </si>
+  <si>
     <t>Clean Bandit, Demi Lovato</t>
   </si>
   <si>
@@ -316,12 +397,18 @@
     <t>LSD</t>
   </si>
   <si>
+    <t>Alan Walker, Gavin James</t>
+  </si>
+  <si>
     <t>Avicii, Aloe Blacc</t>
   </si>
   <si>
     <t>Dua Lipa</t>
   </si>
   <si>
+    <t>Charlie Puth, Se</t>
+  </si>
+  <si>
     <t>Halsey</t>
   </si>
   <si>
@@ -329,6 +416,9 @@
   </si>
   <si>
     <t>Selena Gomez, Marshmello</t>
+  </si>
+  <si>
+    <t>Khalid</t>
   </si>
   <si>
     <t>18-11-2018</t>
@@ -719,13 +809,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D52"/>
+  <dimension ref="A1:D68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.7109375" customWidth="1"/>
+    <col min="1" max="1" width="54.7109375" customWidth="1"/>
     <col min="2" max="2" width="34.7109375" customWidth="1"/>
     <col min="3" max="3" width="14.7109375" customWidth="1"/>
   </cols>
@@ -749,10 +839,10 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>54</v>
+        <v>70</v>
       </c>
       <c r="D2" t="s">
-        <v>105</v>
+        <v>135</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -763,10 +853,10 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="D3" t="s">
-        <v>106</v>
+        <v>136</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -777,10 +867,10 @@
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>56</v>
+        <v>72</v>
       </c>
       <c r="D4" t="s">
-        <v>106</v>
+        <v>135</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -791,10 +881,10 @@
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>57</v>
+        <v>73</v>
       </c>
       <c r="D5" t="s">
-        <v>105</v>
+        <v>136</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -805,10 +895,10 @@
         <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>58</v>
+        <v>74</v>
       </c>
       <c r="D6" t="s">
-        <v>107</v>
+        <v>135</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -819,10 +909,10 @@
         <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>59</v>
+        <v>75</v>
       </c>
       <c r="D7" t="s">
-        <v>107</v>
+        <v>137</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -833,10 +923,10 @@
         <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>60</v>
+        <v>76</v>
       </c>
       <c r="D8" t="s">
-        <v>107</v>
+        <v>137</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -847,10 +937,10 @@
         <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>61</v>
+        <v>77</v>
       </c>
       <c r="D9" t="s">
-        <v>105</v>
+        <v>137</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -861,10 +951,10 @@
         <v>11</v>
       </c>
       <c r="C10" t="s">
-        <v>62</v>
+        <v>78</v>
       </c>
       <c r="D10" t="s">
-        <v>108</v>
+        <v>135</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -875,10 +965,10 @@
         <v>12</v>
       </c>
       <c r="C11" t="s">
-        <v>63</v>
+        <v>79</v>
       </c>
       <c r="D11" t="s">
-        <v>108</v>
+        <v>138</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -889,10 +979,10 @@
         <v>13</v>
       </c>
       <c r="C12" t="s">
-        <v>64</v>
+        <v>80</v>
       </c>
       <c r="D12" t="s">
-        <v>108</v>
+        <v>138</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -903,10 +993,10 @@
         <v>14</v>
       </c>
       <c r="C13" t="s">
-        <v>65</v>
+        <v>81</v>
       </c>
       <c r="D13" t="s">
-        <v>107</v>
+        <v>138</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -917,10 +1007,10 @@
         <v>15</v>
       </c>
       <c r="C14" t="s">
-        <v>66</v>
+        <v>82</v>
       </c>
       <c r="D14" t="s">
-        <v>108</v>
+        <v>137</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -931,10 +1021,10 @@
         <v>16</v>
       </c>
       <c r="C15" t="s">
-        <v>67</v>
+        <v>83</v>
       </c>
       <c r="D15" t="s">
-        <v>105</v>
+        <v>138</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -945,10 +1035,10 @@
         <v>17</v>
       </c>
       <c r="C16" t="s">
-        <v>68</v>
+        <v>84</v>
       </c>
       <c r="D16" t="s">
-        <v>109</v>
+        <v>135</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -959,10 +1049,10 @@
         <v>18</v>
       </c>
       <c r="C17" t="s">
-        <v>69</v>
+        <v>85</v>
       </c>
       <c r="D17" t="s">
-        <v>107</v>
+        <v>139</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -973,10 +1063,10 @@
         <v>19</v>
       </c>
       <c r="C18" t="s">
-        <v>70</v>
+        <v>86</v>
       </c>
       <c r="D18" t="s">
-        <v>108</v>
+        <v>137</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -987,10 +1077,10 @@
         <v>20</v>
       </c>
       <c r="C19" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="D19" t="s">
-        <v>110</v>
+        <v>135</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -1001,10 +1091,10 @@
         <v>21</v>
       </c>
       <c r="C20" t="s">
-        <v>72</v>
+        <v>88</v>
       </c>
       <c r="D20" t="s">
-        <v>108</v>
+        <v>138</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -1015,10 +1105,10 @@
         <v>22</v>
       </c>
       <c r="C21" t="s">
-        <v>73</v>
+        <v>89</v>
       </c>
       <c r="D21" t="s">
-        <v>106</v>
+        <v>140</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -1029,10 +1119,10 @@
         <v>23</v>
       </c>
       <c r="C22" t="s">
-        <v>74</v>
+        <v>90</v>
       </c>
       <c r="D22" t="s">
-        <v>108</v>
+        <v>138</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -1043,10 +1133,10 @@
         <v>24</v>
       </c>
       <c r="C23" t="s">
-        <v>75</v>
+        <v>91</v>
       </c>
       <c r="D23" t="s">
-        <v>108</v>
+        <v>135</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -1057,10 +1147,10 @@
         <v>25</v>
       </c>
       <c r="C24" t="s">
-        <v>76</v>
+        <v>92</v>
       </c>
       <c r="D24" t="s">
-        <v>109</v>
+        <v>136</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -1071,10 +1161,10 @@
         <v>26</v>
       </c>
       <c r="C25" t="s">
-        <v>77</v>
+        <v>93</v>
       </c>
       <c r="D25" t="s">
-        <v>107</v>
+        <v>135</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -1085,10 +1175,10 @@
         <v>27</v>
       </c>
       <c r="C26" t="s">
-        <v>78</v>
+        <v>94</v>
       </c>
       <c r="D26" t="s">
-        <v>107</v>
+        <v>138</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -1099,10 +1189,10 @@
         <v>28</v>
       </c>
       <c r="C27" t="s">
-        <v>79</v>
+        <v>95</v>
       </c>
       <c r="D27" t="s">
-        <v>105</v>
+        <v>138</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -1113,10 +1203,10 @@
         <v>29</v>
       </c>
       <c r="C28" t="s">
-        <v>80</v>
+        <v>96</v>
       </c>
       <c r="D28" t="s">
-        <v>110</v>
+        <v>139</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -1127,10 +1217,10 @@
         <v>30</v>
       </c>
       <c r="C29" t="s">
-        <v>81</v>
+        <v>97</v>
       </c>
       <c r="D29" t="s">
-        <v>111</v>
+        <v>137</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -1141,10 +1231,10 @@
         <v>31</v>
       </c>
       <c r="C30" t="s">
-        <v>82</v>
+        <v>98</v>
       </c>
       <c r="D30" t="s">
-        <v>111</v>
+        <v>137</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -1155,10 +1245,10 @@
         <v>32</v>
       </c>
       <c r="C31" t="s">
-        <v>83</v>
+        <v>99</v>
       </c>
       <c r="D31" t="s">
-        <v>108</v>
+        <v>135</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -1169,10 +1259,10 @@
         <v>33</v>
       </c>
       <c r="C32" t="s">
-        <v>84</v>
+        <v>100</v>
       </c>
       <c r="D32" t="s">
-        <v>108</v>
+        <v>140</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -1183,10 +1273,10 @@
         <v>34</v>
       </c>
       <c r="C33" t="s">
-        <v>85</v>
+        <v>101</v>
       </c>
       <c r="D33" t="s">
-        <v>108</v>
+        <v>135</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -1197,10 +1287,10 @@
         <v>35</v>
       </c>
       <c r="C34" t="s">
-        <v>86</v>
+        <v>102</v>
       </c>
       <c r="D34" t="s">
-        <v>108</v>
+        <v>141</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -1211,10 +1301,10 @@
         <v>36</v>
       </c>
       <c r="C35" t="s">
-        <v>87</v>
+        <v>103</v>
       </c>
       <c r="D35" t="s">
-        <v>112</v>
+        <v>141</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -1225,10 +1315,10 @@
         <v>37</v>
       </c>
       <c r="C36" t="s">
-        <v>88</v>
+        <v>104</v>
       </c>
       <c r="D36" t="s">
-        <v>108</v>
+        <v>135</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -1239,10 +1329,10 @@
         <v>38</v>
       </c>
       <c r="C37" t="s">
-        <v>89</v>
+        <v>105</v>
       </c>
       <c r="D37" t="s">
-        <v>108</v>
+        <v>138</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -1253,10 +1343,10 @@
         <v>39</v>
       </c>
       <c r="C38" t="s">
-        <v>90</v>
+        <v>106</v>
       </c>
       <c r="D38" t="s">
-        <v>111</v>
+        <v>138</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -1267,10 +1357,10 @@
         <v>40</v>
       </c>
       <c r="C39" t="s">
-        <v>91</v>
+        <v>107</v>
       </c>
       <c r="D39" t="s">
-        <v>108</v>
+        <v>135</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -1281,10 +1371,10 @@
         <v>41</v>
       </c>
       <c r="C40" t="s">
-        <v>92</v>
+        <v>108</v>
       </c>
       <c r="D40" t="s">
-        <v>106</v>
+        <v>138</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -1295,10 +1385,10 @@
         <v>42</v>
       </c>
       <c r="C41" t="s">
-        <v>93</v>
+        <v>109</v>
       </c>
       <c r="D41" t="s">
-        <v>112</v>
+        <v>138</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -1309,10 +1399,10 @@
         <v>43</v>
       </c>
       <c r="C42" t="s">
-        <v>94</v>
+        <v>110</v>
       </c>
       <c r="D42" t="s">
-        <v>107</v>
+        <v>142</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -1323,10 +1413,10 @@
         <v>44</v>
       </c>
       <c r="C43" t="s">
-        <v>95</v>
+        <v>111</v>
       </c>
       <c r="D43" t="s">
-        <v>108</v>
+        <v>138</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -1337,10 +1427,10 @@
         <v>45</v>
       </c>
       <c r="C44" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="D44" t="s">
-        <v>113</v>
+        <v>135</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -1351,10 +1441,10 @@
         <v>46</v>
       </c>
       <c r="C45" t="s">
-        <v>97</v>
+        <v>112</v>
       </c>
       <c r="D45" t="s">
-        <v>108</v>
+        <v>138</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -1365,10 +1455,10 @@
         <v>47</v>
       </c>
       <c r="C46" t="s">
-        <v>98</v>
+        <v>113</v>
       </c>
       <c r="D46" t="s">
-        <v>114</v>
+        <v>135</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -1379,10 +1469,10 @@
         <v>48</v>
       </c>
       <c r="C47" t="s">
-        <v>99</v>
+        <v>114</v>
       </c>
       <c r="D47" t="s">
-        <v>111</v>
+        <v>141</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -1393,10 +1483,10 @@
         <v>49</v>
       </c>
       <c r="C48" t="s">
-        <v>100</v>
+        <v>115</v>
       </c>
       <c r="D48" t="s">
-        <v>108</v>
+        <v>138</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -1407,10 +1497,10 @@
         <v>50</v>
       </c>
       <c r="C49" t="s">
-        <v>101</v>
+        <v>116</v>
       </c>
       <c r="D49" t="s">
-        <v>107</v>
+        <v>136</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -1421,10 +1511,10 @@
         <v>51</v>
       </c>
       <c r="C50" t="s">
-        <v>102</v>
+        <v>117</v>
       </c>
       <c r="D50" t="s">
-        <v>114</v>
+        <v>135</v>
       </c>
     </row>
     <row r="51" spans="1:4">
@@ -1435,10 +1525,10 @@
         <v>52</v>
       </c>
       <c r="C51" t="s">
-        <v>103</v>
+        <v>118</v>
       </c>
       <c r="D51" t="s">
-        <v>107</v>
+        <v>135</v>
       </c>
     </row>
     <row r="52" spans="1:4">
@@ -1449,10 +1539,234 @@
         <v>53</v>
       </c>
       <c r="C52" t="s">
-        <v>104</v>
+        <v>119</v>
       </c>
       <c r="D52" t="s">
-        <v>115</v>
+        <v>142</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
+      <c r="A53" s="1">
+        <v>52</v>
+      </c>
+      <c r="B53" t="s">
+        <v>54</v>
+      </c>
+      <c r="C53" t="s">
+        <v>120</v>
+      </c>
+      <c r="D53" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
+      <c r="A54" s="1">
+        <v>53</v>
+      </c>
+      <c r="B54" t="s">
+        <v>55</v>
+      </c>
+      <c r="C54" t="s">
+        <v>121</v>
+      </c>
+      <c r="D54" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
+      <c r="A55" s="1">
+        <v>54</v>
+      </c>
+      <c r="B55" t="s">
+        <v>56</v>
+      </c>
+      <c r="C55" t="s">
+        <v>122</v>
+      </c>
+      <c r="D55" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
+      <c r="A56" s="1">
+        <v>55</v>
+      </c>
+      <c r="B56" t="s">
+        <v>57</v>
+      </c>
+      <c r="C56" t="s">
+        <v>123</v>
+      </c>
+      <c r="D56" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4">
+      <c r="A57" s="1">
+        <v>56</v>
+      </c>
+      <c r="B57" t="s">
+        <v>58</v>
+      </c>
+      <c r="C57" t="s">
+        <v>124</v>
+      </c>
+      <c r="D57" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
+      <c r="A58" s="1">
+        <v>57</v>
+      </c>
+      <c r="B58" t="s">
+        <v>59</v>
+      </c>
+      <c r="C58" t="s">
+        <v>125</v>
+      </c>
+      <c r="D58" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
+      <c r="A59" s="1">
+        <v>58</v>
+      </c>
+      <c r="B59" t="s">
+        <v>60</v>
+      </c>
+      <c r="C59" t="s">
+        <v>126</v>
+      </c>
+      <c r="D59" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
+      <c r="A60" s="1">
+        <v>59</v>
+      </c>
+      <c r="B60" t="s">
+        <v>61</v>
+      </c>
+      <c r="C60" t="s">
+        <v>127</v>
+      </c>
+      <c r="D60" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4">
+      <c r="A61" s="1">
+        <v>60</v>
+      </c>
+      <c r="B61" t="s">
+        <v>62</v>
+      </c>
+      <c r="C61" t="s">
+        <v>128</v>
+      </c>
+      <c r="D61" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4">
+      <c r="A62" s="1">
+        <v>61</v>
+      </c>
+      <c r="B62" t="s">
+        <v>63</v>
+      </c>
+      <c r="C62" t="s">
+        <v>129</v>
+      </c>
+      <c r="D62" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4">
+      <c r="A63" s="1">
+        <v>62</v>
+      </c>
+      <c r="B63" t="s">
+        <v>64</v>
+      </c>
+      <c r="C63" t="s">
+        <v>130</v>
+      </c>
+      <c r="D63" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4">
+      <c r="A64" s="1">
+        <v>63</v>
+      </c>
+      <c r="B64" t="s">
+        <v>65</v>
+      </c>
+      <c r="C64" t="s">
+        <v>131</v>
+      </c>
+      <c r="D64" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4">
+      <c r="A65" s="1">
+        <v>64</v>
+      </c>
+      <c r="B65" t="s">
+        <v>66</v>
+      </c>
+      <c r="C65" t="s">
+        <v>132</v>
+      </c>
+      <c r="D65" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4">
+      <c r="A66" s="1">
+        <v>65</v>
+      </c>
+      <c r="B66" t="s">
+        <v>67</v>
+      </c>
+      <c r="C66" t="s">
+        <v>133</v>
+      </c>
+      <c r="D66" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4">
+      <c r="A67" s="1">
+        <v>66</v>
+      </c>
+      <c r="B67" t="s">
+        <v>68</v>
+      </c>
+      <c r="C67" t="s">
+        <v>132</v>
+      </c>
+      <c r="D67" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4">
+      <c r="A68" s="1">
+        <v>67</v>
+      </c>
+      <c r="B68" t="s">
+        <v>69</v>
+      </c>
+      <c r="C68" t="s">
+        <v>134</v>
+      </c>
+      <c r="D68" t="s">
+        <v>135</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated on 2018-11-18 at 13:29:26
</commit_message>
<xml_diff>
--- a/index.xlsx
+++ b/index.xlsx
@@ -220,7 +220,7 @@
     <t>Wolves</t>
   </si>
   <si>
-    <t>You_re No One Til Someone Lets You Down [500kbps_M4A]</t>
+    <t>You_re No One Til Someone Lets You Down - John Mayer</t>
   </si>
   <si>
     <t>Young Dumb And Broke</t>
@@ -815,7 +815,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="54.7109375" customWidth="1"/>
+    <col min="1" max="1" width="53.7109375" customWidth="1"/>
     <col min="2" max="2" width="34.7109375" customWidth="1"/>
     <col min="3" max="3" width="14.7109375" customWidth="1"/>
   </cols>

</xml_diff>

<commit_message>
Updated on 2018-11-18 at 13:30:46
</commit_message>
<xml_diff>
--- a/index.xlsx
+++ b/index.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="147">
   <si>
     <t>Song Title</t>
   </si>
@@ -220,7 +220,7 @@
     <t>Wolves</t>
   </si>
   <si>
-    <t>You_re No One Til Someone Lets You Down - John Mayer</t>
+    <t>You_re No One Til Someone Lets You Down</t>
   </si>
   <si>
     <t>Young Dumb And Broke</t>
@@ -416,6 +416,9 @@
   </si>
   <si>
     <t>Selena Gomez, Marshmello</t>
+  </si>
+  <si>
+    <t>John Mayer</t>
   </si>
   <si>
     <t>Khalid</t>
@@ -815,7 +818,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="53.7109375" customWidth="1"/>
+    <col min="1" max="1" width="40.7109375" customWidth="1"/>
     <col min="2" max="2" width="34.7109375" customWidth="1"/>
     <col min="3" max="3" width="14.7109375" customWidth="1"/>
   </cols>
@@ -842,7 +845,7 @@
         <v>70</v>
       </c>
       <c r="D2" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -856,7 +859,7 @@
         <v>71</v>
       </c>
       <c r="D3" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -870,7 +873,7 @@
         <v>72</v>
       </c>
       <c r="D4" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -884,7 +887,7 @@
         <v>73</v>
       </c>
       <c r="D5" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -898,7 +901,7 @@
         <v>74</v>
       </c>
       <c r="D6" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -912,7 +915,7 @@
         <v>75</v>
       </c>
       <c r="D7" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -926,7 +929,7 @@
         <v>76</v>
       </c>
       <c r="D8" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -940,7 +943,7 @@
         <v>77</v>
       </c>
       <c r="D9" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -954,7 +957,7 @@
         <v>78</v>
       </c>
       <c r="D10" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -968,7 +971,7 @@
         <v>79</v>
       </c>
       <c r="D11" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -982,7 +985,7 @@
         <v>80</v>
       </c>
       <c r="D12" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -996,7 +999,7 @@
         <v>81</v>
       </c>
       <c r="D13" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -1010,7 +1013,7 @@
         <v>82</v>
       </c>
       <c r="D14" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -1024,7 +1027,7 @@
         <v>83</v>
       </c>
       <c r="D15" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -1038,7 +1041,7 @@
         <v>84</v>
       </c>
       <c r="D16" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -1052,7 +1055,7 @@
         <v>85</v>
       </c>
       <c r="D17" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -1066,7 +1069,7 @@
         <v>86</v>
       </c>
       <c r="D18" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -1080,7 +1083,7 @@
         <v>87</v>
       </c>
       <c r="D19" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -1094,7 +1097,7 @@
         <v>88</v>
       </c>
       <c r="D20" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -1108,7 +1111,7 @@
         <v>89</v>
       </c>
       <c r="D21" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -1122,7 +1125,7 @@
         <v>90</v>
       </c>
       <c r="D22" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -1136,7 +1139,7 @@
         <v>91</v>
       </c>
       <c r="D23" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -1150,7 +1153,7 @@
         <v>92</v>
       </c>
       <c r="D24" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -1164,7 +1167,7 @@
         <v>93</v>
       </c>
       <c r="D25" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -1178,7 +1181,7 @@
         <v>94</v>
       </c>
       <c r="D26" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -1192,7 +1195,7 @@
         <v>95</v>
       </c>
       <c r="D27" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -1206,7 +1209,7 @@
         <v>96</v>
       </c>
       <c r="D28" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -1220,7 +1223,7 @@
         <v>97</v>
       </c>
       <c r="D29" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -1234,7 +1237,7 @@
         <v>98</v>
       </c>
       <c r="D30" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -1248,7 +1251,7 @@
         <v>99</v>
       </c>
       <c r="D31" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -1262,7 +1265,7 @@
         <v>100</v>
       </c>
       <c r="D32" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -1276,7 +1279,7 @@
         <v>101</v>
       </c>
       <c r="D33" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -1290,7 +1293,7 @@
         <v>102</v>
       </c>
       <c r="D34" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -1304,7 +1307,7 @@
         <v>103</v>
       </c>
       <c r="D35" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -1318,7 +1321,7 @@
         <v>104</v>
       </c>
       <c r="D36" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -1332,7 +1335,7 @@
         <v>105</v>
       </c>
       <c r="D37" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -1346,7 +1349,7 @@
         <v>106</v>
       </c>
       <c r="D38" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -1360,7 +1363,7 @@
         <v>107</v>
       </c>
       <c r="D39" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -1374,7 +1377,7 @@
         <v>108</v>
       </c>
       <c r="D40" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -1388,7 +1391,7 @@
         <v>109</v>
       </c>
       <c r="D41" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -1402,7 +1405,7 @@
         <v>110</v>
       </c>
       <c r="D42" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -1416,7 +1419,7 @@
         <v>111</v>
       </c>
       <c r="D43" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -1430,7 +1433,7 @@
         <v>104</v>
       </c>
       <c r="D44" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -1444,7 +1447,7 @@
         <v>112</v>
       </c>
       <c r="D45" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -1458,7 +1461,7 @@
         <v>113</v>
       </c>
       <c r="D46" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -1472,7 +1475,7 @@
         <v>114</v>
       </c>
       <c r="D47" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -1486,7 +1489,7 @@
         <v>115</v>
       </c>
       <c r="D48" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -1500,7 +1503,7 @@
         <v>116</v>
       </c>
       <c r="D49" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -1514,7 +1517,7 @@
         <v>117</v>
       </c>
       <c r="D50" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="51" spans="1:4">
@@ -1528,7 +1531,7 @@
         <v>118</v>
       </c>
       <c r="D51" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="52" spans="1:4">
@@ -1542,7 +1545,7 @@
         <v>119</v>
       </c>
       <c r="D52" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="53" spans="1:4">
@@ -1556,7 +1559,7 @@
         <v>120</v>
       </c>
       <c r="D53" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="54" spans="1:4">
@@ -1570,7 +1573,7 @@
         <v>121</v>
       </c>
       <c r="D54" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="55" spans="1:4">
@@ -1584,7 +1587,7 @@
         <v>122</v>
       </c>
       <c r="D55" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="56" spans="1:4">
@@ -1598,7 +1601,7 @@
         <v>123</v>
       </c>
       <c r="D56" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="57" spans="1:4">
@@ -1612,7 +1615,7 @@
         <v>124</v>
       </c>
       <c r="D57" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="58" spans="1:4">
@@ -1626,7 +1629,7 @@
         <v>125</v>
       </c>
       <c r="D58" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="59" spans="1:4">
@@ -1640,7 +1643,7 @@
         <v>126</v>
       </c>
       <c r="D59" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="60" spans="1:4">
@@ -1654,7 +1657,7 @@
         <v>127</v>
       </c>
       <c r="D60" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="61" spans="1:4">
@@ -1668,7 +1671,7 @@
         <v>128</v>
       </c>
       <c r="D61" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="62" spans="1:4">
@@ -1682,7 +1685,7 @@
         <v>129</v>
       </c>
       <c r="D62" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="63" spans="1:4">
@@ -1696,7 +1699,7 @@
         <v>130</v>
       </c>
       <c r="D63" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="64" spans="1:4">
@@ -1710,7 +1713,7 @@
         <v>131</v>
       </c>
       <c r="D64" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="65" spans="1:4">
@@ -1724,7 +1727,7 @@
         <v>132</v>
       </c>
       <c r="D65" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="66" spans="1:4">
@@ -1738,7 +1741,7 @@
         <v>133</v>
       </c>
       <c r="D66" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="67" spans="1:4">
@@ -1749,10 +1752,10 @@
         <v>68</v>
       </c>
       <c r="C67" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="D67" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="68" spans="1:4">
@@ -1763,10 +1766,10 @@
         <v>69</v>
       </c>
       <c r="C68" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D68" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Now parses the EXIF data
- Parsing EXIF data gives reliable results, even when your songs are not in a fixed filename format
</commit_message>
<xml_diff>
--- a/index.xlsx
+++ b/index.xlsx
@@ -14,15 +14,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="220">
   <si>
     <t>Song Title</t>
   </si>
   <si>
-    <t>Authors</t>
-  </si>
-  <si>
-    <t>Date Modified</t>
+    <t>Album</t>
+  </si>
+  <si>
+    <t>Artists</t>
+  </si>
+  <si>
+    <t>Genre</t>
+  </si>
+  <si>
+    <t>Year</t>
   </si>
   <si>
     <t>2U</t>
@@ -64,10 +70,10 @@
     <t>Diamond Heart</t>
   </si>
   <si>
-    <t>Don_t Leave Me Alone</t>
-  </si>
-  <si>
-    <t>Don_t Let Me Down</t>
+    <t>Don't Leave Me Alone</t>
+  </si>
+  <si>
+    <t>Don't Let Me Down</t>
   </si>
   <si>
     <t>Dusk Till Dawn</t>
@@ -94,7 +100,7 @@
     <t>Girls Like You</t>
   </si>
   <si>
-    <t>God_s Plan</t>
+    <t>God's Plan</t>
   </si>
   <si>
     <t>Happier</t>
@@ -112,7 +118,7 @@
     <t>Ignite</t>
   </si>
   <si>
-    <t>It Ain_t Me</t>
+    <t>It Ain't Me</t>
   </si>
   <si>
     <t>Jackie Chan</t>
@@ -175,7 +181,7 @@
     <t>Rockabye</t>
   </si>
   <si>
-    <t>Sad_</t>
+    <t>Sad!</t>
   </si>
   <si>
     <t>Sing Me To Sleep</t>
@@ -208,7 +214,7 @@
     <t>Want To</t>
   </si>
   <si>
-    <t>We Don_t Talk Anymore</t>
+    <t>We Don't Talk Anymore</t>
   </si>
   <si>
     <t>Without Me</t>
@@ -220,16 +226,208 @@
     <t>Wolves</t>
   </si>
   <si>
-    <t>You_re No One Til Someone Lets You Down</t>
-  </si>
-  <si>
-    <t>Young Dumb And Broke</t>
+    <t>You're No One 'Til Someone Lets You Down</t>
+  </si>
+  <si>
+    <t>Young Dumb &amp; Broke</t>
+  </si>
+  <si>
+    <t>2U (Single)</t>
+  </si>
+  <si>
+    <t>All Falls Down (Single)</t>
+  </si>
+  <si>
+    <t>Alone (Single)</t>
+  </si>
+  <si>
+    <t>AsTRonoMia (Single)</t>
+  </si>
+  <si>
+    <t>Voicenotes</t>
+  </si>
+  <si>
+    <t>Baby (Single)</t>
+  </si>
+  <si>
+    <t>Bad Liar (Single)</t>
+  </si>
+  <si>
+    <t>Battle Symphony (Single)</t>
+  </si>
+  <si>
+    <t>Complicated (Single)</t>
+  </si>
+  <si>
+    <t>Connection (Single)</t>
+  </si>
+  <si>
+    <t>Doo-Wops &amp; Hooligans</t>
+  </si>
+  <si>
+    <t>Darkside (Single)</t>
+  </si>
+  <si>
+    <t>Diamond Heart (Single)</t>
+  </si>
+  <si>
+    <t>Don't Leave Me Alone (Single)</t>
+  </si>
+  <si>
+    <t>Dusk Till Dawn (Single)</t>
+  </si>
+  <si>
+    <t>Eastside (Single)</t>
+  </si>
+  <si>
+    <t>Faded (Single)</t>
+  </si>
+  <si>
+    <t>Finest Hour (Single)</t>
+  </si>
+  <si>
+    <t>Follow Your Fire (Single)</t>
+  </si>
+  <si>
+    <t>AVĪCI (01)</t>
+  </si>
+  <si>
+    <t>Friends (Single)</t>
+  </si>
+  <si>
+    <t>Girls Like You (Single)</t>
+  </si>
+  <si>
+    <t>Scary Hours (Single)</t>
+  </si>
+  <si>
+    <t>Happier (Single)</t>
+  </si>
+  <si>
+    <t>Happy Now (Single)</t>
+  </si>
+  <si>
+    <t>Havana (Single)</t>
+  </si>
+  <si>
+    <t>High On Life (Single)</t>
+  </si>
+  <si>
+    <t>Ignite (Single)</t>
+  </si>
+  <si>
+    <t>It Ain't Me (Single)</t>
+  </si>
+  <si>
+    <t>Jackie Chan (Single)</t>
+  </si>
+  <si>
+    <t>Encore</t>
+  </si>
+  <si>
+    <t>Like I Do (Single)</t>
+  </si>
+  <si>
+    <t>Fifty Shades Of Grey (Original Motion Picture Soundtrack)</t>
+  </si>
+  <si>
+    <t>Purpose (Deluxe Edition)</t>
+  </si>
+  <si>
+    <t>Lovers on the Sun - EP</t>
+  </si>
+  <si>
+    <t>Lullaby (Single)</t>
+  </si>
+  <si>
+    <t>Magenta Riddim (Single)</t>
+  </si>
+  <si>
+    <t>Unknown</t>
+  </si>
+  <si>
+    <t>Natural (Single)</t>
+  </si>
+  <si>
+    <t>No Brainer (Single)</t>
+  </si>
+  <si>
+    <t>Ocean (Single)</t>
+  </si>
+  <si>
+    <t>My Worlds (My World &amp; My World 2.0)</t>
+  </si>
+  <si>
+    <t>Daughtry (Wal-Mart Edition)</t>
+  </si>
+  <si>
+    <t>Paris (Single)</t>
+  </si>
+  <si>
+    <t>Rain (Single)</t>
+  </si>
+  <si>
+    <t>Remind Me To Forget (Single)</t>
+  </si>
+  <si>
+    <t>Right Now (Single)</t>
+  </si>
+  <si>
+    <t>Rise (Single)</t>
+  </si>
+  <si>
+    <t>Rockabye (Single)</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>Solo (Single)</t>
+  </si>
+  <si>
+    <t>So Good</t>
+  </si>
+  <si>
+    <t>NOW That's What I Call Music! 90</t>
+  </si>
+  <si>
+    <t>The Wave (Single)</t>
+  </si>
+  <si>
+    <t>This Feeling (Single)</t>
+  </si>
+  <si>
+    <t>Thunderclouds (Single)</t>
+  </si>
+  <si>
+    <t>Tired (Single)</t>
+  </si>
+  <si>
+    <t>True</t>
+  </si>
+  <si>
+    <t>Want To (Single)</t>
+  </si>
+  <si>
+    <t>Nine Track Mind</t>
+  </si>
+  <si>
+    <t>Without Me (Single)</t>
+  </si>
+  <si>
+    <t>Wolves (Single)</t>
+  </si>
+  <si>
+    <t>Paradise Valley</t>
+  </si>
+  <si>
+    <t>American Teen</t>
   </si>
   <si>
     <t>David Guetta, Justin Bieber</t>
   </si>
   <si>
-    <t>Alan Walker, Noah Cyrus</t>
+    <t>Alan Walker, Noah Cyrus, Digital Farm Animals</t>
   </si>
   <si>
     <t>Alan Walker, Noonie Bao</t>
@@ -241,7 +439,7 @@
     <t>Charlie Puth</t>
   </si>
   <si>
-    <t>Clean Bandit, Marina And The Diam</t>
+    <t>Clean Bandit, Marina And The Diamonds, Luis Fonsi</t>
   </si>
   <si>
     <t>Selena Gomez</t>
@@ -250,7 +448,7 @@
     <t>Linkin Park</t>
   </si>
   <si>
-    <t>Dimitri Vegas, Like_Mike, D_</t>
+    <t>Dimitri Vegas &amp; Like Mike, David Guetta, Kiiara</t>
   </si>
   <si>
     <t>OneRepublic</t>
@@ -259,16 +457,16 @@
     <t>Bruno Mars</t>
   </si>
   <si>
-    <t>Alan Walker, Tomine Harket, A</t>
-  </si>
-  <si>
-    <t>Alan Walker, Sophia Soma</t>
-  </si>
-  <si>
-    <t>David Guetta, Ann</t>
-  </si>
-  <si>
-    <t>The Chainsmokers, Da</t>
+    <t>Alan Walker, Tomine Harket, Au/Ra</t>
+  </si>
+  <si>
+    <t>Alan Walker, Sophia Somajo</t>
+  </si>
+  <si>
+    <t>David Guetta, Anne-Marie</t>
+  </si>
+  <si>
+    <t>The Chainsmokers, Daya</t>
   </si>
   <si>
     <t>ZAYN, Sia</t>
@@ -286,7 +484,7 @@
     <t>Kodaline</t>
   </si>
   <si>
-    <t>Avicii, Vargas Lagola</t>
+    <t>Avicii, Vargas &amp; Lagola</t>
   </si>
   <si>
     <t>Marshmello, Anne-Marie</t>
@@ -301,7 +499,7 @@
     <t>Marshmello, Bastille</t>
   </si>
   <si>
-    <t>Zedd, Elley Duhe</t>
+    <t>Zedd, Elley Duhé</t>
   </si>
   <si>
     <t>Camila Cabello, Young Thug</t>
@@ -310,19 +508,19 @@
     <t>Martin Garrix, Bonn</t>
   </si>
   <si>
-    <t>K-391, Alan Walker, Julie Berga</t>
+    <t>K-391, Alan Walker, Julie Bergan, Seungri</t>
   </si>
   <si>
     <t>Kygo, Selena Gomez</t>
   </si>
   <si>
-    <t>Ti__sto, Dzeko, Preme, Pos</t>
-  </si>
-  <si>
-    <t>DJ Snake, Justin Biebe</t>
-  </si>
-  <si>
-    <t>David Guetta, Martin Garrix_</t>
+    <t>Tiësto, Dzeko, Preme, Post Malone</t>
+  </si>
+  <si>
+    <t>DJ Snake, Justin Bieber</t>
+  </si>
+  <si>
+    <t>David Guetta, Martin Garrix, Brooks</t>
   </si>
   <si>
     <t>Ellie Goulding</t>
@@ -331,7 +529,7 @@
     <t>Justin Bieber</t>
   </si>
   <si>
-    <t>David Guetta, Sam Ma</t>
+    <t>David Guetta, Sam Martin</t>
   </si>
   <si>
     <t>R3hab, Mike Williams</t>
@@ -346,7 +544,7 @@
     <t>Imagine Dragons</t>
   </si>
   <si>
-    <t>DJ Khaled, Justin Bieber, C</t>
+    <t>DJ Khaled, Justin Bieber, Chance The Rapper, Quavo</t>
   </si>
   <si>
     <t>Martin Garrix, Khalid</t>
@@ -367,16 +565,16 @@
     <t>Nick Jonas, Robin Schulz</t>
   </si>
   <si>
-    <t>Jonas Blue, Jack Jack</t>
-  </si>
-  <si>
-    <t>Clean Bandit, Sean Paul, Anne</t>
+    <t>Jonas Blue, Jack &amp; Jack</t>
+  </si>
+  <si>
+    <t>Clean Bandit, Sean Paul, Anne-Marie</t>
   </si>
   <si>
     <t>XXXTENTACION</t>
   </si>
   <si>
-    <t>Alan Walker, Iselin S</t>
+    <t>Alan Walker, Iselin Solhei</t>
   </si>
   <si>
     <t>Clean Bandit, Demi Lovato</t>
@@ -391,7 +589,7 @@
     <t>R3hab, Lia Marie Johnson</t>
   </si>
   <si>
-    <t>The Chainsmokers, Kelsea</t>
+    <t>The Chainsmokers, Kelsea Ballerini</t>
   </si>
   <si>
     <t>LSD</t>
@@ -406,13 +604,13 @@
     <t>Dua Lipa</t>
   </si>
   <si>
-    <t>Charlie Puth, Se</t>
+    <t>Charlie Puth, Selena Gomez</t>
   </si>
   <si>
     <t>Halsey</t>
   </si>
   <si>
-    <t>Unknown</t>
+    <t>Avicii, Sandro Cavazza</t>
   </si>
   <si>
     <t>Selena Gomez, Marshmello</t>
@@ -424,37 +622,58 @@
     <t>Khalid</t>
   </si>
   <si>
-    <t>18-11-2018</t>
-  </si>
-  <si>
-    <t>12-10-2018</t>
-  </si>
-  <si>
-    <t>11-11-2018</t>
-  </si>
-  <si>
-    <t>25-10-2018</t>
-  </si>
-  <si>
-    <t>13-10-2018</t>
-  </si>
-  <si>
-    <t>29-9-2018</t>
-  </si>
-  <si>
-    <t>11-10-2018</t>
-  </si>
-  <si>
-    <t>16-11-2018</t>
-  </si>
-  <si>
-    <t>1-10-2018</t>
-  </si>
-  <si>
-    <t>19-10-2018</t>
-  </si>
-  <si>
-    <t>12-11-2018</t>
+    <t>Electronic</t>
+  </si>
+  <si>
+    <t>Pop</t>
+  </si>
+  <si>
+    <t>Dance</t>
+  </si>
+  <si>
+    <t>Pop, rock...</t>
+  </si>
+  <si>
+    <t>Rap, hiphop</t>
+  </si>
+  <si>
+    <t>Soundtrack</t>
+  </si>
+  <si>
+    <t>Rock</t>
+  </si>
+  <si>
+    <t>R&amp;B/Soul</t>
+  </si>
+  <si>
+    <t>2017</t>
+  </si>
+  <si>
+    <t>2016</t>
+  </si>
+  <si>
+    <t>2010</t>
+  </si>
+  <si>
+    <t>2018</t>
+  </si>
+  <si>
+    <t>2011</t>
+  </si>
+  <si>
+    <t>2015</t>
+  </si>
+  <si>
+    <t>2014</t>
+  </si>
+  <si>
+    <t>2005</t>
+  </si>
+  <si>
+    <t>2006</t>
+  </si>
+  <si>
+    <t>2013</t>
   </si>
 </sst>
 </file>
@@ -812,18 +1031,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D68"/>
+  <dimension ref="A1:F68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="40.7109375" customWidth="1"/>
-    <col min="2" max="2" width="34.7109375" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" customWidth="1"/>
+    <col min="1" max="1" width="41.7109375" customWidth="1"/>
+    <col min="2" max="2" width="58.7109375" customWidth="1"/>
+    <col min="3" max="3" width="51.7109375" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" customWidth="1"/>
+    <col min="5" max="5" width="5.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:6">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -833,943 +1054,1351 @@
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D2" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="E2" t="s">
+        <v>202</v>
+      </c>
+      <c r="F2" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="D3" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="E3" t="s">
+        <v>202</v>
+      </c>
+      <c r="F3" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D4" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
+        <v>138</v>
+      </c>
+      <c r="E4" t="s">
+        <v>202</v>
+      </c>
+      <c r="F4" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" s="1">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="D5" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
+        <v>139</v>
+      </c>
+      <c r="E5" t="s">
+        <v>202</v>
+      </c>
+      <c r="F5" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" s="1">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D6" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
+        <v>140</v>
+      </c>
+      <c r="E6" t="s">
+        <v>203</v>
+      </c>
+      <c r="F6" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" s="1">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D7" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
+        <v>141</v>
+      </c>
+      <c r="E7" t="s">
+        <v>204</v>
+      </c>
+      <c r="F7" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" s="1">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D8" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
+        <v>142</v>
+      </c>
+      <c r="E8" t="s">
+        <v>203</v>
+      </c>
+      <c r="F8" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" s="1">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C9" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D9" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
+        <v>143</v>
+      </c>
+      <c r="E9" t="s">
+        <v>203</v>
+      </c>
+      <c r="F9" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" s="1">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C10" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="D10" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
+        <v>144</v>
+      </c>
+      <c r="E10" t="s">
+        <v>202</v>
+      </c>
+      <c r="F10" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" s="1">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C11" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="D11" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
+        <v>145</v>
+      </c>
+      <c r="E11" t="s">
+        <v>203</v>
+      </c>
+      <c r="F11" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12" s="1">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C12" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="D12" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
+        <v>146</v>
+      </c>
+      <c r="E12" t="s">
+        <v>205</v>
+      </c>
+      <c r="F12" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13" s="1">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C13" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D13" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
+        <v>147</v>
+      </c>
+      <c r="E13" t="s">
+        <v>202</v>
+      </c>
+      <c r="F13" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14" s="1">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C14" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D14" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
+        <v>148</v>
+      </c>
+      <c r="E14" t="s">
+        <v>202</v>
+      </c>
+      <c r="F14" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15" s="1">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C15" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="D15" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
+        <v>149</v>
+      </c>
+      <c r="E15" t="s">
+        <v>202</v>
+      </c>
+      <c r="F15" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16" s="1">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C16" t="s">
-        <v>84</v>
+        <v>19</v>
       </c>
       <c r="D16" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
+        <v>150</v>
+      </c>
+      <c r="E16" t="s">
+        <v>202</v>
+      </c>
+      <c r="F16" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17" s="1">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C17" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D17" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
+        <v>151</v>
+      </c>
+      <c r="E17" t="s">
+        <v>203</v>
+      </c>
+      <c r="F17" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18" s="1">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C18" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D18" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
+        <v>152</v>
+      </c>
+      <c r="E18" t="s">
+        <v>203</v>
+      </c>
+      <c r="F18" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
       <c r="A19" s="1">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C19" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D19" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
+        <v>153</v>
+      </c>
+      <c r="E19" t="s">
+        <v>202</v>
+      </c>
+      <c r="F19" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
       <c r="A20" s="1">
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C20" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D20" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
+        <v>154</v>
+      </c>
+      <c r="E20" t="s">
+        <v>202</v>
+      </c>
+      <c r="F20" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
       <c r="A21" s="1">
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C21" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D21" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
+        <v>155</v>
+      </c>
+      <c r="E21" t="s">
+        <v>203</v>
+      </c>
+      <c r="F21" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
       <c r="A22" s="1">
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C22" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D22" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
+        <v>156</v>
+      </c>
+      <c r="E22" t="s">
+        <v>202</v>
+      </c>
+      <c r="F22" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
       <c r="A23" s="1">
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C23" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D23" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4">
+        <v>157</v>
+      </c>
+      <c r="E23" t="s">
+        <v>202</v>
+      </c>
+      <c r="F23" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
       <c r="A24" s="1">
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C24" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D24" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4">
+        <v>158</v>
+      </c>
+      <c r="E24" t="s">
+        <v>203</v>
+      </c>
+      <c r="F24" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
       <c r="A25" s="1">
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C25" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D25" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4">
+        <v>159</v>
+      </c>
+      <c r="E25" t="s">
+        <v>206</v>
+      </c>
+      <c r="F25" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
       <c r="A26" s="1">
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C26" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D26" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4">
+        <v>160</v>
+      </c>
+      <c r="E26" t="s">
+        <v>202</v>
+      </c>
+      <c r="F26" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
       <c r="A27" s="1">
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C27" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D27" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4">
+        <v>161</v>
+      </c>
+      <c r="E27" t="s">
+        <v>203</v>
+      </c>
+      <c r="F27" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
       <c r="A28" s="1">
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C28" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D28" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4">
+        <v>162</v>
+      </c>
+      <c r="E28" t="s">
+        <v>203</v>
+      </c>
+      <c r="F28" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
       <c r="A29" s="1">
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C29" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D29" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4">
+        <v>163</v>
+      </c>
+      <c r="E29" t="s">
+        <v>202</v>
+      </c>
+      <c r="F29" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
       <c r="A30" s="1">
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C30" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D30" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4">
+        <v>164</v>
+      </c>
+      <c r="E30" t="s">
+        <v>202</v>
+      </c>
+      <c r="F30" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
       <c r="A31" s="1">
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C31" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D31" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4">
+        <v>165</v>
+      </c>
+      <c r="E31" t="s">
+        <v>202</v>
+      </c>
+      <c r="F31" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
       <c r="A32" s="1">
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C32" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D32" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4">
+        <v>166</v>
+      </c>
+      <c r="E32" t="s">
+        <v>202</v>
+      </c>
+      <c r="F32" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
       <c r="A33" s="1">
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C33" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D33" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4">
+        <v>167</v>
+      </c>
+      <c r="E33" t="s">
+        <v>202</v>
+      </c>
+      <c r="F33" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
       <c r="A34" s="1">
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C34" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D34" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4">
+        <v>168</v>
+      </c>
+      <c r="E34" t="s">
+        <v>202</v>
+      </c>
+      <c r="F34" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
       <c r="A35" s="1">
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C35" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D35" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4">
+        <v>169</v>
+      </c>
+      <c r="E35" t="s">
+        <v>207</v>
+      </c>
+      <c r="F35" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
       <c r="A36" s="1">
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C36" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D36" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4">
+        <v>170</v>
+      </c>
+      <c r="E36" t="s">
+        <v>203</v>
+      </c>
+      <c r="F36" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
       <c r="A37" s="1">
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C37" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D37" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4">
+        <v>171</v>
+      </c>
+      <c r="E37" t="s">
+        <v>202</v>
+      </c>
+      <c r="F37" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
       <c r="A38" s="1">
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C38" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D38" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4">
+        <v>172</v>
+      </c>
+      <c r="E38" t="s">
+        <v>202</v>
+      </c>
+      <c r="F38" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
       <c r="A39" s="1">
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C39" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D39" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4">
+        <v>173</v>
+      </c>
+      <c r="E39" t="s">
+        <v>202</v>
+      </c>
+      <c r="F39" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
       <c r="A40" s="1">
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C40" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D40" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4">
+        <v>174</v>
+      </c>
+      <c r="E40" t="s">
+        <v>206</v>
+      </c>
+      <c r="F40" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
       <c r="A41" s="1">
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C41" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D41" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4">
+        <v>175</v>
+      </c>
+      <c r="E41" t="s">
+        <v>203</v>
+      </c>
+      <c r="F41" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
       <c r="A42" s="1">
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C42" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D42" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4">
+        <v>176</v>
+      </c>
+      <c r="E42" t="s">
+        <v>206</v>
+      </c>
+      <c r="F42" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
       <c r="A43" s="1">
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C43" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D43" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4">
+        <v>177</v>
+      </c>
+      <c r="E43" t="s">
+        <v>202</v>
+      </c>
+      <c r="F43" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
       <c r="A44" s="1">
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C44" t="s">
-        <v>104</v>
+        <v>113</v>
       </c>
       <c r="D44" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4">
+        <v>170</v>
+      </c>
+      <c r="E44" t="s">
+        <v>203</v>
+      </c>
+      <c r="F44" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
       <c r="A45" s="1">
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C45" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="D45" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4">
+        <v>178</v>
+      </c>
+      <c r="E45" t="s">
+        <v>208</v>
+      </c>
+      <c r="F45" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
       <c r="A46" s="1">
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C46" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D46" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4">
+        <v>179</v>
+      </c>
+      <c r="E46" t="s">
+        <v>202</v>
+      </c>
+      <c r="F46" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
       <c r="A47" s="1">
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C47" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="D47" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4">
+        <v>180</v>
+      </c>
+      <c r="E47" t="s">
+        <v>203</v>
+      </c>
+      <c r="F47" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
       <c r="A48" s="1">
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C48" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="D48" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4">
+        <v>181</v>
+      </c>
+      <c r="E48" t="s">
+        <v>202</v>
+      </c>
+      <c r="F48" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6">
       <c r="A49" s="1">
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C49" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="D49" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4">
+        <v>182</v>
+      </c>
+      <c r="E49" t="s">
+        <v>203</v>
+      </c>
+      <c r="F49" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
       <c r="A50" s="1">
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C50" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="D50" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4">
+        <v>183</v>
+      </c>
+      <c r="E50" t="s">
+        <v>202</v>
+      </c>
+      <c r="F50" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6">
       <c r="A51" s="1">
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C51" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="D51" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4">
+        <v>184</v>
+      </c>
+      <c r="E51" t="s">
+        <v>204</v>
+      </c>
+      <c r="F51" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6">
       <c r="A52" s="1">
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C52" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="D52" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4">
+        <v>185</v>
+      </c>
+      <c r="E52" t="s">
+        <v>206</v>
+      </c>
+      <c r="F52" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6">
       <c r="A53" s="1">
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C53" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="D53" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4">
+        <v>186</v>
+      </c>
+      <c r="E53" t="s">
+        <v>203</v>
+      </c>
+      <c r="F53" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6">
       <c r="A54" s="1">
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C54" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D54" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4">
+        <v>187</v>
+      </c>
+      <c r="E54" t="s">
+        <v>203</v>
+      </c>
+      <c r="F54" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6">
       <c r="A55" s="1">
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C55" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D55" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4">
+        <v>188</v>
+      </c>
+      <c r="E55" t="s">
+        <v>203</v>
+      </c>
+      <c r="F55" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6">
       <c r="A56" s="1">
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C56" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D56" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4">
+        <v>189</v>
+      </c>
+      <c r="E56" t="s">
+        <v>203</v>
+      </c>
+      <c r="F56" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6">
       <c r="A57" s="1">
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C57" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D57" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4">
+        <v>190</v>
+      </c>
+      <c r="E57" t="s">
+        <v>202</v>
+      </c>
+      <c r="F57" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6">
       <c r="A58" s="1">
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C58" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D58" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4">
+        <v>191</v>
+      </c>
+      <c r="E58" t="s">
+        <v>202</v>
+      </c>
+      <c r="F58" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6">
       <c r="A59" s="1">
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C59" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D59" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4">
+        <v>192</v>
+      </c>
+      <c r="E59" t="s">
+        <v>203</v>
+      </c>
+      <c r="F59" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6">
       <c r="A60" s="1">
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C60" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D60" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4">
+        <v>193</v>
+      </c>
+      <c r="E60" t="s">
+        <v>202</v>
+      </c>
+      <c r="F60" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6">
       <c r="A61" s="1">
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C61" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D61" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4">
+        <v>194</v>
+      </c>
+      <c r="E61" t="s">
+        <v>204</v>
+      </c>
+      <c r="F61" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6">
       <c r="A62" s="1">
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C62" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D62" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4">
+        <v>195</v>
+      </c>
+      <c r="E62" t="s">
+        <v>203</v>
+      </c>
+      <c r="F62" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6">
       <c r="A63" s="1">
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C63" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D63" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4">
+        <v>196</v>
+      </c>
+      <c r="E63" t="s">
+        <v>203</v>
+      </c>
+      <c r="F63" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6">
       <c r="A64" s="1">
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C64" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D64" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4">
+        <v>197</v>
+      </c>
+      <c r="E64" t="s">
+        <v>203</v>
+      </c>
+      <c r="F64" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6">
       <c r="A65" s="1">
         <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C65" t="s">
-        <v>132</v>
+        <v>91</v>
       </c>
       <c r="D65" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4">
+        <v>198</v>
+      </c>
+      <c r="E65" t="s">
+        <v>202</v>
+      </c>
+      <c r="F65" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6">
       <c r="A66" s="1">
         <v>65</v>
       </c>
       <c r="B66" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C66" t="s">
         <v>133</v>
       </c>
       <c r="D66" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4">
+        <v>199</v>
+      </c>
+      <c r="E66" t="s">
+        <v>203</v>
+      </c>
+      <c r="F66" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6">
       <c r="A67" s="1">
         <v>66</v>
       </c>
       <c r="B67" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C67" t="s">
         <v>134</v>
       </c>
       <c r="D67" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4">
+        <v>200</v>
+      </c>
+      <c r="E67" t="s">
+        <v>208</v>
+      </c>
+      <c r="F67" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6">
       <c r="A68" s="1">
         <v>67</v>
       </c>
       <c r="B68" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C68" t="s">
         <v>135</v>
       </c>
       <c r="D68" t="s">
-        <v>136</v>
+        <v>201</v>
+      </c>
+      <c r="E68" t="s">
+        <v>209</v>
+      </c>
+      <c r="F68" t="s">
+        <v>210</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated on 2018-12-15 at 20:57:58
</commit_message>
<xml_diff>
--- a/index.xlsx
+++ b/index.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="238">
   <si>
     <t>Song Title</t>
   </si>
@@ -67,6 +67,9 @@
     <t>Darkside</t>
   </si>
   <si>
+    <t>Darts In The Dark</t>
+  </si>
+  <si>
     <t>Diamond Heart</t>
   </si>
   <si>
@@ -142,6 +145,9 @@
     <t>Lullaby</t>
   </si>
   <si>
+    <t>MIA</t>
+  </si>
+  <si>
     <t>Magenta Riddim</t>
   </si>
   <si>
@@ -172,6 +178,9 @@
     <t>Remind Me To Forget</t>
   </si>
   <si>
+    <t>Rewrite The Stars</t>
+  </si>
+  <si>
     <t>Right Now</t>
   </si>
   <si>
@@ -190,9 +199,15 @@
     <t>Solo</t>
   </si>
   <si>
+    <t>Sweet But Psycho</t>
+  </si>
+  <si>
     <t>Symphony</t>
   </si>
   <si>
+    <t>Taste The Feeling</t>
+  </si>
+  <si>
     <t>The Nights</t>
   </si>
   <si>
@@ -208,6 +223,9 @@
     <t>Tired</t>
   </si>
   <si>
+    <t>Trampoline</t>
+  </si>
+  <si>
     <t>Wake Me Up</t>
   </si>
   <si>
@@ -268,6 +286,9 @@
     <t>Darkside (Single)</t>
   </si>
   <si>
+    <t>Darts In The Dark (Single)</t>
+  </si>
+  <si>
     <t>Diamond Heart (Single)</t>
   </si>
   <si>
@@ -340,6 +361,9 @@
     <t>Lullaby (Single)</t>
   </si>
   <si>
+    <t>MIA (Single)</t>
+  </si>
+  <si>
     <t>Magenta Riddim (Single)</t>
   </si>
   <si>
@@ -370,6 +394,9 @@
     <t>Remind Me To Forget (Single)</t>
   </si>
   <si>
+    <t>The Greatest Showman: Reimagined</t>
+  </si>
+  <si>
     <t>Right Now (Single)</t>
   </si>
   <si>
@@ -385,9 +412,15 @@
     <t>Solo (Single)</t>
   </si>
   <si>
+    <t>Sweet But Psycho (Single)</t>
+  </si>
+  <si>
     <t>So Good</t>
   </si>
   <si>
+    <t>Taste the Feeling - Single</t>
+  </si>
+  <si>
     <t>NOW That's What I Call Music! 90</t>
   </si>
   <si>
@@ -460,6 +493,9 @@
     <t>Alan Walker, Tomine Harket, Au/Ra</t>
   </si>
   <si>
+    <t>MAGIC!</t>
+  </si>
+  <si>
     <t>Alan Walker, Sophia Somajo</t>
   </si>
   <si>
@@ -535,6 +571,9 @@
     <t>R3hab, Mike Williams</t>
   </si>
   <si>
+    <t>Bad Bunny, Drake</t>
+  </si>
+  <si>
     <t>DJ Snake</t>
   </si>
   <si>
@@ -562,6 +601,9 @@
     <t>Kygo, Miguel</t>
   </si>
   <si>
+    <t>James Arthur, Anne-Marie</t>
+  </si>
+  <si>
     <t>Nick Jonas, Robin Schulz</t>
   </si>
   <si>
@@ -580,9 +622,15 @@
     <t>Clean Bandit, Demi Lovato</t>
   </si>
   <si>
+    <t>Ava Max</t>
+  </si>
+  <si>
     <t>Clean Bandit, Zara Larsson</t>
   </si>
   <si>
+    <t>Avicii, Conrad Sewell</t>
+  </si>
+  <si>
     <t>Avicii</t>
   </si>
   <si>
@@ -598,6 +646,9 @@
     <t>Alan Walker, Gavin James</t>
   </si>
   <si>
+    <t>SHAED</t>
+  </si>
+  <si>
     <t>Avicii, Aloe Blacc</t>
   </si>
   <si>
@@ -641,6 +692,9 @@
   </si>
   <si>
     <t>Rock</t>
+  </si>
+  <si>
+    <t>Alternative</t>
   </si>
   <si>
     <t>R&amp;B/Soul</t>
@@ -1031,7 +1085,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F68"/>
+  <dimension ref="A1:F74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1069,16 +1123,16 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="D2" t="s">
-        <v>136</v>
+        <v>147</v>
       </c>
       <c r="E2" t="s">
-        <v>202</v>
+        <v>219</v>
       </c>
       <c r="F2" t="s">
-        <v>210</v>
+        <v>228</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -1089,16 +1143,16 @@
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="D3" t="s">
-        <v>137</v>
+        <v>148</v>
       </c>
       <c r="E3" t="s">
-        <v>202</v>
+        <v>219</v>
       </c>
       <c r="F3" t="s">
-        <v>210</v>
+        <v>228</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -1109,16 +1163,16 @@
         <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="D4" t="s">
-        <v>138</v>
+        <v>149</v>
       </c>
       <c r="E4" t="s">
-        <v>202</v>
+        <v>219</v>
       </c>
       <c r="F4" t="s">
-        <v>211</v>
+        <v>229</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -1129,16 +1183,16 @@
         <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="D5" t="s">
-        <v>139</v>
+        <v>150</v>
       </c>
       <c r="E5" t="s">
-        <v>202</v>
+        <v>219</v>
       </c>
       <c r="F5" t="s">
-        <v>212</v>
+        <v>230</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -1149,16 +1203,16 @@
         <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="D6" t="s">
-        <v>140</v>
+        <v>151</v>
       </c>
       <c r="E6" t="s">
-        <v>203</v>
+        <v>220</v>
       </c>
       <c r="F6" t="s">
-        <v>213</v>
+        <v>231</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -1169,16 +1223,16 @@
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="D7" t="s">
-        <v>141</v>
+        <v>152</v>
       </c>
       <c r="E7" t="s">
-        <v>204</v>
+        <v>221</v>
       </c>
       <c r="F7" t="s">
-        <v>213</v>
+        <v>231</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -1189,16 +1243,16 @@
         <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="D8" t="s">
-        <v>142</v>
+        <v>153</v>
       </c>
       <c r="E8" t="s">
-        <v>203</v>
+        <v>220</v>
       </c>
       <c r="F8" t="s">
-        <v>210</v>
+        <v>228</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -1209,16 +1263,16 @@
         <v>12</v>
       </c>
       <c r="C9" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="D9" t="s">
-        <v>143</v>
+        <v>154</v>
       </c>
       <c r="E9" t="s">
-        <v>203</v>
+        <v>220</v>
       </c>
       <c r="F9" t="s">
-        <v>210</v>
+        <v>228</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -1229,16 +1283,16 @@
         <v>13</v>
       </c>
       <c r="C10" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="D10" t="s">
-        <v>144</v>
+        <v>155</v>
       </c>
       <c r="E10" t="s">
-        <v>202</v>
+        <v>219</v>
       </c>
       <c r="F10" t="s">
-        <v>210</v>
+        <v>228</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -1249,16 +1303,16 @@
         <v>14</v>
       </c>
       <c r="C11" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="D11" t="s">
-        <v>145</v>
+        <v>156</v>
       </c>
       <c r="E11" t="s">
-        <v>203</v>
+        <v>220</v>
       </c>
       <c r="F11" t="s">
-        <v>213</v>
+        <v>231</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -1269,16 +1323,16 @@
         <v>15</v>
       </c>
       <c r="C12" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="D12" t="s">
-        <v>146</v>
+        <v>157</v>
       </c>
       <c r="E12" t="s">
-        <v>205</v>
+        <v>222</v>
       </c>
       <c r="F12" t="s">
-        <v>214</v>
+        <v>232</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -1289,16 +1343,16 @@
         <v>16</v>
       </c>
       <c r="C13" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="D13" t="s">
-        <v>147</v>
+        <v>158</v>
       </c>
       <c r="E13" t="s">
-        <v>202</v>
+        <v>219</v>
       </c>
       <c r="F13" t="s">
-        <v>213</v>
+        <v>231</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -1309,16 +1363,16 @@
         <v>17</v>
       </c>
       <c r="C14" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="D14" t="s">
-        <v>148</v>
+        <v>159</v>
       </c>
       <c r="E14" t="s">
-        <v>202</v>
+        <v>220</v>
       </c>
       <c r="F14" t="s">
-        <v>213</v>
+        <v>228</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -1329,16 +1383,16 @@
         <v>18</v>
       </c>
       <c r="C15" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="D15" t="s">
-        <v>149</v>
+        <v>160</v>
       </c>
       <c r="E15" t="s">
-        <v>202</v>
+        <v>219</v>
       </c>
       <c r="F15" t="s">
-        <v>213</v>
+        <v>231</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -1349,16 +1403,16 @@
         <v>19</v>
       </c>
       <c r="C16" t="s">
-        <v>19</v>
+        <v>92</v>
       </c>
       <c r="D16" t="s">
-        <v>150</v>
+        <v>161</v>
       </c>
       <c r="E16" t="s">
-        <v>202</v>
+        <v>219</v>
       </c>
       <c r="F16" t="s">
-        <v>211</v>
+        <v>231</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -1369,16 +1423,16 @@
         <v>20</v>
       </c>
       <c r="C17" t="s">
-        <v>86</v>
+        <v>20</v>
       </c>
       <c r="D17" t="s">
-        <v>151</v>
+        <v>162</v>
       </c>
       <c r="E17" t="s">
-        <v>203</v>
+        <v>219</v>
       </c>
       <c r="F17" t="s">
-        <v>210</v>
+        <v>229</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -1389,16 +1443,16 @@
         <v>21</v>
       </c>
       <c r="C18" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="D18" t="s">
-        <v>152</v>
+        <v>163</v>
       </c>
       <c r="E18" t="s">
-        <v>203</v>
+        <v>220</v>
       </c>
       <c r="F18" t="s">
-        <v>213</v>
+        <v>228</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -1409,16 +1463,16 @@
         <v>22</v>
       </c>
       <c r="C19" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="D19" t="s">
-        <v>153</v>
+        <v>164</v>
       </c>
       <c r="E19" t="s">
-        <v>202</v>
+        <v>220</v>
       </c>
       <c r="F19" t="s">
-        <v>215</v>
+        <v>231</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -1429,16 +1483,16 @@
         <v>23</v>
       </c>
       <c r="C20" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="D20" t="s">
-        <v>154</v>
+        <v>165</v>
       </c>
       <c r="E20" t="s">
-        <v>202</v>
+        <v>219</v>
       </c>
       <c r="F20" t="s">
-        <v>213</v>
+        <v>233</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -1449,16 +1503,16 @@
         <v>24</v>
       </c>
       <c r="C21" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="D21" t="s">
-        <v>155</v>
+        <v>166</v>
       </c>
       <c r="E21" t="s">
-        <v>203</v>
+        <v>219</v>
       </c>
       <c r="F21" t="s">
-        <v>213</v>
+        <v>231</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -1469,16 +1523,16 @@
         <v>25</v>
       </c>
       <c r="C22" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="D22" t="s">
-        <v>156</v>
+        <v>167</v>
       </c>
       <c r="E22" t="s">
-        <v>202</v>
+        <v>220</v>
       </c>
       <c r="F22" t="s">
-        <v>210</v>
+        <v>231</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -1489,16 +1543,16 @@
         <v>26</v>
       </c>
       <c r="C23" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="D23" t="s">
-        <v>157</v>
+        <v>168</v>
       </c>
       <c r="E23" t="s">
-        <v>202</v>
+        <v>219</v>
       </c>
       <c r="F23" t="s">
-        <v>213</v>
+        <v>228</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -1509,16 +1563,16 @@
         <v>27</v>
       </c>
       <c r="C24" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="D24" t="s">
-        <v>158</v>
+        <v>169</v>
       </c>
       <c r="E24" t="s">
-        <v>203</v>
+        <v>219</v>
       </c>
       <c r="F24" t="s">
-        <v>213</v>
+        <v>231</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -1529,16 +1583,16 @@
         <v>28</v>
       </c>
       <c r="C25" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="D25" t="s">
-        <v>159</v>
+        <v>170</v>
       </c>
       <c r="E25" t="s">
-        <v>206</v>
+        <v>220</v>
       </c>
       <c r="F25" t="s">
-        <v>213</v>
+        <v>231</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -1549,16 +1603,16 @@
         <v>29</v>
       </c>
       <c r="C26" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="D26" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="E26" t="s">
-        <v>202</v>
+        <v>223</v>
       </c>
       <c r="F26" t="s">
-        <v>213</v>
+        <v>231</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -1569,16 +1623,16 @@
         <v>30</v>
       </c>
       <c r="C27" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="D27" t="s">
-        <v>161</v>
+        <v>172</v>
       </c>
       <c r="E27" t="s">
-        <v>203</v>
+        <v>219</v>
       </c>
       <c r="F27" t="s">
-        <v>213</v>
+        <v>231</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -1589,16 +1643,16 @@
         <v>31</v>
       </c>
       <c r="C28" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="D28" t="s">
-        <v>162</v>
+        <v>173</v>
       </c>
       <c r="E28" t="s">
-        <v>203</v>
+        <v>220</v>
       </c>
       <c r="F28" t="s">
-        <v>210</v>
+        <v>231</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -1609,16 +1663,16 @@
         <v>32</v>
       </c>
       <c r="C29" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="D29" t="s">
-        <v>163</v>
+        <v>174</v>
       </c>
       <c r="E29" t="s">
-        <v>202</v>
+        <v>220</v>
       </c>
       <c r="F29" t="s">
-        <v>213</v>
+        <v>228</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -1629,16 +1683,16 @@
         <v>33</v>
       </c>
       <c r="C30" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="D30" t="s">
-        <v>164</v>
+        <v>175</v>
       </c>
       <c r="E30" t="s">
-        <v>202</v>
+        <v>219</v>
       </c>
       <c r="F30" t="s">
-        <v>213</v>
+        <v>231</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -1649,16 +1703,16 @@
         <v>34</v>
       </c>
       <c r="C31" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="D31" t="s">
-        <v>165</v>
+        <v>176</v>
       </c>
       <c r="E31" t="s">
-        <v>202</v>
+        <v>219</v>
       </c>
       <c r="F31" t="s">
-        <v>210</v>
+        <v>231</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -1669,16 +1723,16 @@
         <v>35</v>
       </c>
       <c r="C32" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="D32" t="s">
-        <v>166</v>
+        <v>177</v>
       </c>
       <c r="E32" t="s">
-        <v>202</v>
+        <v>219</v>
       </c>
       <c r="F32" t="s">
-        <v>213</v>
+        <v>228</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -1689,16 +1743,16 @@
         <v>36</v>
       </c>
       <c r="C33" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="D33" t="s">
-        <v>167</v>
+        <v>178</v>
       </c>
       <c r="E33" t="s">
-        <v>202</v>
+        <v>219</v>
       </c>
       <c r="F33" t="s">
-        <v>211</v>
+        <v>231</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -1709,16 +1763,16 @@
         <v>37</v>
       </c>
       <c r="C34" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="D34" t="s">
-        <v>168</v>
+        <v>179</v>
       </c>
       <c r="E34" t="s">
-        <v>202</v>
+        <v>219</v>
       </c>
       <c r="F34" t="s">
-        <v>213</v>
+        <v>229</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -1729,16 +1783,16 @@
         <v>38</v>
       </c>
       <c r="C35" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="D35" t="s">
-        <v>169</v>
+        <v>180</v>
       </c>
       <c r="E35" t="s">
-        <v>207</v>
+        <v>219</v>
       </c>
       <c r="F35" t="s">
-        <v>215</v>
+        <v>231</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -1749,16 +1803,16 @@
         <v>39</v>
       </c>
       <c r="C36" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="D36" t="s">
-        <v>170</v>
+        <v>181</v>
       </c>
       <c r="E36" t="s">
-        <v>203</v>
+        <v>224</v>
       </c>
       <c r="F36" t="s">
-        <v>215</v>
+        <v>233</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -1769,16 +1823,16 @@
         <v>40</v>
       </c>
       <c r="C37" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="D37" t="s">
-        <v>171</v>
+        <v>182</v>
       </c>
       <c r="E37" t="s">
-        <v>202</v>
+        <v>220</v>
       </c>
       <c r="F37" t="s">
-        <v>216</v>
+        <v>233</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -1789,16 +1843,16 @@
         <v>41</v>
       </c>
       <c r="C38" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="D38" t="s">
-        <v>172</v>
+        <v>183</v>
       </c>
       <c r="E38" t="s">
-        <v>202</v>
+        <v>219</v>
       </c>
       <c r="F38" t="s">
-        <v>213</v>
+        <v>234</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -1809,16 +1863,16 @@
         <v>42</v>
       </c>
       <c r="C39" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="D39" t="s">
-        <v>173</v>
+        <v>184</v>
       </c>
       <c r="E39" t="s">
-        <v>202</v>
+        <v>219</v>
       </c>
       <c r="F39" t="s">
-        <v>213</v>
+        <v>231</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -1829,16 +1883,16 @@
         <v>43</v>
       </c>
       <c r="C40" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="D40" t="s">
-        <v>174</v>
+        <v>185</v>
       </c>
       <c r="E40" t="s">
-        <v>206</v>
+        <v>223</v>
       </c>
       <c r="F40" t="s">
-        <v>217</v>
+        <v>231</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -1849,16 +1903,16 @@
         <v>44</v>
       </c>
       <c r="C41" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="D41" t="s">
-        <v>175</v>
+        <v>186</v>
       </c>
       <c r="E41" t="s">
-        <v>203</v>
+        <v>219</v>
       </c>
       <c r="F41" t="s">
-        <v>213</v>
+        <v>231</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -1869,16 +1923,16 @@
         <v>45</v>
       </c>
       <c r="C42" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="D42" t="s">
-        <v>176</v>
+        <v>187</v>
       </c>
       <c r="E42" t="s">
-        <v>206</v>
+        <v>223</v>
       </c>
       <c r="F42" t="s">
-        <v>213</v>
+        <v>235</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -1889,16 +1943,16 @@
         <v>46</v>
       </c>
       <c r="C43" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="D43" t="s">
-        <v>177</v>
+        <v>188</v>
       </c>
       <c r="E43" t="s">
-        <v>202</v>
+        <v>220</v>
       </c>
       <c r="F43" t="s">
-        <v>213</v>
+        <v>231</v>
       </c>
     </row>
     <row r="44" spans="1:6">
@@ -1909,16 +1963,16 @@
         <v>47</v>
       </c>
       <c r="C44" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="D44" t="s">
-        <v>170</v>
+        <v>189</v>
       </c>
       <c r="E44" t="s">
-        <v>203</v>
+        <v>223</v>
       </c>
       <c r="F44" t="s">
-        <v>212</v>
+        <v>231</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -1929,16 +1983,16 @@
         <v>48</v>
       </c>
       <c r="C45" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="D45" t="s">
-        <v>178</v>
+        <v>190</v>
       </c>
       <c r="E45" t="s">
-        <v>208</v>
+        <v>219</v>
       </c>
       <c r="F45" t="s">
-        <v>218</v>
+        <v>231</v>
       </c>
     </row>
     <row r="46" spans="1:6">
@@ -1949,16 +2003,16 @@
         <v>49</v>
       </c>
       <c r="C46" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="D46" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="E46" t="s">
-        <v>202</v>
+        <v>220</v>
       </c>
       <c r="F46" t="s">
-        <v>210</v>
+        <v>230</v>
       </c>
     </row>
     <row r="47" spans="1:6">
@@ -1969,16 +2023,16 @@
         <v>50</v>
       </c>
       <c r="C47" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="D47" t="s">
-        <v>180</v>
+        <v>191</v>
       </c>
       <c r="E47" t="s">
-        <v>203</v>
+        <v>225</v>
       </c>
       <c r="F47" t="s">
-        <v>210</v>
+        <v>236</v>
       </c>
     </row>
     <row r="48" spans="1:6">
@@ -1989,16 +2043,16 @@
         <v>51</v>
       </c>
       <c r="C48" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="D48" t="s">
-        <v>181</v>
+        <v>192</v>
       </c>
       <c r="E48" t="s">
-        <v>202</v>
+        <v>219</v>
       </c>
       <c r="F48" t="s">
-        <v>213</v>
+        <v>228</v>
       </c>
     </row>
     <row r="49" spans="1:6">
@@ -2009,16 +2063,16 @@
         <v>52</v>
       </c>
       <c r="C49" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="D49" t="s">
-        <v>182</v>
+        <v>193</v>
       </c>
       <c r="E49" t="s">
-        <v>203</v>
+        <v>220</v>
       </c>
       <c r="F49" t="s">
-        <v>213</v>
+        <v>228</v>
       </c>
     </row>
     <row r="50" spans="1:6">
@@ -2029,16 +2083,16 @@
         <v>53</v>
       </c>
       <c r="C50" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="D50" t="s">
-        <v>183</v>
+        <v>194</v>
       </c>
       <c r="E50" t="s">
-        <v>202</v>
+        <v>219</v>
       </c>
       <c r="F50" t="s">
-        <v>213</v>
+        <v>231</v>
       </c>
     </row>
     <row r="51" spans="1:6">
@@ -2049,16 +2103,16 @@
         <v>54</v>
       </c>
       <c r="C51" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="D51" t="s">
-        <v>184</v>
+        <v>195</v>
       </c>
       <c r="E51" t="s">
-        <v>204</v>
+        <v>224</v>
       </c>
       <c r="F51" t="s">
-        <v>211</v>
+        <v>231</v>
       </c>
     </row>
     <row r="52" spans="1:6">
@@ -2069,16 +2123,16 @@
         <v>55</v>
       </c>
       <c r="C52" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="D52" t="s">
-        <v>185</v>
+        <v>196</v>
       </c>
       <c r="E52" t="s">
-        <v>206</v>
+        <v>220</v>
       </c>
       <c r="F52" t="s">
-        <v>213</v>
+        <v>231</v>
       </c>
     </row>
     <row r="53" spans="1:6">
@@ -2089,16 +2143,16 @@
         <v>56</v>
       </c>
       <c r="C53" t="s">
-        <v>109</v>
+        <v>128</v>
       </c>
       <c r="D53" t="s">
-        <v>186</v>
+        <v>197</v>
       </c>
       <c r="E53" t="s">
-        <v>203</v>
+        <v>219</v>
       </c>
       <c r="F53" t="s">
-        <v>211</v>
+        <v>231</v>
       </c>
     </row>
     <row r="54" spans="1:6">
@@ -2109,16 +2163,16 @@
         <v>57</v>
       </c>
       <c r="C54" t="s">
-        <v>122</v>
+        <v>129</v>
       </c>
       <c r="D54" t="s">
-        <v>187</v>
+        <v>198</v>
       </c>
       <c r="E54" t="s">
-        <v>203</v>
+        <v>221</v>
       </c>
       <c r="F54" t="s">
-        <v>213</v>
+        <v>229</v>
       </c>
     </row>
     <row r="55" spans="1:6">
@@ -2129,16 +2183,16 @@
         <v>58</v>
       </c>
       <c r="C55" t="s">
-        <v>123</v>
+        <v>130</v>
       </c>
       <c r="D55" t="s">
-        <v>188</v>
+        <v>199</v>
       </c>
       <c r="E55" t="s">
-        <v>203</v>
+        <v>223</v>
       </c>
       <c r="F55" t="s">
-        <v>210</v>
+        <v>231</v>
       </c>
     </row>
     <row r="56" spans="1:6">
@@ -2149,16 +2203,16 @@
         <v>59</v>
       </c>
       <c r="C56" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="D56" t="s">
-        <v>189</v>
+        <v>200</v>
       </c>
       <c r="E56" t="s">
-        <v>203</v>
+        <v>220</v>
       </c>
       <c r="F56" t="s">
-        <v>215</v>
+        <v>229</v>
       </c>
     </row>
     <row r="57" spans="1:6">
@@ -2169,16 +2223,16 @@
         <v>60</v>
       </c>
       <c r="C57" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="D57" t="s">
-        <v>190</v>
+        <v>201</v>
       </c>
       <c r="E57" t="s">
-        <v>202</v>
+        <v>220</v>
       </c>
       <c r="F57" t="s">
-        <v>213</v>
+        <v>231</v>
       </c>
     </row>
     <row r="58" spans="1:6">
@@ -2189,16 +2243,16 @@
         <v>61</v>
       </c>
       <c r="C58" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="D58" t="s">
-        <v>191</v>
+        <v>202</v>
       </c>
       <c r="E58" t="s">
-        <v>202</v>
+        <v>220</v>
       </c>
       <c r="F58" t="s">
-        <v>213</v>
+        <v>231</v>
       </c>
     </row>
     <row r="59" spans="1:6">
@@ -2209,16 +2263,16 @@
         <v>62</v>
       </c>
       <c r="C59" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="D59" t="s">
-        <v>192</v>
+        <v>203</v>
       </c>
       <c r="E59" t="s">
-        <v>203</v>
+        <v>220</v>
       </c>
       <c r="F59" t="s">
-        <v>213</v>
+        <v>228</v>
       </c>
     </row>
     <row r="60" spans="1:6">
@@ -2229,16 +2283,16 @@
         <v>63</v>
       </c>
       <c r="C60" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="D60" t="s">
-        <v>193</v>
+        <v>204</v>
       </c>
       <c r="E60" t="s">
-        <v>202</v>
+        <v>219</v>
       </c>
       <c r="F60" t="s">
-        <v>210</v>
+        <v>229</v>
       </c>
     </row>
     <row r="61" spans="1:6">
@@ -2249,16 +2303,16 @@
         <v>64</v>
       </c>
       <c r="C61" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="D61" t="s">
-        <v>194</v>
+        <v>205</v>
       </c>
       <c r="E61" t="s">
-        <v>204</v>
+        <v>220</v>
       </c>
       <c r="F61" t="s">
-        <v>219</v>
+        <v>233</v>
       </c>
     </row>
     <row r="62" spans="1:6">
@@ -2269,16 +2323,16 @@
         <v>65</v>
       </c>
       <c r="C62" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="D62" t="s">
-        <v>195</v>
+        <v>206</v>
       </c>
       <c r="E62" t="s">
-        <v>203</v>
+        <v>219</v>
       </c>
       <c r="F62" t="s">
-        <v>213</v>
+        <v>231</v>
       </c>
     </row>
     <row r="63" spans="1:6">
@@ -2289,16 +2343,16 @@
         <v>66</v>
       </c>
       <c r="C63" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="D63" t="s">
-        <v>196</v>
+        <v>207</v>
       </c>
       <c r="E63" t="s">
-        <v>203</v>
+        <v>219</v>
       </c>
       <c r="F63" t="s">
-        <v>211</v>
+        <v>231</v>
       </c>
     </row>
     <row r="64" spans="1:6">
@@ -2309,16 +2363,16 @@
         <v>67</v>
       </c>
       <c r="C64" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="D64" t="s">
-        <v>197</v>
+        <v>208</v>
       </c>
       <c r="E64" t="s">
-        <v>203</v>
+        <v>220</v>
       </c>
       <c r="F64" t="s">
-        <v>213</v>
+        <v>231</v>
       </c>
     </row>
     <row r="65" spans="1:6">
@@ -2329,16 +2383,16 @@
         <v>68</v>
       </c>
       <c r="C65" t="s">
-        <v>91</v>
+        <v>139</v>
       </c>
       <c r="D65" t="s">
-        <v>198</v>
+        <v>209</v>
       </c>
       <c r="E65" t="s">
-        <v>202</v>
+        <v>219</v>
       </c>
       <c r="F65" t="s">
-        <v>210</v>
+        <v>228</v>
       </c>
     </row>
     <row r="66" spans="1:6">
@@ -2349,16 +2403,16 @@
         <v>69</v>
       </c>
       <c r="C66" t="s">
-        <v>133</v>
+        <v>69</v>
       </c>
       <c r="D66" t="s">
-        <v>199</v>
+        <v>210</v>
       </c>
       <c r="E66" t="s">
-        <v>203</v>
+        <v>226</v>
       </c>
       <c r="F66" t="s">
-        <v>210</v>
+        <v>231</v>
       </c>
     </row>
     <row r="67" spans="1:6">
@@ -2369,16 +2423,16 @@
         <v>70</v>
       </c>
       <c r="C67" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="D67" t="s">
-        <v>200</v>
+        <v>211</v>
       </c>
       <c r="E67" t="s">
-        <v>208</v>
+        <v>221</v>
       </c>
       <c r="F67" t="s">
-        <v>219</v>
+        <v>237</v>
       </c>
     </row>
     <row r="68" spans="1:6">
@@ -2389,16 +2443,136 @@
         <v>71</v>
       </c>
       <c r="C68" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="D68" t="s">
-        <v>201</v>
+        <v>212</v>
       </c>
       <c r="E68" t="s">
-        <v>209</v>
+        <v>220</v>
       </c>
       <c r="F68" t="s">
-        <v>210</v>
+        <v>231</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6">
+      <c r="A69" s="1">
+        <v>68</v>
+      </c>
+      <c r="B69" t="s">
+        <v>72</v>
+      </c>
+      <c r="C69" t="s">
+        <v>142</v>
+      </c>
+      <c r="D69" t="s">
+        <v>213</v>
+      </c>
+      <c r="E69" t="s">
+        <v>220</v>
+      </c>
+      <c r="F69" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6">
+      <c r="A70" s="1">
+        <v>69</v>
+      </c>
+      <c r="B70" t="s">
+        <v>73</v>
+      </c>
+      <c r="C70" t="s">
+        <v>143</v>
+      </c>
+      <c r="D70" t="s">
+        <v>214</v>
+      </c>
+      <c r="E70" t="s">
+        <v>220</v>
+      </c>
+      <c r="F70" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6">
+      <c r="A71" s="1">
+        <v>70</v>
+      </c>
+      <c r="B71" t="s">
+        <v>74</v>
+      </c>
+      <c r="C71" t="s">
+        <v>98</v>
+      </c>
+      <c r="D71" t="s">
+        <v>215</v>
+      </c>
+      <c r="E71" t="s">
+        <v>219</v>
+      </c>
+      <c r="F71" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6">
+      <c r="A72" s="1">
+        <v>71</v>
+      </c>
+      <c r="B72" t="s">
+        <v>75</v>
+      </c>
+      <c r="C72" t="s">
+        <v>144</v>
+      </c>
+      <c r="D72" t="s">
+        <v>216</v>
+      </c>
+      <c r="E72" t="s">
+        <v>220</v>
+      </c>
+      <c r="F72" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6">
+      <c r="A73" s="1">
+        <v>72</v>
+      </c>
+      <c r="B73" t="s">
+        <v>76</v>
+      </c>
+      <c r="C73" t="s">
+        <v>145</v>
+      </c>
+      <c r="D73" t="s">
+        <v>217</v>
+      </c>
+      <c r="E73" t="s">
+        <v>225</v>
+      </c>
+      <c r="F73" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6">
+      <c r="A74" s="1">
+        <v>73</v>
+      </c>
+      <c r="B74" t="s">
+        <v>77</v>
+      </c>
+      <c r="C74" t="s">
+        <v>146</v>
+      </c>
+      <c r="D74" t="s">
+        <v>218</v>
+      </c>
+      <c r="E74" t="s">
+        <v>227</v>
+      </c>
+      <c r="F74" t="s">
+        <v>228</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated on 2018-12-15 at 22:46:10
</commit_message>
<xml_diff>
--- a/index.xlsx
+++ b/index.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="246">
   <si>
     <t>Song Title</t>
   </si>
@@ -34,6 +34,9 @@
     <t>2U</t>
   </si>
   <si>
+    <t>Ain't That Why</t>
+  </si>
+  <si>
     <t>All Falls Down</t>
   </si>
   <si>
@@ -55,6 +58,9 @@
     <t>Battle Symphony</t>
   </si>
   <si>
+    <t>Blank Space</t>
+  </si>
+  <si>
     <t>Complicated</t>
   </si>
   <si>
@@ -121,6 +127,9 @@
     <t>Ignite</t>
   </si>
   <si>
+    <t>In My Blood</t>
+  </si>
+  <si>
     <t>It Ain't Me</t>
   </si>
   <si>
@@ -253,6 +262,9 @@
     <t>2U (Single)</t>
   </si>
   <si>
+    <t>Ain't That Why (Single)</t>
+  </si>
+  <si>
     <t>All Falls Down (Single)</t>
   </si>
   <si>
@@ -274,6 +286,9 @@
     <t>Battle Symphony (Single)</t>
   </si>
   <si>
+    <t>1989 (Deluxe Edition)</t>
+  </si>
+  <si>
     <t>Complicated (Single)</t>
   </si>
   <si>
@@ -337,6 +352,9 @@
     <t>Ignite (Single)</t>
   </si>
   <si>
+    <t>In My Blood (Single)</t>
+  </si>
+  <si>
     <t>It Ain't Me (Single)</t>
   </si>
   <si>
@@ -481,6 +499,9 @@
     <t>Linkin Park</t>
   </si>
   <si>
+    <t>Taylor Swift</t>
+  </si>
+  <si>
     <t>Dimitri Vegas &amp; Like Mike, David Guetta, Kiiara</t>
   </si>
   <si>
@@ -545,6 +566,9 @@
   </si>
   <si>
     <t>K-391, Alan Walker, Julie Bergan, Seungri</t>
+  </si>
+  <si>
+    <t>Shawn Mendes</t>
   </si>
   <si>
     <t>Kygo, Selena Gomez</t>
@@ -1085,7 +1109,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F74"/>
+  <dimension ref="A1:F77"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1095,7 +1119,7 @@
     <col min="2" max="2" width="58.7109375" customWidth="1"/>
     <col min="3" max="3" width="51.7109375" customWidth="1"/>
     <col min="4" max="4" width="13.7109375" customWidth="1"/>
-    <col min="5" max="5" width="5.7109375" customWidth="1"/>
+    <col min="5" max="5" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -1123,16 +1147,16 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="D2" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="E2" t="s">
-        <v>219</v>
+        <v>227</v>
       </c>
       <c r="F2" t="s">
-        <v>228</v>
+        <v>236</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -1143,16 +1167,16 @@
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="D3" t="s">
-        <v>148</v>
+        <v>123</v>
       </c>
       <c r="E3" t="s">
-        <v>219</v>
+        <v>227</v>
       </c>
       <c r="F3" t="s">
-        <v>228</v>
+        <v>123</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -1163,16 +1187,16 @@
         <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="D4" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
       <c r="E4" t="s">
-        <v>219</v>
+        <v>227</v>
       </c>
       <c r="F4" t="s">
-        <v>229</v>
+        <v>236</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -1183,16 +1207,16 @@
         <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="D5" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="E5" t="s">
-        <v>219</v>
+        <v>227</v>
       </c>
       <c r="F5" t="s">
-        <v>230</v>
+        <v>237</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -1203,16 +1227,16 @@
         <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="D6" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="E6" t="s">
-        <v>220</v>
+        <v>227</v>
       </c>
       <c r="F6" t="s">
-        <v>231</v>
+        <v>238</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -1223,16 +1247,16 @@
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="D7" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="E7" t="s">
-        <v>221</v>
+        <v>228</v>
       </c>
       <c r="F7" t="s">
-        <v>231</v>
+        <v>239</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -1243,16 +1267,16 @@
         <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="D8" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="E8" t="s">
-        <v>220</v>
+        <v>229</v>
       </c>
       <c r="F8" t="s">
-        <v>228</v>
+        <v>239</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -1263,16 +1287,16 @@
         <v>12</v>
       </c>
       <c r="C9" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="D9" t="s">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="E9" t="s">
-        <v>220</v>
+        <v>228</v>
       </c>
       <c r="F9" t="s">
-        <v>228</v>
+        <v>236</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -1283,16 +1307,16 @@
         <v>13</v>
       </c>
       <c r="C10" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="D10" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="E10" t="s">
-        <v>219</v>
+        <v>228</v>
       </c>
       <c r="F10" t="s">
-        <v>228</v>
+        <v>236</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -1303,16 +1327,16 @@
         <v>14</v>
       </c>
       <c r="C11" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="D11" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
       <c r="E11" t="s">
-        <v>220</v>
+        <v>228</v>
       </c>
       <c r="F11" t="s">
-        <v>231</v>
+        <v>123</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -1323,16 +1347,16 @@
         <v>15</v>
       </c>
       <c r="C12" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="D12" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
       <c r="E12" t="s">
-        <v>222</v>
+        <v>227</v>
       </c>
       <c r="F12" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -1343,16 +1367,16 @@
         <v>16</v>
       </c>
       <c r="C13" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="D13" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="E13" t="s">
-        <v>219</v>
+        <v>228</v>
       </c>
       <c r="F13" t="s">
-        <v>231</v>
+        <v>239</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -1363,16 +1387,16 @@
         <v>17</v>
       </c>
       <c r="C14" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="D14" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
       <c r="E14" t="s">
-        <v>220</v>
+        <v>230</v>
       </c>
       <c r="F14" t="s">
-        <v>228</v>
+        <v>240</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -1383,16 +1407,16 @@
         <v>18</v>
       </c>
       <c r="C15" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="D15" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
       <c r="E15" t="s">
-        <v>219</v>
+        <v>227</v>
       </c>
       <c r="F15" t="s">
-        <v>231</v>
+        <v>239</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -1403,16 +1427,16 @@
         <v>19</v>
       </c>
       <c r="C16" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="D16" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="E16" t="s">
-        <v>219</v>
+        <v>228</v>
       </c>
       <c r="F16" t="s">
-        <v>231</v>
+        <v>236</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -1423,16 +1447,16 @@
         <v>20</v>
       </c>
       <c r="C17" t="s">
-        <v>20</v>
+        <v>96</v>
       </c>
       <c r="D17" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
       <c r="E17" t="s">
-        <v>219</v>
+        <v>227</v>
       </c>
       <c r="F17" t="s">
-        <v>229</v>
+        <v>239</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -1443,16 +1467,16 @@
         <v>21</v>
       </c>
       <c r="C18" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="D18" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="E18" t="s">
-        <v>220</v>
+        <v>227</v>
       </c>
       <c r="F18" t="s">
-        <v>228</v>
+        <v>239</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -1463,16 +1487,16 @@
         <v>22</v>
       </c>
       <c r="C19" t="s">
-        <v>94</v>
+        <v>22</v>
       </c>
       <c r="D19" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="E19" t="s">
-        <v>220</v>
+        <v>227</v>
       </c>
       <c r="F19" t="s">
-        <v>231</v>
+        <v>237</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -1483,16 +1507,16 @@
         <v>23</v>
       </c>
       <c r="C20" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="D20" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
       <c r="E20" t="s">
-        <v>219</v>
+        <v>228</v>
       </c>
       <c r="F20" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -1503,16 +1527,16 @@
         <v>24</v>
       </c>
       <c r="C21" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="D21" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="E21" t="s">
-        <v>219</v>
+        <v>228</v>
       </c>
       <c r="F21" t="s">
-        <v>231</v>
+        <v>239</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -1523,16 +1547,16 @@
         <v>25</v>
       </c>
       <c r="C22" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="D22" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
       <c r="E22" t="s">
-        <v>220</v>
+        <v>227</v>
       </c>
       <c r="F22" t="s">
-        <v>231</v>
+        <v>241</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -1543,16 +1567,16 @@
         <v>26</v>
       </c>
       <c r="C23" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="D23" t="s">
-        <v>168</v>
+        <v>173</v>
       </c>
       <c r="E23" t="s">
-        <v>219</v>
+        <v>227</v>
       </c>
       <c r="F23" t="s">
-        <v>228</v>
+        <v>239</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -1563,16 +1587,16 @@
         <v>27</v>
       </c>
       <c r="C24" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="D24" t="s">
-        <v>169</v>
+        <v>174</v>
       </c>
       <c r="E24" t="s">
-        <v>219</v>
+        <v>228</v>
       </c>
       <c r="F24" t="s">
-        <v>231</v>
+        <v>239</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -1583,16 +1607,16 @@
         <v>28</v>
       </c>
       <c r="C25" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="D25" t="s">
-        <v>170</v>
+        <v>175</v>
       </c>
       <c r="E25" t="s">
-        <v>220</v>
+        <v>227</v>
       </c>
       <c r="F25" t="s">
-        <v>231</v>
+        <v>236</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -1603,16 +1627,16 @@
         <v>29</v>
       </c>
       <c r="C26" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="D26" t="s">
-        <v>171</v>
+        <v>176</v>
       </c>
       <c r="E26" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="F26" t="s">
-        <v>231</v>
+        <v>239</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -1623,16 +1647,16 @@
         <v>30</v>
       </c>
       <c r="C27" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="D27" t="s">
-        <v>172</v>
+        <v>177</v>
       </c>
       <c r="E27" t="s">
-        <v>219</v>
+        <v>228</v>
       </c>
       <c r="F27" t="s">
-        <v>231</v>
+        <v>239</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -1643,16 +1667,16 @@
         <v>31</v>
       </c>
       <c r="C28" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="D28" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
       <c r="E28" t="s">
-        <v>220</v>
+        <v>231</v>
       </c>
       <c r="F28" t="s">
-        <v>231</v>
+        <v>239</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -1663,16 +1687,16 @@
         <v>32</v>
       </c>
       <c r="C29" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="D29" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="E29" t="s">
-        <v>220</v>
+        <v>227</v>
       </c>
       <c r="F29" t="s">
-        <v>228</v>
+        <v>239</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -1683,16 +1707,16 @@
         <v>33</v>
       </c>
       <c r="C30" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="D30" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
       <c r="E30" t="s">
-        <v>219</v>
+        <v>228</v>
       </c>
       <c r="F30" t="s">
-        <v>231</v>
+        <v>239</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -1703,16 +1727,16 @@
         <v>34</v>
       </c>
       <c r="C31" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="D31" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
       <c r="E31" t="s">
-        <v>219</v>
+        <v>228</v>
       </c>
       <c r="F31" t="s">
-        <v>231</v>
+        <v>236</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -1723,16 +1747,16 @@
         <v>35</v>
       </c>
       <c r="C32" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="D32" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
       <c r="E32" t="s">
-        <v>219</v>
+        <v>227</v>
       </c>
       <c r="F32" t="s">
-        <v>228</v>
+        <v>239</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -1743,16 +1767,16 @@
         <v>36</v>
       </c>
       <c r="C33" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="D33" t="s">
-        <v>178</v>
+        <v>183</v>
       </c>
       <c r="E33" t="s">
-        <v>219</v>
+        <v>227</v>
       </c>
       <c r="F33" t="s">
-        <v>231</v>
+        <v>239</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -1763,16 +1787,16 @@
         <v>37</v>
       </c>
       <c r="C34" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="D34" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
       <c r="E34" t="s">
-        <v>219</v>
+        <v>228</v>
       </c>
       <c r="F34" t="s">
-        <v>229</v>
+        <v>123</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -1783,16 +1807,16 @@
         <v>38</v>
       </c>
       <c r="C35" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="D35" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="E35" t="s">
-        <v>219</v>
+        <v>227</v>
       </c>
       <c r="F35" t="s">
-        <v>231</v>
+        <v>236</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -1803,16 +1827,16 @@
         <v>39</v>
       </c>
       <c r="C36" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="D36" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="E36" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="F36" t="s">
-        <v>233</v>
+        <v>239</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -1823,16 +1847,16 @@
         <v>40</v>
       </c>
       <c r="C37" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="D37" t="s">
-        <v>182</v>
+        <v>187</v>
       </c>
       <c r="E37" t="s">
-        <v>220</v>
+        <v>227</v>
       </c>
       <c r="F37" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -1843,16 +1867,16 @@
         <v>41</v>
       </c>
       <c r="C38" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="D38" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="E38" t="s">
-        <v>219</v>
+        <v>227</v>
       </c>
       <c r="F38" t="s">
-        <v>234</v>
+        <v>239</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -1863,16 +1887,16 @@
         <v>42</v>
       </c>
       <c r="C39" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="D39" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
       <c r="E39" t="s">
-        <v>219</v>
+        <v>232</v>
       </c>
       <c r="F39" t="s">
-        <v>231</v>
+        <v>241</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -1883,16 +1907,16 @@
         <v>43</v>
       </c>
       <c r="C40" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="D40" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
       <c r="E40" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="F40" t="s">
-        <v>231</v>
+        <v>241</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -1903,16 +1927,16 @@
         <v>44</v>
       </c>
       <c r="C41" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="D41" t="s">
-        <v>186</v>
+        <v>191</v>
       </c>
       <c r="E41" t="s">
-        <v>219</v>
+        <v>227</v>
       </c>
       <c r="F41" t="s">
-        <v>231</v>
+        <v>242</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -1923,16 +1947,16 @@
         <v>45</v>
       </c>
       <c r="C42" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="D42" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
       <c r="E42" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="F42" t="s">
-        <v>235</v>
+        <v>239</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -1943,16 +1967,16 @@
         <v>46</v>
       </c>
       <c r="C43" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="D43" t="s">
-        <v>188</v>
+        <v>193</v>
       </c>
       <c r="E43" t="s">
-        <v>220</v>
+        <v>231</v>
       </c>
       <c r="F43" t="s">
-        <v>231</v>
+        <v>239</v>
       </c>
     </row>
     <row r="44" spans="1:6">
@@ -1963,16 +1987,16 @@
         <v>47</v>
       </c>
       <c r="C44" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="D44" t="s">
-        <v>189</v>
+        <v>194</v>
       </c>
       <c r="E44" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="F44" t="s">
-        <v>231</v>
+        <v>239</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -1983,16 +2007,16 @@
         <v>48</v>
       </c>
       <c r="C45" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="D45" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
       <c r="E45" t="s">
-        <v>219</v>
+        <v>231</v>
       </c>
       <c r="F45" t="s">
-        <v>231</v>
+        <v>243</v>
       </c>
     </row>
     <row r="46" spans="1:6">
@@ -2003,16 +2027,16 @@
         <v>49</v>
       </c>
       <c r="C46" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="D46" t="s">
-        <v>182</v>
+        <v>196</v>
       </c>
       <c r="E46" t="s">
-        <v>220</v>
+        <v>228</v>
       </c>
       <c r="F46" t="s">
-        <v>230</v>
+        <v>239</v>
       </c>
     </row>
     <row r="47" spans="1:6">
@@ -2023,16 +2047,16 @@
         <v>50</v>
       </c>
       <c r="C47" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="D47" t="s">
-        <v>191</v>
+        <v>197</v>
       </c>
       <c r="E47" t="s">
-        <v>225</v>
+        <v>231</v>
       </c>
       <c r="F47" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
     </row>
     <row r="48" spans="1:6">
@@ -2043,16 +2067,16 @@
         <v>51</v>
       </c>
       <c r="C48" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="D48" t="s">
-        <v>192</v>
+        <v>198</v>
       </c>
       <c r="E48" t="s">
-        <v>219</v>
+        <v>227</v>
       </c>
       <c r="F48" t="s">
-        <v>228</v>
+        <v>239</v>
       </c>
     </row>
     <row r="49" spans="1:6">
@@ -2063,16 +2087,16 @@
         <v>52</v>
       </c>
       <c r="C49" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="D49" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="E49" t="s">
-        <v>220</v>
+        <v>228</v>
       </c>
       <c r="F49" t="s">
-        <v>228</v>
+        <v>238</v>
       </c>
     </row>
     <row r="50" spans="1:6">
@@ -2083,16 +2107,16 @@
         <v>53</v>
       </c>
       <c r="C50" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="D50" t="s">
-        <v>194</v>
+        <v>199</v>
       </c>
       <c r="E50" t="s">
-        <v>219</v>
+        <v>233</v>
       </c>
       <c r="F50" t="s">
-        <v>231</v>
+        <v>244</v>
       </c>
     </row>
     <row r="51" spans="1:6">
@@ -2103,16 +2127,16 @@
         <v>54</v>
       </c>
       <c r="C51" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="D51" t="s">
-        <v>195</v>
+        <v>200</v>
       </c>
       <c r="E51" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="F51" t="s">
-        <v>231</v>
+        <v>236</v>
       </c>
     </row>
     <row r="52" spans="1:6">
@@ -2123,16 +2147,16 @@
         <v>55</v>
       </c>
       <c r="C52" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="D52" t="s">
-        <v>196</v>
+        <v>201</v>
       </c>
       <c r="E52" t="s">
-        <v>220</v>
+        <v>228</v>
       </c>
       <c r="F52" t="s">
-        <v>231</v>
+        <v>236</v>
       </c>
     </row>
     <row r="53" spans="1:6">
@@ -2143,16 +2167,16 @@
         <v>56</v>
       </c>
       <c r="C53" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="D53" t="s">
-        <v>197</v>
+        <v>202</v>
       </c>
       <c r="E53" t="s">
-        <v>219</v>
+        <v>227</v>
       </c>
       <c r="F53" t="s">
-        <v>231</v>
+        <v>239</v>
       </c>
     </row>
     <row r="54" spans="1:6">
@@ -2163,16 +2187,16 @@
         <v>57</v>
       </c>
       <c r="C54" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="D54" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
       <c r="E54" t="s">
-        <v>221</v>
+        <v>232</v>
       </c>
       <c r="F54" t="s">
-        <v>229</v>
+        <v>239</v>
       </c>
     </row>
     <row r="55" spans="1:6">
@@ -2183,16 +2207,16 @@
         <v>58</v>
       </c>
       <c r="C55" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="D55" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
       <c r="E55" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="F55" t="s">
-        <v>231</v>
+        <v>239</v>
       </c>
     </row>
     <row r="56" spans="1:6">
@@ -2203,16 +2227,16 @@
         <v>59</v>
       </c>
       <c r="C56" t="s">
-        <v>117</v>
+        <v>134</v>
       </c>
       <c r="D56" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
       <c r="E56" t="s">
-        <v>220</v>
+        <v>227</v>
       </c>
       <c r="F56" t="s">
-        <v>229</v>
+        <v>239</v>
       </c>
     </row>
     <row r="57" spans="1:6">
@@ -2223,16 +2247,16 @@
         <v>60</v>
       </c>
       <c r="C57" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="D57" t="s">
-        <v>201</v>
+        <v>206</v>
       </c>
       <c r="E57" t="s">
-        <v>220</v>
+        <v>229</v>
       </c>
       <c r="F57" t="s">
-        <v>231</v>
+        <v>237</v>
       </c>
     </row>
     <row r="58" spans="1:6">
@@ -2243,16 +2267,16 @@
         <v>61</v>
       </c>
       <c r="C58" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="D58" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="E58" t="s">
-        <v>220</v>
+        <v>231</v>
       </c>
       <c r="F58" t="s">
-        <v>231</v>
+        <v>239</v>
       </c>
     </row>
     <row r="59" spans="1:6">
@@ -2263,16 +2287,16 @@
         <v>62</v>
       </c>
       <c r="C59" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="D59" t="s">
-        <v>203</v>
+        <v>208</v>
       </c>
       <c r="E59" t="s">
-        <v>220</v>
+        <v>228</v>
       </c>
       <c r="F59" t="s">
-        <v>228</v>
+        <v>237</v>
       </c>
     </row>
     <row r="60" spans="1:6">
@@ -2283,16 +2307,16 @@
         <v>63</v>
       </c>
       <c r="C60" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="D60" t="s">
-        <v>204</v>
+        <v>209</v>
       </c>
       <c r="E60" t="s">
-        <v>219</v>
+        <v>228</v>
       </c>
       <c r="F60" t="s">
-        <v>229</v>
+        <v>239</v>
       </c>
     </row>
     <row r="61" spans="1:6">
@@ -2303,16 +2327,16 @@
         <v>64</v>
       </c>
       <c r="C61" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="D61" t="s">
-        <v>205</v>
+        <v>210</v>
       </c>
       <c r="E61" t="s">
-        <v>220</v>
+        <v>228</v>
       </c>
       <c r="F61" t="s">
-        <v>233</v>
+        <v>239</v>
       </c>
     </row>
     <row r="62" spans="1:6">
@@ -2323,16 +2347,16 @@
         <v>65</v>
       </c>
       <c r="C62" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="D62" t="s">
-        <v>206</v>
+        <v>211</v>
       </c>
       <c r="E62" t="s">
-        <v>219</v>
+        <v>228</v>
       </c>
       <c r="F62" t="s">
-        <v>231</v>
+        <v>236</v>
       </c>
     </row>
     <row r="63" spans="1:6">
@@ -2343,16 +2367,16 @@
         <v>66</v>
       </c>
       <c r="C63" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="D63" t="s">
-        <v>207</v>
+        <v>212</v>
       </c>
       <c r="E63" t="s">
-        <v>219</v>
+        <v>227</v>
       </c>
       <c r="F63" t="s">
-        <v>231</v>
+        <v>237</v>
       </c>
     </row>
     <row r="64" spans="1:6">
@@ -2363,16 +2387,16 @@
         <v>67</v>
       </c>
       <c r="C64" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="D64" t="s">
-        <v>208</v>
+        <v>213</v>
       </c>
       <c r="E64" t="s">
-        <v>220</v>
+        <v>228</v>
       </c>
       <c r="F64" t="s">
-        <v>231</v>
+        <v>241</v>
       </c>
     </row>
     <row r="65" spans="1:6">
@@ -2383,16 +2407,16 @@
         <v>68</v>
       </c>
       <c r="C65" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="D65" t="s">
-        <v>209</v>
+        <v>214</v>
       </c>
       <c r="E65" t="s">
-        <v>219</v>
+        <v>227</v>
       </c>
       <c r="F65" t="s">
-        <v>228</v>
+        <v>239</v>
       </c>
     </row>
     <row r="66" spans="1:6">
@@ -2403,16 +2427,16 @@
         <v>69</v>
       </c>
       <c r="C66" t="s">
-        <v>69</v>
+        <v>143</v>
       </c>
       <c r="D66" t="s">
-        <v>210</v>
+        <v>215</v>
       </c>
       <c r="E66" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="F66" t="s">
-        <v>231</v>
+        <v>239</v>
       </c>
     </row>
     <row r="67" spans="1:6">
@@ -2423,16 +2447,16 @@
         <v>70</v>
       </c>
       <c r="C67" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="D67" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="E67" t="s">
-        <v>221</v>
+        <v>228</v>
       </c>
       <c r="F67" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
     </row>
     <row r="68" spans="1:6">
@@ -2443,16 +2467,16 @@
         <v>71</v>
       </c>
       <c r="C68" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="D68" t="s">
-        <v>212</v>
+        <v>217</v>
       </c>
       <c r="E68" t="s">
-        <v>220</v>
+        <v>227</v>
       </c>
       <c r="F68" t="s">
-        <v>231</v>
+        <v>236</v>
       </c>
     </row>
     <row r="69" spans="1:6">
@@ -2463,16 +2487,16 @@
         <v>72</v>
       </c>
       <c r="C69" t="s">
-        <v>142</v>
+        <v>72</v>
       </c>
       <c r="D69" t="s">
-        <v>213</v>
+        <v>218</v>
       </c>
       <c r="E69" t="s">
-        <v>220</v>
+        <v>234</v>
       </c>
       <c r="F69" t="s">
-        <v>229</v>
+        <v>239</v>
       </c>
     </row>
     <row r="70" spans="1:6">
@@ -2483,16 +2507,16 @@
         <v>73</v>
       </c>
       <c r="C70" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="D70" t="s">
-        <v>214</v>
+        <v>219</v>
       </c>
       <c r="E70" t="s">
-        <v>220</v>
+        <v>229</v>
       </c>
       <c r="F70" t="s">
-        <v>231</v>
+        <v>245</v>
       </c>
     </row>
     <row r="71" spans="1:6">
@@ -2503,16 +2527,16 @@
         <v>74</v>
       </c>
       <c r="C71" t="s">
-        <v>98</v>
+        <v>147</v>
       </c>
       <c r="D71" t="s">
-        <v>215</v>
+        <v>220</v>
       </c>
       <c r="E71" t="s">
-        <v>219</v>
+        <v>228</v>
       </c>
       <c r="F71" t="s">
-        <v>228</v>
+        <v>239</v>
       </c>
     </row>
     <row r="72" spans="1:6">
@@ -2523,16 +2547,16 @@
         <v>75</v>
       </c>
       <c r="C72" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="D72" t="s">
-        <v>216</v>
+        <v>221</v>
       </c>
       <c r="E72" t="s">
-        <v>220</v>
+        <v>228</v>
       </c>
       <c r="F72" t="s">
-        <v>228</v>
+        <v>237</v>
       </c>
     </row>
     <row r="73" spans="1:6">
@@ -2543,16 +2567,16 @@
         <v>76</v>
       </c>
       <c r="C73" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="D73" t="s">
-        <v>217</v>
+        <v>222</v>
       </c>
       <c r="E73" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="F73" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
     </row>
     <row r="74" spans="1:6">
@@ -2563,16 +2587,76 @@
         <v>77</v>
       </c>
       <c r="C74" t="s">
-        <v>146</v>
+        <v>103</v>
       </c>
       <c r="D74" t="s">
-        <v>218</v>
+        <v>223</v>
       </c>
       <c r="E74" t="s">
         <v>227</v>
       </c>
       <c r="F74" t="s">
-        <v>228</v>
+        <v>236</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6">
+      <c r="A75" s="1">
+        <v>74</v>
+      </c>
+      <c r="B75" t="s">
+        <v>78</v>
+      </c>
+      <c r="C75" t="s">
+        <v>150</v>
+      </c>
+      <c r="D75" t="s">
+        <v>224</v>
+      </c>
+      <c r="E75" t="s">
+        <v>228</v>
+      </c>
+      <c r="F75" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6">
+      <c r="A76" s="1">
+        <v>75</v>
+      </c>
+      <c r="B76" t="s">
+        <v>79</v>
+      </c>
+      <c r="C76" t="s">
+        <v>151</v>
+      </c>
+      <c r="D76" t="s">
+        <v>225</v>
+      </c>
+      <c r="E76" t="s">
+        <v>233</v>
+      </c>
+      <c r="F76" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6">
+      <c r="A77" s="1">
+        <v>76</v>
+      </c>
+      <c r="B77" t="s">
+        <v>80</v>
+      </c>
+      <c r="C77" t="s">
+        <v>152</v>
+      </c>
+      <c r="D77" t="s">
+        <v>226</v>
+      </c>
+      <c r="E77" t="s">
+        <v>235</v>
+      </c>
+      <c r="F77" t="s">
+        <v>236</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated on 2018-12-17 at 18:15:47
</commit_message>
<xml_diff>
--- a/index.xlsx
+++ b/index.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="252">
   <si>
     <t>Song Title</t>
   </si>
@@ -79,6 +79,9 @@
     <t>Diamond Heart</t>
   </si>
   <si>
+    <t>Different World</t>
+  </si>
+  <si>
     <t>Don't Leave Me Alone</t>
   </si>
   <si>
@@ -139,6 +142,9 @@
     <t>Let Me Love You</t>
   </si>
   <si>
+    <t>Let You Love Me</t>
+  </si>
+  <si>
     <t>Like I Do</t>
   </si>
   <si>
@@ -364,6 +370,9 @@
     <t>Encore</t>
   </si>
   <si>
+    <t>Phoenix</t>
+  </si>
+  <si>
     <t>Like I Do (Single)</t>
   </si>
   <si>
@@ -520,6 +529,9 @@
     <t>Alan Walker, Sophia Somajo</t>
   </si>
   <si>
+    <t>Alan Walker, K-391, Sofia Carson, Corsak</t>
+  </si>
+  <si>
     <t>David Guetta, Anne-Marie</t>
   </si>
   <si>
@@ -580,6 +592,9 @@
     <t>DJ Snake, Justin Bieber</t>
   </si>
   <si>
+    <t>Rita Ora</t>
+  </si>
+  <si>
     <t>David Guetta, Martin Garrix, Brooks</t>
   </si>
   <si>
@@ -710,6 +725,9 @@
   </si>
   <si>
     <t>Rap, hiphop</t>
+  </si>
+  <si>
+    <t>Pop/Rock</t>
   </si>
   <si>
     <t>Soundtrack</t>
@@ -1109,7 +1127,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F77"/>
+  <dimension ref="A1:F79"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1147,16 +1165,16 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D2" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="E2" t="s">
-        <v>227</v>
+        <v>232</v>
       </c>
       <c r="F2" t="s">
-        <v>236</v>
+        <v>242</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -1167,16 +1185,16 @@
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D3" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="E3" t="s">
-        <v>227</v>
+        <v>232</v>
       </c>
       <c r="F3" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -1187,16 +1205,16 @@
         <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="D4" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="E4" t="s">
-        <v>227</v>
+        <v>232</v>
       </c>
       <c r="F4" t="s">
-        <v>236</v>
+        <v>242</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -1207,16 +1225,16 @@
         <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D5" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="E5" t="s">
-        <v>227</v>
+        <v>232</v>
       </c>
       <c r="F5" t="s">
-        <v>237</v>
+        <v>243</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -1227,16 +1245,16 @@
         <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="D6" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="E6" t="s">
-        <v>227</v>
+        <v>232</v>
       </c>
       <c r="F6" t="s">
-        <v>238</v>
+        <v>244</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -1247,16 +1265,16 @@
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D7" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="E7" t="s">
-        <v>228</v>
+        <v>233</v>
       </c>
       <c r="F7" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -1267,16 +1285,16 @@
         <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D8" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="E8" t="s">
-        <v>229</v>
+        <v>234</v>
       </c>
       <c r="F8" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -1287,16 +1305,16 @@
         <v>12</v>
       </c>
       <c r="C9" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="D9" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="E9" t="s">
-        <v>228</v>
+        <v>233</v>
       </c>
       <c r="F9" t="s">
-        <v>236</v>
+        <v>242</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -1307,16 +1325,16 @@
         <v>13</v>
       </c>
       <c r="C10" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="D10" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="E10" t="s">
-        <v>228</v>
+        <v>233</v>
       </c>
       <c r="F10" t="s">
-        <v>236</v>
+        <v>242</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -1327,16 +1345,16 @@
         <v>14</v>
       </c>
       <c r="C11" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D11" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="E11" t="s">
-        <v>228</v>
+        <v>233</v>
       </c>
       <c r="F11" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -1347,16 +1365,16 @@
         <v>15</v>
       </c>
       <c r="C12" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="D12" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="E12" t="s">
-        <v>227</v>
+        <v>232</v>
       </c>
       <c r="F12" t="s">
-        <v>236</v>
+        <v>242</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -1367,16 +1385,16 @@
         <v>16</v>
       </c>
       <c r="C13" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="D13" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="E13" t="s">
-        <v>228</v>
+        <v>233</v>
       </c>
       <c r="F13" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -1387,16 +1405,16 @@
         <v>17</v>
       </c>
       <c r="C14" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D14" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="E14" t="s">
-        <v>230</v>
+        <v>235</v>
       </c>
       <c r="F14" t="s">
-        <v>240</v>
+        <v>246</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -1407,16 +1425,16 @@
         <v>18</v>
       </c>
       <c r="C15" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D15" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="E15" t="s">
-        <v>227</v>
+        <v>232</v>
       </c>
       <c r="F15" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -1427,16 +1445,16 @@
         <v>19</v>
       </c>
       <c r="C16" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D16" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="E16" t="s">
-        <v>228</v>
+        <v>233</v>
       </c>
       <c r="F16" t="s">
-        <v>236</v>
+        <v>242</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -1447,16 +1465,16 @@
         <v>20</v>
       </c>
       <c r="C17" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="D17" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="E17" t="s">
-        <v>227</v>
+        <v>232</v>
       </c>
       <c r="F17" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -1467,16 +1485,16 @@
         <v>21</v>
       </c>
       <c r="C18" t="s">
-        <v>97</v>
+        <v>21</v>
       </c>
       <c r="D18" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="E18" t="s">
-        <v>227</v>
+        <v>232</v>
       </c>
       <c r="F18" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -1487,16 +1505,16 @@
         <v>22</v>
       </c>
       <c r="C19" t="s">
-        <v>22</v>
+        <v>99</v>
       </c>
       <c r="D19" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="E19" t="s">
-        <v>227</v>
+        <v>232</v>
       </c>
       <c r="F19" t="s">
-        <v>237</v>
+        <v>245</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -1507,16 +1525,16 @@
         <v>23</v>
       </c>
       <c r="C20" t="s">
-        <v>98</v>
+        <v>23</v>
       </c>
       <c r="D20" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="E20" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="F20" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -1527,16 +1545,16 @@
         <v>24</v>
       </c>
       <c r="C21" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D21" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="E21" t="s">
-        <v>228</v>
+        <v>233</v>
       </c>
       <c r="F21" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -1547,16 +1565,16 @@
         <v>25</v>
       </c>
       <c r="C22" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D22" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="E22" t="s">
-        <v>227</v>
+        <v>233</v>
       </c>
       <c r="F22" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -1567,16 +1585,16 @@
         <v>26</v>
       </c>
       <c r="C23" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D23" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="E23" t="s">
-        <v>227</v>
+        <v>232</v>
       </c>
       <c r="F23" t="s">
-        <v>239</v>
+        <v>247</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -1587,16 +1605,16 @@
         <v>27</v>
       </c>
       <c r="C24" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D24" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="E24" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="F24" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -1607,16 +1625,16 @@
         <v>28</v>
       </c>
       <c r="C25" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D25" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="E25" t="s">
-        <v>227</v>
+        <v>233</v>
       </c>
       <c r="F25" t="s">
-        <v>236</v>
+        <v>245</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -1627,16 +1645,16 @@
         <v>29</v>
       </c>
       <c r="C26" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D26" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="E26" t="s">
-        <v>227</v>
+        <v>232</v>
       </c>
       <c r="F26" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -1647,16 +1665,16 @@
         <v>30</v>
       </c>
       <c r="C27" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D27" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="E27" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="F27" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -1667,16 +1685,16 @@
         <v>31</v>
       </c>
       <c r="C28" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D28" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="E28" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="F28" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -1687,16 +1705,16 @@
         <v>32</v>
       </c>
       <c r="C29" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D29" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="E29" t="s">
-        <v>227</v>
+        <v>236</v>
       </c>
       <c r="F29" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -1707,16 +1725,16 @@
         <v>33</v>
       </c>
       <c r="C30" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D30" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="E30" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="F30" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -1727,16 +1745,16 @@
         <v>34</v>
       </c>
       <c r="C31" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D31" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="E31" t="s">
-        <v>228</v>
+        <v>233</v>
       </c>
       <c r="F31" t="s">
-        <v>236</v>
+        <v>245</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -1747,16 +1765,16 @@
         <v>35</v>
       </c>
       <c r="C32" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D32" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="E32" t="s">
-        <v>227</v>
+        <v>233</v>
       </c>
       <c r="F32" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -1767,16 +1785,16 @@
         <v>36</v>
       </c>
       <c r="C33" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D33" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="E33" t="s">
-        <v>227</v>
+        <v>232</v>
       </c>
       <c r="F33" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -1787,16 +1805,16 @@
         <v>37</v>
       </c>
       <c r="C34" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D34" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="E34" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="F34" t="s">
-        <v>123</v>
+        <v>245</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -1807,16 +1825,16 @@
         <v>38</v>
       </c>
       <c r="C35" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D35" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="E35" t="s">
-        <v>227</v>
+        <v>233</v>
       </c>
       <c r="F35" t="s">
-        <v>236</v>
+        <v>126</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -1827,16 +1845,16 @@
         <v>39</v>
       </c>
       <c r="C36" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D36" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="E36" t="s">
-        <v>227</v>
+        <v>232</v>
       </c>
       <c r="F36" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -1847,16 +1865,16 @@
         <v>40</v>
       </c>
       <c r="C37" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D37" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="E37" t="s">
-        <v>227</v>
+        <v>232</v>
       </c>
       <c r="F37" t="s">
-        <v>237</v>
+        <v>245</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -1867,16 +1885,16 @@
         <v>41</v>
       </c>
       <c r="C38" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D38" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="E38" t="s">
-        <v>227</v>
+        <v>232</v>
       </c>
       <c r="F38" t="s">
-        <v>239</v>
+        <v>243</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -1887,16 +1905,16 @@
         <v>42</v>
       </c>
       <c r="C39" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D39" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="E39" t="s">
-        <v>232</v>
+        <v>237</v>
       </c>
       <c r="F39" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -1907,16 +1925,16 @@
         <v>43</v>
       </c>
       <c r="C40" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D40" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="E40" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="F40" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -1927,16 +1945,16 @@
         <v>44</v>
       </c>
       <c r="C41" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D41" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="E41" t="s">
-        <v>227</v>
+        <v>238</v>
       </c>
       <c r="F41" t="s">
-        <v>242</v>
+        <v>247</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -1947,16 +1965,16 @@
         <v>45</v>
       </c>
       <c r="C42" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D42" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="E42" t="s">
-        <v>227</v>
+        <v>233</v>
       </c>
       <c r="F42" t="s">
-        <v>239</v>
+        <v>247</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -1967,16 +1985,16 @@
         <v>46</v>
       </c>
       <c r="C43" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D43" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="E43" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="F43" t="s">
-        <v>239</v>
+        <v>248</v>
       </c>
     </row>
     <row r="44" spans="1:6">
@@ -1987,16 +2005,16 @@
         <v>47</v>
       </c>
       <c r="C44" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D44" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="E44" t="s">
-        <v>227</v>
+        <v>232</v>
       </c>
       <c r="F44" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -2007,16 +2025,16 @@
         <v>48</v>
       </c>
       <c r="C45" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D45" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="E45" t="s">
-        <v>231</v>
+        <v>236</v>
       </c>
       <c r="F45" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
     </row>
     <row r="46" spans="1:6">
@@ -2027,16 +2045,16 @@
         <v>49</v>
       </c>
       <c r="C46" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D46" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="E46" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="F46" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
     </row>
     <row r="47" spans="1:6">
@@ -2047,16 +2065,16 @@
         <v>50</v>
       </c>
       <c r="C47" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D47" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="E47" t="s">
-        <v>231</v>
+        <v>236</v>
       </c>
       <c r="F47" t="s">
-        <v>239</v>
+        <v>249</v>
       </c>
     </row>
     <row r="48" spans="1:6">
@@ -2067,16 +2085,16 @@
         <v>51</v>
       </c>
       <c r="C48" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D48" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="E48" t="s">
-        <v>227</v>
+        <v>233</v>
       </c>
       <c r="F48" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
     </row>
     <row r="49" spans="1:6">
@@ -2087,16 +2105,16 @@
         <v>52</v>
       </c>
       <c r="C49" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D49" t="s">
-        <v>190</v>
+        <v>202</v>
       </c>
       <c r="E49" t="s">
-        <v>228</v>
+        <v>236</v>
       </c>
       <c r="F49" t="s">
-        <v>238</v>
+        <v>245</v>
       </c>
     </row>
     <row r="50" spans="1:6">
@@ -2107,16 +2125,16 @@
         <v>53</v>
       </c>
       <c r="C50" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D50" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="E50" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F50" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="51" spans="1:6">
@@ -2127,16 +2145,16 @@
         <v>54</v>
       </c>
       <c r="C51" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D51" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="E51" t="s">
-        <v>227</v>
+        <v>233</v>
       </c>
       <c r="F51" t="s">
-        <v>236</v>
+        <v>244</v>
       </c>
     </row>
     <row r="52" spans="1:6">
@@ -2147,16 +2165,16 @@
         <v>55</v>
       </c>
       <c r="C52" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D52" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="E52" t="s">
-        <v>228</v>
+        <v>239</v>
       </c>
       <c r="F52" t="s">
-        <v>236</v>
+        <v>250</v>
       </c>
     </row>
     <row r="53" spans="1:6">
@@ -2167,16 +2185,16 @@
         <v>56</v>
       </c>
       <c r="C53" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D53" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="E53" t="s">
-        <v>227</v>
+        <v>232</v>
       </c>
       <c r="F53" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
     </row>
     <row r="54" spans="1:6">
@@ -2187,16 +2205,16 @@
         <v>57</v>
       </c>
       <c r="C54" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D54" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="E54" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="F54" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
     </row>
     <row r="55" spans="1:6">
@@ -2207,16 +2225,16 @@
         <v>58</v>
       </c>
       <c r="C55" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D55" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="E55" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="F55" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
     </row>
     <row r="56" spans="1:6">
@@ -2227,16 +2245,16 @@
         <v>59</v>
       </c>
       <c r="C56" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D56" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="E56" t="s">
-        <v>227</v>
+        <v>238</v>
       </c>
       <c r="F56" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
     </row>
     <row r="57" spans="1:6">
@@ -2247,16 +2265,16 @@
         <v>60</v>
       </c>
       <c r="C57" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D57" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="E57" t="s">
-        <v>229</v>
+        <v>233</v>
       </c>
       <c r="F57" t="s">
-        <v>237</v>
+        <v>245</v>
       </c>
     </row>
     <row r="58" spans="1:6">
@@ -2267,16 +2285,16 @@
         <v>61</v>
       </c>
       <c r="C58" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D58" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="E58" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="F58" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
     </row>
     <row r="59" spans="1:6">
@@ -2287,16 +2305,16 @@
         <v>62</v>
       </c>
       <c r="C59" t="s">
-        <v>123</v>
+        <v>138</v>
       </c>
       <c r="D59" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="E59" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
       <c r="F59" t="s">
-        <v>237</v>
+        <v>243</v>
       </c>
     </row>
     <row r="60" spans="1:6">
@@ -2307,16 +2325,16 @@
         <v>63</v>
       </c>
       <c r="C60" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="D60" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="E60" t="s">
-        <v>228</v>
+        <v>236</v>
       </c>
       <c r="F60" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
     </row>
     <row r="61" spans="1:6">
@@ -2327,16 +2345,16 @@
         <v>64</v>
       </c>
       <c r="C61" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="D61" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="E61" t="s">
-        <v>228</v>
+        <v>233</v>
       </c>
       <c r="F61" t="s">
-        <v>239</v>
+        <v>243</v>
       </c>
     </row>
     <row r="62" spans="1:6">
@@ -2347,16 +2365,16 @@
         <v>65</v>
       </c>
       <c r="C62" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D62" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="E62" t="s">
-        <v>228</v>
+        <v>233</v>
       </c>
       <c r="F62" t="s">
-        <v>236</v>
+        <v>245</v>
       </c>
     </row>
     <row r="63" spans="1:6">
@@ -2367,16 +2385,16 @@
         <v>66</v>
       </c>
       <c r="C63" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D63" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="E63" t="s">
-        <v>227</v>
+        <v>233</v>
       </c>
       <c r="F63" t="s">
-        <v>237</v>
+        <v>245</v>
       </c>
     </row>
     <row r="64" spans="1:6">
@@ -2387,16 +2405,16 @@
         <v>67</v>
       </c>
       <c r="C64" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D64" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="E64" t="s">
-        <v>228</v>
+        <v>233</v>
       </c>
       <c r="F64" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="65" spans="1:6">
@@ -2407,16 +2425,16 @@
         <v>68</v>
       </c>
       <c r="C65" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D65" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="E65" t="s">
-        <v>227</v>
+        <v>232</v>
       </c>
       <c r="F65" t="s">
-        <v>239</v>
+        <v>243</v>
       </c>
     </row>
     <row r="66" spans="1:6">
@@ -2427,16 +2445,16 @@
         <v>69</v>
       </c>
       <c r="C66" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D66" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="E66" t="s">
-        <v>227</v>
+        <v>233</v>
       </c>
       <c r="F66" t="s">
-        <v>239</v>
+        <v>247</v>
       </c>
     </row>
     <row r="67" spans="1:6">
@@ -2447,16 +2465,16 @@
         <v>70</v>
       </c>
       <c r="C67" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D67" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="E67" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="F67" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
     </row>
     <row r="68" spans="1:6">
@@ -2467,16 +2485,16 @@
         <v>71</v>
       </c>
       <c r="C68" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D68" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="E68" t="s">
-        <v>227</v>
+        <v>232</v>
       </c>
       <c r="F68" t="s">
-        <v>236</v>
+        <v>245</v>
       </c>
     </row>
     <row r="69" spans="1:6">
@@ -2487,16 +2505,16 @@
         <v>72</v>
       </c>
       <c r="C69" t="s">
-        <v>72</v>
+        <v>147</v>
       </c>
       <c r="D69" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="E69" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="F69" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
     </row>
     <row r="70" spans="1:6">
@@ -2507,16 +2525,16 @@
         <v>73</v>
       </c>
       <c r="C70" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="D70" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="E70" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="F70" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="71" spans="1:6">
@@ -2527,16 +2545,16 @@
         <v>74</v>
       </c>
       <c r="C71" t="s">
-        <v>147</v>
+        <v>74</v>
       </c>
       <c r="D71" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="E71" t="s">
-        <v>228</v>
+        <v>240</v>
       </c>
       <c r="F71" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
     </row>
     <row r="72" spans="1:6">
@@ -2547,16 +2565,16 @@
         <v>75</v>
       </c>
       <c r="C72" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D72" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="E72" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
       <c r="F72" t="s">
-        <v>237</v>
+        <v>251</v>
       </c>
     </row>
     <row r="73" spans="1:6">
@@ -2567,16 +2585,16 @@
         <v>76</v>
       </c>
       <c r="C73" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D73" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="E73" t="s">
-        <v>228</v>
+        <v>233</v>
       </c>
       <c r="F73" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
     </row>
     <row r="74" spans="1:6">
@@ -2587,16 +2605,16 @@
         <v>77</v>
       </c>
       <c r="C74" t="s">
-        <v>103</v>
+        <v>151</v>
       </c>
       <c r="D74" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="E74" t="s">
-        <v>227</v>
+        <v>233</v>
       </c>
       <c r="F74" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
     </row>
     <row r="75" spans="1:6">
@@ -2607,16 +2625,16 @@
         <v>78</v>
       </c>
       <c r="C75" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="D75" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="E75" t="s">
-        <v>228</v>
+        <v>233</v>
       </c>
       <c r="F75" t="s">
-        <v>236</v>
+        <v>245</v>
       </c>
     </row>
     <row r="76" spans="1:6">
@@ -2627,16 +2645,16 @@
         <v>79</v>
       </c>
       <c r="C76" t="s">
-        <v>151</v>
+        <v>105</v>
       </c>
       <c r="D76" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="E76" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F76" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="77" spans="1:6">
@@ -2647,16 +2665,56 @@
         <v>80</v>
       </c>
       <c r="C77" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D77" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="E77" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="F77" t="s">
-        <v>236</v>
+        <v>242</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6">
+      <c r="A78" s="1">
+        <v>77</v>
+      </c>
+      <c r="B78" t="s">
+        <v>81</v>
+      </c>
+      <c r="C78" t="s">
+        <v>154</v>
+      </c>
+      <c r="D78" t="s">
+        <v>230</v>
+      </c>
+      <c r="E78" t="s">
+        <v>239</v>
+      </c>
+      <c r="F78" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6">
+      <c r="A79" s="1">
+        <v>78</v>
+      </c>
+      <c r="B79" t="s">
+        <v>82</v>
+      </c>
+      <c r="C79" t="s">
+        <v>155</v>
+      </c>
+      <c r="D79" t="s">
+        <v>231</v>
+      </c>
+      <c r="E79" t="s">
+        <v>241</v>
+      </c>
+      <c r="F79" t="s">
+        <v>242</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated on 2018-12-22 at 14:25:18
</commit_message>
<xml_diff>
--- a/index.xlsx
+++ b/index.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="266">
   <si>
     <t>Song Title</t>
   </si>
@@ -61,6 +61,9 @@
     <t>Blank Space</t>
   </si>
   <si>
+    <t>Promises</t>
+  </si>
+  <si>
     <t>Complicated</t>
   </si>
   <si>
@@ -76,6 +79,9 @@
     <t>Darts In The Dark</t>
   </si>
   <si>
+    <t>Dangerous (feat. Sam Martin)</t>
+  </si>
+  <si>
     <t>Diamond Heart</t>
   </si>
   <si>
@@ -91,6 +97,9 @@
     <t>Dusk Till Dawn</t>
   </si>
   <si>
+    <t>In My Mind</t>
+  </si>
+  <si>
     <t>Eastside</t>
   </si>
   <si>
@@ -109,6 +118,9 @@
     <t>Friends</t>
   </si>
   <si>
+    <t>Shotgun</t>
+  </si>
+  <si>
     <t>Girls Like You</t>
   </si>
   <si>
@@ -238,6 +250,9 @@
     <t>Tired</t>
   </si>
   <si>
+    <t>Leave a Light On</t>
+  </si>
+  <si>
     <t>Trampoline</t>
   </si>
   <si>
@@ -310,6 +325,9 @@
     <t>Darts In The Dark (Single)</t>
   </si>
   <si>
+    <t>Listen Again</t>
+  </si>
+  <si>
     <t>Diamond Heart (Single)</t>
   </si>
   <si>
@@ -337,6 +355,9 @@
     <t>Friends (Single)</t>
   </si>
   <si>
+    <t>Staying at Tamara's</t>
+  </si>
+  <si>
     <t>Girls Like You (Single)</t>
   </si>
   <si>
@@ -511,6 +532,9 @@
     <t>Taylor Swift</t>
   </si>
   <si>
+    <t>Calvin Harris;Sam Smith</t>
+  </si>
+  <si>
     <t>Dimitri Vegas &amp; Like Mike, David Guetta, Kiiara</t>
   </si>
   <si>
@@ -526,6 +550,9 @@
     <t>MAGIC!</t>
   </si>
   <si>
+    <t>David Guetta;Sam Martin</t>
+  </si>
+  <si>
     <t>Alan Walker, Sophia Somajo</t>
   </si>
   <si>
@@ -541,6 +568,9 @@
     <t>ZAYN, Sia</t>
   </si>
   <si>
+    <t>Dynoro;Gigi D'Agostino</t>
+  </si>
+  <si>
     <t>Benny Blanco, Halsey, Khalid</t>
   </si>
   <si>
@@ -559,6 +589,9 @@
     <t>Marshmello, Anne-Marie</t>
   </si>
   <si>
+    <t>George Ezra</t>
+  </si>
+  <si>
     <t>Maroon 5, Cardi B</t>
   </si>
   <si>
@@ -685,6 +718,9 @@
     <t>Alan Walker, Gavin James</t>
   </si>
   <si>
+    <t>Tom Walker</t>
+  </si>
+  <si>
     <t>SHAED</t>
   </si>
   <si>
@@ -724,6 +760,9 @@
     <t>Pop, rock...</t>
   </si>
   <si>
+    <t>Singer &amp; Songwriter</t>
+  </si>
+  <si>
     <t>Rap, hiphop</t>
   </si>
   <si>
@@ -734,6 +773,9 @@
   </si>
   <si>
     <t>Rock</t>
+  </si>
+  <si>
+    <t>Alternative;Indie Pop;Indie Rock;Singer &amp; Songwriter</t>
   </si>
   <si>
     <t>Alternative</t>
@@ -1127,7 +1169,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F79"/>
+  <dimension ref="A1:F84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1136,7 +1178,7 @@
     <col min="1" max="1" width="41.7109375" customWidth="1"/>
     <col min="2" max="2" width="58.7109375" customWidth="1"/>
     <col min="3" max="3" width="51.7109375" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" customWidth="1"/>
+    <col min="4" max="4" width="53.7109375" customWidth="1"/>
     <col min="5" max="5" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1165,16 +1207,16 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="D2" t="s">
-        <v>156</v>
+        <v>163</v>
       </c>
       <c r="E2" t="s">
-        <v>232</v>
+        <v>244</v>
       </c>
       <c r="F2" t="s">
-        <v>242</v>
+        <v>256</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -1185,16 +1227,16 @@
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="D3" t="s">
-        <v>126</v>
+        <v>133</v>
       </c>
       <c r="E3" t="s">
-        <v>232</v>
+        <v>244</v>
       </c>
       <c r="F3" t="s">
-        <v>126</v>
+        <v>133</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -1205,16 +1247,16 @@
         <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="D4" t="s">
-        <v>157</v>
+        <v>164</v>
       </c>
       <c r="E4" t="s">
-        <v>232</v>
+        <v>244</v>
       </c>
       <c r="F4" t="s">
-        <v>242</v>
+        <v>256</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -1225,16 +1267,16 @@
         <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="D5" t="s">
-        <v>158</v>
+        <v>165</v>
       </c>
       <c r="E5" t="s">
-        <v>232</v>
+        <v>244</v>
       </c>
       <c r="F5" t="s">
-        <v>243</v>
+        <v>257</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -1245,16 +1287,16 @@
         <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="D6" t="s">
-        <v>159</v>
+        <v>166</v>
       </c>
       <c r="E6" t="s">
-        <v>232</v>
+        <v>244</v>
       </c>
       <c r="F6" t="s">
-        <v>244</v>
+        <v>258</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -1265,16 +1307,16 @@
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="D7" t="s">
-        <v>160</v>
+        <v>167</v>
       </c>
       <c r="E7" t="s">
-        <v>233</v>
+        <v>245</v>
       </c>
       <c r="F7" t="s">
-        <v>245</v>
+        <v>259</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -1285,16 +1327,16 @@
         <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="D8" t="s">
-        <v>161</v>
+        <v>168</v>
       </c>
       <c r="E8" t="s">
-        <v>234</v>
+        <v>246</v>
       </c>
       <c r="F8" t="s">
-        <v>245</v>
+        <v>259</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -1305,16 +1347,16 @@
         <v>12</v>
       </c>
       <c r="C9" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="D9" t="s">
-        <v>162</v>
+        <v>169</v>
       </c>
       <c r="E9" t="s">
-        <v>233</v>
+        <v>245</v>
       </c>
       <c r="F9" t="s">
-        <v>242</v>
+        <v>256</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -1325,16 +1367,16 @@
         <v>13</v>
       </c>
       <c r="C10" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="D10" t="s">
-        <v>163</v>
+        <v>170</v>
       </c>
       <c r="E10" t="s">
-        <v>233</v>
+        <v>245</v>
       </c>
       <c r="F10" t="s">
-        <v>242</v>
+        <v>256</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -1345,16 +1387,16 @@
         <v>14</v>
       </c>
       <c r="C11" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="D11" t="s">
-        <v>164</v>
+        <v>171</v>
       </c>
       <c r="E11" t="s">
-        <v>233</v>
+        <v>245</v>
       </c>
       <c r="F11" t="s">
-        <v>126</v>
+        <v>133</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -1365,16 +1407,16 @@
         <v>15</v>
       </c>
       <c r="C12" t="s">
-        <v>93</v>
+        <v>15</v>
       </c>
       <c r="D12" t="s">
-        <v>165</v>
+        <v>172</v>
       </c>
       <c r="E12" t="s">
-        <v>232</v>
+        <v>246</v>
       </c>
       <c r="F12" t="s">
-        <v>242</v>
+        <v>259</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -1385,16 +1427,16 @@
         <v>16</v>
       </c>
       <c r="C13" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="D13" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
       <c r="E13" t="s">
-        <v>233</v>
+        <v>244</v>
       </c>
       <c r="F13" t="s">
-        <v>245</v>
+        <v>256</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -1405,16 +1447,16 @@
         <v>17</v>
       </c>
       <c r="C14" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="D14" t="s">
-        <v>167</v>
+        <v>174</v>
       </c>
       <c r="E14" t="s">
-        <v>235</v>
+        <v>245</v>
       </c>
       <c r="F14" t="s">
-        <v>246</v>
+        <v>259</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -1425,16 +1467,16 @@
         <v>18</v>
       </c>
       <c r="C15" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="D15" t="s">
-        <v>168</v>
+        <v>175</v>
       </c>
       <c r="E15" t="s">
-        <v>232</v>
+        <v>247</v>
       </c>
       <c r="F15" t="s">
-        <v>245</v>
+        <v>260</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -1445,16 +1487,16 @@
         <v>19</v>
       </c>
       <c r="C16" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="D16" t="s">
-        <v>169</v>
+        <v>176</v>
       </c>
       <c r="E16" t="s">
-        <v>233</v>
+        <v>244</v>
       </c>
       <c r="F16" t="s">
-        <v>242</v>
+        <v>259</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -1465,16 +1507,16 @@
         <v>20</v>
       </c>
       <c r="C17" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="D17" t="s">
-        <v>170</v>
+        <v>177</v>
       </c>
       <c r="E17" t="s">
-        <v>232</v>
+        <v>245</v>
       </c>
       <c r="F17" t="s">
-        <v>245</v>
+        <v>256</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -1485,16 +1527,16 @@
         <v>21</v>
       </c>
       <c r="C18" t="s">
-        <v>21</v>
+        <v>103</v>
       </c>
       <c r="D18" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="E18" t="s">
-        <v>232</v>
+        <v>246</v>
       </c>
       <c r="F18" t="s">
-        <v>245</v>
+        <v>261</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -1505,16 +1547,16 @@
         <v>22</v>
       </c>
       <c r="C19" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="D19" t="s">
-        <v>172</v>
+        <v>179</v>
       </c>
       <c r="E19" t="s">
-        <v>232</v>
+        <v>244</v>
       </c>
       <c r="F19" t="s">
-        <v>245</v>
+        <v>259</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -1528,13 +1570,13 @@
         <v>23</v>
       </c>
       <c r="D20" t="s">
-        <v>173</v>
+        <v>180</v>
       </c>
       <c r="E20" t="s">
-        <v>232</v>
+        <v>244</v>
       </c>
       <c r="F20" t="s">
-        <v>243</v>
+        <v>259</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -1545,16 +1587,16 @@
         <v>24</v>
       </c>
       <c r="C21" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="D21" t="s">
-        <v>174</v>
+        <v>181</v>
       </c>
       <c r="E21" t="s">
-        <v>233</v>
+        <v>244</v>
       </c>
       <c r="F21" t="s">
-        <v>242</v>
+        <v>259</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -1565,16 +1607,16 @@
         <v>25</v>
       </c>
       <c r="C22" t="s">
-        <v>101</v>
+        <v>25</v>
       </c>
       <c r="D22" t="s">
-        <v>175</v>
+        <v>182</v>
       </c>
       <c r="E22" t="s">
-        <v>233</v>
+        <v>244</v>
       </c>
       <c r="F22" t="s">
-        <v>245</v>
+        <v>257</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -1585,16 +1627,16 @@
         <v>26</v>
       </c>
       <c r="C23" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="D23" t="s">
-        <v>176</v>
+        <v>183</v>
       </c>
       <c r="E23" t="s">
-        <v>232</v>
+        <v>245</v>
       </c>
       <c r="F23" t="s">
-        <v>247</v>
+        <v>256</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -1605,16 +1647,16 @@
         <v>27</v>
       </c>
       <c r="C24" t="s">
-        <v>103</v>
+        <v>27</v>
       </c>
       <c r="D24" t="s">
-        <v>177</v>
+        <v>184</v>
       </c>
       <c r="E24" t="s">
-        <v>232</v>
+        <v>246</v>
       </c>
       <c r="F24" t="s">
-        <v>245</v>
+        <v>259</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -1625,16 +1667,16 @@
         <v>28</v>
       </c>
       <c r="C25" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="D25" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
       <c r="E25" t="s">
-        <v>233</v>
+        <v>245</v>
       </c>
       <c r="F25" t="s">
-        <v>245</v>
+        <v>259</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -1645,16 +1687,16 @@
         <v>29</v>
       </c>
       <c r="C26" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="D26" t="s">
-        <v>179</v>
+        <v>186</v>
       </c>
       <c r="E26" t="s">
-        <v>232</v>
+        <v>244</v>
       </c>
       <c r="F26" t="s">
-        <v>242</v>
+        <v>261</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -1665,16 +1707,16 @@
         <v>30</v>
       </c>
       <c r="C27" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="D27" t="s">
-        <v>180</v>
+        <v>187</v>
       </c>
       <c r="E27" t="s">
-        <v>232</v>
+        <v>244</v>
       </c>
       <c r="F27" t="s">
-        <v>245</v>
+        <v>259</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -1685,16 +1727,16 @@
         <v>31</v>
       </c>
       <c r="C28" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="D28" t="s">
-        <v>181</v>
+        <v>188</v>
       </c>
       <c r="E28" t="s">
-        <v>233</v>
+        <v>245</v>
       </c>
       <c r="F28" t="s">
-        <v>245</v>
+        <v>259</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -1705,16 +1747,16 @@
         <v>32</v>
       </c>
       <c r="C29" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="D29" t="s">
-        <v>182</v>
+        <v>189</v>
       </c>
       <c r="E29" t="s">
-        <v>236</v>
+        <v>244</v>
       </c>
       <c r="F29" t="s">
-        <v>245</v>
+        <v>256</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -1725,16 +1767,16 @@
         <v>33</v>
       </c>
       <c r="C30" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="D30" t="s">
-        <v>183</v>
+        <v>190</v>
       </c>
       <c r="E30" t="s">
-        <v>232</v>
+        <v>244</v>
       </c>
       <c r="F30" t="s">
-        <v>245</v>
+        <v>259</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -1745,16 +1787,16 @@
         <v>34</v>
       </c>
       <c r="C31" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="D31" t="s">
-        <v>184</v>
+        <v>191</v>
       </c>
       <c r="E31" t="s">
-        <v>233</v>
+        <v>248</v>
       </c>
       <c r="F31" t="s">
-        <v>245</v>
+        <v>259</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -1765,16 +1807,16 @@
         <v>35</v>
       </c>
       <c r="C32" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="D32" t="s">
-        <v>185</v>
+        <v>192</v>
       </c>
       <c r="E32" t="s">
-        <v>233</v>
+        <v>245</v>
       </c>
       <c r="F32" t="s">
-        <v>242</v>
+        <v>259</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -1785,16 +1827,16 @@
         <v>36</v>
       </c>
       <c r="C33" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="D33" t="s">
-        <v>186</v>
+        <v>193</v>
       </c>
       <c r="E33" t="s">
-        <v>232</v>
+        <v>249</v>
       </c>
       <c r="F33" t="s">
-        <v>245</v>
+        <v>259</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -1805,16 +1847,16 @@
         <v>37</v>
       </c>
       <c r="C34" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="D34" t="s">
-        <v>187</v>
+        <v>194</v>
       </c>
       <c r="E34" t="s">
-        <v>232</v>
+        <v>244</v>
       </c>
       <c r="F34" t="s">
-        <v>245</v>
+        <v>259</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -1825,16 +1867,16 @@
         <v>38</v>
       </c>
       <c r="C35" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="D35" t="s">
-        <v>188</v>
+        <v>195</v>
       </c>
       <c r="E35" t="s">
-        <v>233</v>
+        <v>245</v>
       </c>
       <c r="F35" t="s">
-        <v>126</v>
+        <v>259</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -1845,16 +1887,16 @@
         <v>39</v>
       </c>
       <c r="C36" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="D36" t="s">
-        <v>189</v>
+        <v>196</v>
       </c>
       <c r="E36" t="s">
-        <v>232</v>
+        <v>245</v>
       </c>
       <c r="F36" t="s">
-        <v>242</v>
+        <v>256</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -1865,16 +1907,16 @@
         <v>40</v>
       </c>
       <c r="C37" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="D37" t="s">
-        <v>190</v>
+        <v>197</v>
       </c>
       <c r="E37" t="s">
-        <v>232</v>
+        <v>244</v>
       </c>
       <c r="F37" t="s">
-        <v>245</v>
+        <v>259</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -1885,16 +1927,16 @@
         <v>41</v>
       </c>
       <c r="C38" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="D38" t="s">
-        <v>191</v>
+        <v>198</v>
       </c>
       <c r="E38" t="s">
-        <v>232</v>
+        <v>244</v>
       </c>
       <c r="F38" t="s">
-        <v>243</v>
+        <v>259</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -1905,16 +1947,16 @@
         <v>42</v>
       </c>
       <c r="C39" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="D39" t="s">
-        <v>192</v>
+        <v>199</v>
       </c>
       <c r="E39" t="s">
-        <v>237</v>
+        <v>245</v>
       </c>
       <c r="F39" t="s">
-        <v>245</v>
+        <v>133</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -1925,16 +1967,16 @@
         <v>43</v>
       </c>
       <c r="C40" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="D40" t="s">
-        <v>193</v>
+        <v>200</v>
       </c>
       <c r="E40" t="s">
-        <v>232</v>
+        <v>244</v>
       </c>
       <c r="F40" t="s">
-        <v>245</v>
+        <v>256</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -1945,16 +1987,16 @@
         <v>44</v>
       </c>
       <c r="C41" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="D41" t="s">
-        <v>194</v>
+        <v>201</v>
       </c>
       <c r="E41" t="s">
-        <v>238</v>
+        <v>244</v>
       </c>
       <c r="F41" t="s">
-        <v>247</v>
+        <v>259</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -1965,16 +2007,16 @@
         <v>45</v>
       </c>
       <c r="C42" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="D42" t="s">
-        <v>195</v>
+        <v>202</v>
       </c>
       <c r="E42" t="s">
-        <v>233</v>
+        <v>244</v>
       </c>
       <c r="F42" t="s">
-        <v>247</v>
+        <v>257</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -1985,16 +2027,16 @@
         <v>46</v>
       </c>
       <c r="C43" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="D43" t="s">
-        <v>196</v>
+        <v>203</v>
       </c>
       <c r="E43" t="s">
-        <v>232</v>
+        <v>250</v>
       </c>
       <c r="F43" t="s">
-        <v>248</v>
+        <v>259</v>
       </c>
     </row>
     <row r="44" spans="1:6">
@@ -2005,16 +2047,16 @@
         <v>47</v>
       </c>
       <c r="C44" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="D44" t="s">
-        <v>197</v>
+        <v>204</v>
       </c>
       <c r="E44" t="s">
-        <v>232</v>
+        <v>244</v>
       </c>
       <c r="F44" t="s">
-        <v>245</v>
+        <v>259</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -2025,16 +2067,16 @@
         <v>48</v>
       </c>
       <c r="C45" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="D45" t="s">
-        <v>198</v>
+        <v>205</v>
       </c>
       <c r="E45" t="s">
-        <v>236</v>
+        <v>251</v>
       </c>
       <c r="F45" t="s">
-        <v>245</v>
+        <v>261</v>
       </c>
     </row>
     <row r="46" spans="1:6">
@@ -2045,16 +2087,16 @@
         <v>49</v>
       </c>
       <c r="C46" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="D46" t="s">
-        <v>199</v>
+        <v>206</v>
       </c>
       <c r="E46" t="s">
-        <v>232</v>
+        <v>245</v>
       </c>
       <c r="F46" t="s">
-        <v>245</v>
+        <v>261</v>
       </c>
     </row>
     <row r="47" spans="1:6">
@@ -2065,16 +2107,16 @@
         <v>50</v>
       </c>
       <c r="C47" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="D47" t="s">
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="E47" t="s">
-        <v>236</v>
+        <v>244</v>
       </c>
       <c r="F47" t="s">
-        <v>249</v>
+        <v>262</v>
       </c>
     </row>
     <row r="48" spans="1:6">
@@ -2085,16 +2127,16 @@
         <v>51</v>
       </c>
       <c r="C48" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="D48" t="s">
-        <v>201</v>
+        <v>208</v>
       </c>
       <c r="E48" t="s">
-        <v>233</v>
+        <v>244</v>
       </c>
       <c r="F48" t="s">
-        <v>245</v>
+        <v>259</v>
       </c>
     </row>
     <row r="49" spans="1:6">
@@ -2105,16 +2147,16 @@
         <v>52</v>
       </c>
       <c r="C49" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="D49" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="E49" t="s">
-        <v>236</v>
+        <v>249</v>
       </c>
       <c r="F49" t="s">
-        <v>245</v>
+        <v>259</v>
       </c>
     </row>
     <row r="50" spans="1:6">
@@ -2125,16 +2167,16 @@
         <v>53</v>
       </c>
       <c r="C50" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="D50" t="s">
-        <v>203</v>
+        <v>210</v>
       </c>
       <c r="E50" t="s">
-        <v>232</v>
+        <v>244</v>
       </c>
       <c r="F50" t="s">
-        <v>245</v>
+        <v>259</v>
       </c>
     </row>
     <row r="51" spans="1:6">
@@ -2145,16 +2187,16 @@
         <v>54</v>
       </c>
       <c r="C51" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="D51" t="s">
-        <v>195</v>
+        <v>211</v>
       </c>
       <c r="E51" t="s">
-        <v>233</v>
+        <v>249</v>
       </c>
       <c r="F51" t="s">
-        <v>244</v>
+        <v>263</v>
       </c>
     </row>
     <row r="52" spans="1:6">
@@ -2165,16 +2207,16 @@
         <v>55</v>
       </c>
       <c r="C52" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="D52" t="s">
-        <v>204</v>
+        <v>212</v>
       </c>
       <c r="E52" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
       <c r="F52" t="s">
-        <v>250</v>
+        <v>259</v>
       </c>
     </row>
     <row r="53" spans="1:6">
@@ -2185,16 +2227,16 @@
         <v>56</v>
       </c>
       <c r="C53" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="D53" t="s">
-        <v>205</v>
+        <v>213</v>
       </c>
       <c r="E53" t="s">
-        <v>232</v>
+        <v>249</v>
       </c>
       <c r="F53" t="s">
-        <v>242</v>
+        <v>259</v>
       </c>
     </row>
     <row r="54" spans="1:6">
@@ -2205,16 +2247,16 @@
         <v>57</v>
       </c>
       <c r="C54" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="D54" t="s">
-        <v>206</v>
+        <v>214</v>
       </c>
       <c r="E54" t="s">
-        <v>233</v>
+        <v>244</v>
       </c>
       <c r="F54" t="s">
-        <v>242</v>
+        <v>259</v>
       </c>
     </row>
     <row r="55" spans="1:6">
@@ -2225,16 +2267,16 @@
         <v>58</v>
       </c>
       <c r="C55" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="D55" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E55" t="s">
-        <v>232</v>
+        <v>245</v>
       </c>
       <c r="F55" t="s">
-        <v>245</v>
+        <v>258</v>
       </c>
     </row>
     <row r="56" spans="1:6">
@@ -2245,16 +2287,16 @@
         <v>59</v>
       </c>
       <c r="C56" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="D56" t="s">
-        <v>208</v>
+        <v>215</v>
       </c>
       <c r="E56" t="s">
-        <v>238</v>
+        <v>252</v>
       </c>
       <c r="F56" t="s">
-        <v>245</v>
+        <v>264</v>
       </c>
     </row>
     <row r="57" spans="1:6">
@@ -2265,16 +2307,16 @@
         <v>60</v>
       </c>
       <c r="C57" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="D57" t="s">
-        <v>209</v>
+        <v>216</v>
       </c>
       <c r="E57" t="s">
-        <v>233</v>
+        <v>244</v>
       </c>
       <c r="F57" t="s">
-        <v>245</v>
+        <v>256</v>
       </c>
     </row>
     <row r="58" spans="1:6">
@@ -2285,16 +2327,16 @@
         <v>61</v>
       </c>
       <c r="C58" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="D58" t="s">
-        <v>210</v>
+        <v>217</v>
       </c>
       <c r="E58" t="s">
-        <v>232</v>
+        <v>245</v>
       </c>
       <c r="F58" t="s">
-        <v>245</v>
+        <v>256</v>
       </c>
     </row>
     <row r="59" spans="1:6">
@@ -2305,16 +2347,16 @@
         <v>62</v>
       </c>
       <c r="C59" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="D59" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="E59" t="s">
-        <v>234</v>
+        <v>244</v>
       </c>
       <c r="F59" t="s">
-        <v>243</v>
+        <v>259</v>
       </c>
     </row>
     <row r="60" spans="1:6">
@@ -2325,16 +2367,16 @@
         <v>63</v>
       </c>
       <c r="C60" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="D60" t="s">
-        <v>212</v>
+        <v>219</v>
       </c>
       <c r="E60" t="s">
-        <v>236</v>
+        <v>251</v>
       </c>
       <c r="F60" t="s">
-        <v>245</v>
+        <v>259</v>
       </c>
     </row>
     <row r="61" spans="1:6">
@@ -2345,16 +2387,16 @@
         <v>64</v>
       </c>
       <c r="C61" t="s">
-        <v>126</v>
+        <v>143</v>
       </c>
       <c r="D61" t="s">
-        <v>213</v>
+        <v>220</v>
       </c>
       <c r="E61" t="s">
-        <v>233</v>
+        <v>245</v>
       </c>
       <c r="F61" t="s">
-        <v>243</v>
+        <v>259</v>
       </c>
     </row>
     <row r="62" spans="1:6">
@@ -2365,16 +2407,16 @@
         <v>65</v>
       </c>
       <c r="C62" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="D62" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="E62" t="s">
-        <v>233</v>
+        <v>244</v>
       </c>
       <c r="F62" t="s">
-        <v>245</v>
+        <v>259</v>
       </c>
     </row>
     <row r="63" spans="1:6">
@@ -2385,16 +2427,16 @@
         <v>66</v>
       </c>
       <c r="C63" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="D63" t="s">
-        <v>215</v>
+        <v>222</v>
       </c>
       <c r="E63" t="s">
-        <v>233</v>
+        <v>246</v>
       </c>
       <c r="F63" t="s">
-        <v>245</v>
+        <v>257</v>
       </c>
     </row>
     <row r="64" spans="1:6">
@@ -2405,16 +2447,16 @@
         <v>67</v>
       </c>
       <c r="C64" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="D64" t="s">
-        <v>216</v>
+        <v>223</v>
       </c>
       <c r="E64" t="s">
-        <v>233</v>
+        <v>249</v>
       </c>
       <c r="F64" t="s">
-        <v>242</v>
+        <v>259</v>
       </c>
     </row>
     <row r="65" spans="1:6">
@@ -2425,16 +2467,16 @@
         <v>68</v>
       </c>
       <c r="C65" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="D65" t="s">
-        <v>217</v>
+        <v>224</v>
       </c>
       <c r="E65" t="s">
-        <v>232</v>
+        <v>245</v>
       </c>
       <c r="F65" t="s">
-        <v>243</v>
+        <v>257</v>
       </c>
     </row>
     <row r="66" spans="1:6">
@@ -2445,16 +2487,16 @@
         <v>69</v>
       </c>
       <c r="C66" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="D66" t="s">
-        <v>218</v>
+        <v>225</v>
       </c>
       <c r="E66" t="s">
-        <v>233</v>
+        <v>245</v>
       </c>
       <c r="F66" t="s">
-        <v>247</v>
+        <v>259</v>
       </c>
     </row>
     <row r="67" spans="1:6">
@@ -2465,16 +2507,16 @@
         <v>70</v>
       </c>
       <c r="C67" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="D67" t="s">
-        <v>219</v>
+        <v>226</v>
       </c>
       <c r="E67" t="s">
-        <v>232</v>
+        <v>245</v>
       </c>
       <c r="F67" t="s">
-        <v>245</v>
+        <v>259</v>
       </c>
     </row>
     <row r="68" spans="1:6">
@@ -2485,16 +2527,16 @@
         <v>71</v>
       </c>
       <c r="C68" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="D68" t="s">
-        <v>220</v>
+        <v>227</v>
       </c>
       <c r="E68" t="s">
-        <v>232</v>
+        <v>245</v>
       </c>
       <c r="F68" t="s">
-        <v>245</v>
+        <v>256</v>
       </c>
     </row>
     <row r="69" spans="1:6">
@@ -2505,16 +2547,16 @@
         <v>72</v>
       </c>
       <c r="C69" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="D69" t="s">
-        <v>221</v>
+        <v>228</v>
       </c>
       <c r="E69" t="s">
-        <v>233</v>
+        <v>244</v>
       </c>
       <c r="F69" t="s">
-        <v>245</v>
+        <v>257</v>
       </c>
     </row>
     <row r="70" spans="1:6">
@@ -2525,16 +2567,16 @@
         <v>73</v>
       </c>
       <c r="C70" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="D70" t="s">
-        <v>222</v>
+        <v>229</v>
       </c>
       <c r="E70" t="s">
-        <v>232</v>
+        <v>245</v>
       </c>
       <c r="F70" t="s">
-        <v>242</v>
+        <v>261</v>
       </c>
     </row>
     <row r="71" spans="1:6">
@@ -2545,16 +2587,16 @@
         <v>74</v>
       </c>
       <c r="C71" t="s">
-        <v>74</v>
+        <v>152</v>
       </c>
       <c r="D71" t="s">
-        <v>223</v>
+        <v>230</v>
       </c>
       <c r="E71" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="F71" t="s">
-        <v>245</v>
+        <v>259</v>
       </c>
     </row>
     <row r="72" spans="1:6">
@@ -2565,16 +2607,16 @@
         <v>75</v>
       </c>
       <c r="C72" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="D72" t="s">
-        <v>224</v>
+        <v>231</v>
       </c>
       <c r="E72" t="s">
-        <v>234</v>
+        <v>244</v>
       </c>
       <c r="F72" t="s">
-        <v>251</v>
+        <v>259</v>
       </c>
     </row>
     <row r="73" spans="1:6">
@@ -2585,16 +2627,16 @@
         <v>76</v>
       </c>
       <c r="C73" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="D73" t="s">
-        <v>225</v>
+        <v>232</v>
       </c>
       <c r="E73" t="s">
-        <v>233</v>
+        <v>245</v>
       </c>
       <c r="F73" t="s">
-        <v>245</v>
+        <v>259</v>
       </c>
     </row>
     <row r="74" spans="1:6">
@@ -2605,16 +2647,16 @@
         <v>77</v>
       </c>
       <c r="C74" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="D74" t="s">
-        <v>226</v>
+        <v>233</v>
       </c>
       <c r="E74" t="s">
-        <v>233</v>
+        <v>244</v>
       </c>
       <c r="F74" t="s">
-        <v>243</v>
+        <v>256</v>
       </c>
     </row>
     <row r="75" spans="1:6">
@@ -2625,16 +2667,16 @@
         <v>78</v>
       </c>
       <c r="C75" t="s">
-        <v>152</v>
+        <v>78</v>
       </c>
       <c r="D75" t="s">
-        <v>227</v>
+        <v>234</v>
       </c>
       <c r="E75" t="s">
-        <v>233</v>
+        <v>253</v>
       </c>
       <c r="F75" t="s">
-        <v>245</v>
+        <v>256</v>
       </c>
     </row>
     <row r="76" spans="1:6">
@@ -2645,16 +2687,16 @@
         <v>79</v>
       </c>
       <c r="C76" t="s">
-        <v>105</v>
+        <v>79</v>
       </c>
       <c r="D76" t="s">
-        <v>228</v>
+        <v>235</v>
       </c>
       <c r="E76" t="s">
-        <v>232</v>
+        <v>254</v>
       </c>
       <c r="F76" t="s">
-        <v>242</v>
+        <v>259</v>
       </c>
     </row>
     <row r="77" spans="1:6">
@@ -2665,16 +2707,16 @@
         <v>80</v>
       </c>
       <c r="C77" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="D77" t="s">
-        <v>229</v>
+        <v>236</v>
       </c>
       <c r="E77" t="s">
-        <v>233</v>
+        <v>246</v>
       </c>
       <c r="F77" t="s">
-        <v>242</v>
+        <v>265</v>
       </c>
     </row>
     <row r="78" spans="1:6">
@@ -2685,16 +2727,16 @@
         <v>81</v>
       </c>
       <c r="C78" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="D78" t="s">
-        <v>230</v>
+        <v>237</v>
       </c>
       <c r="E78" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
       <c r="F78" t="s">
-        <v>251</v>
+        <v>259</v>
       </c>
     </row>
     <row r="79" spans="1:6">
@@ -2705,16 +2747,116 @@
         <v>82</v>
       </c>
       <c r="C79" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="D79" t="s">
-        <v>231</v>
+        <v>238</v>
       </c>
       <c r="E79" t="s">
+        <v>245</v>
+      </c>
+      <c r="F79" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6">
+      <c r="A80" s="1">
+        <v>79</v>
+      </c>
+      <c r="B80" t="s">
+        <v>83</v>
+      </c>
+      <c r="C80" t="s">
+        <v>159</v>
+      </c>
+      <c r="D80" t="s">
+        <v>239</v>
+      </c>
+      <c r="E80" t="s">
+        <v>245</v>
+      </c>
+      <c r="F80" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6">
+      <c r="A81" s="1">
+        <v>80</v>
+      </c>
+      <c r="B81" t="s">
+        <v>84</v>
+      </c>
+      <c r="C81" t="s">
+        <v>111</v>
+      </c>
+      <c r="D81" t="s">
+        <v>240</v>
+      </c>
+      <c r="E81" t="s">
+        <v>244</v>
+      </c>
+      <c r="F81" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6">
+      <c r="A82" s="1">
+        <v>81</v>
+      </c>
+      <c r="B82" t="s">
+        <v>85</v>
+      </c>
+      <c r="C82" t="s">
+        <v>160</v>
+      </c>
+      <c r="D82" t="s">
         <v>241</v>
       </c>
-      <c r="F79" t="s">
+      <c r="E82" t="s">
+        <v>245</v>
+      </c>
+      <c r="F82" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6">
+      <c r="A83" s="1">
+        <v>82</v>
+      </c>
+      <c r="B83" t="s">
+        <v>86</v>
+      </c>
+      <c r="C83" t="s">
+        <v>161</v>
+      </c>
+      <c r="D83" t="s">
         <v>242</v>
+      </c>
+      <c r="E83" t="s">
+        <v>252</v>
+      </c>
+      <c r="F83" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6">
+      <c r="A84" s="1">
+        <v>83</v>
+      </c>
+      <c r="B84" t="s">
+        <v>87</v>
+      </c>
+      <c r="C84" t="s">
+        <v>162</v>
+      </c>
+      <c r="D84" t="s">
+        <v>243</v>
+      </c>
+      <c r="E84" t="s">
+        <v>255</v>
+      </c>
+      <c r="F84" t="s">
+        <v>256</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated on 2019-01-03 at 00:47:37
</commit_message>
<xml_diff>
--- a/index.xlsx
+++ b/index.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="268">
   <si>
     <t>Song Title</t>
   </si>
@@ -43,6 +43,9 @@
     <t>Alone</t>
   </si>
   <si>
+    <t>thank u, next</t>
+  </si>
+  <si>
     <t>Astronomia</t>
   </si>
   <si>
@@ -514,6 +517,9 @@
     <t>Alan Walker, Noonie Bao</t>
   </si>
   <si>
+    <t>Ariana Grande</t>
+  </si>
+  <si>
     <t>Tony Igy</t>
   </si>
   <si>
@@ -790,10 +796,10 @@
     <t>2016</t>
   </si>
   <si>
+    <t>2018</t>
+  </si>
+  <si>
     <t>2010</t>
-  </si>
-  <si>
-    <t>2018</t>
   </si>
   <si>
     <t>2011</t>
@@ -1169,7 +1175,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F84"/>
+  <dimension ref="A1:F85"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1207,16 +1213,16 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D2" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="E2" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="F2" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -1227,16 +1233,16 @@
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D3" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E3" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="F3" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -1247,16 +1253,16 @@
         <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D4" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="E4" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="F4" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -1267,16 +1273,16 @@
         <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D5" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E5" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="F5" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -1287,16 +1293,16 @@
         <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>92</v>
+        <v>9</v>
       </c>
       <c r="D6" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="E6" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="F6" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -1310,13 +1316,13 @@
         <v>93</v>
       </c>
       <c r="D7" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="E7" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="F7" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -1330,13 +1336,13 @@
         <v>94</v>
       </c>
       <c r="D8" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E8" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="F8" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -1350,13 +1356,13 @@
         <v>95</v>
       </c>
       <c r="D9" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="E9" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="F9" t="s">
-        <v>256</v>
+        <v>260</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -1370,13 +1376,13 @@
         <v>96</v>
       </c>
       <c r="D10" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="E10" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="F10" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -1390,13 +1396,13 @@
         <v>97</v>
       </c>
       <c r="D11" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="E11" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="F11" t="s">
-        <v>133</v>
+        <v>258</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -1407,16 +1413,16 @@
         <v>15</v>
       </c>
       <c r="C12" t="s">
-        <v>15</v>
+        <v>98</v>
       </c>
       <c r="D12" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="E12" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="F12" t="s">
-        <v>259</v>
+        <v>134</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -1427,16 +1433,16 @@
         <v>16</v>
       </c>
       <c r="C13" t="s">
-        <v>98</v>
+        <v>16</v>
       </c>
       <c r="D13" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="E13" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="F13" t="s">
-        <v>256</v>
+        <v>260</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -1450,13 +1456,13 @@
         <v>99</v>
       </c>
       <c r="D14" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="E14" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="F14" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -1470,7 +1476,7 @@
         <v>100</v>
       </c>
       <c r="D15" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E15" t="s">
         <v>247</v>
@@ -1490,13 +1496,13 @@
         <v>101</v>
       </c>
       <c r="D16" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="E16" t="s">
-        <v>244</v>
+        <v>249</v>
       </c>
       <c r="F16" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -1510,13 +1516,13 @@
         <v>102</v>
       </c>
       <c r="D17" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="E17" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="F17" t="s">
-        <v>256</v>
+        <v>260</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -1530,13 +1536,13 @@
         <v>103</v>
       </c>
       <c r="D18" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="E18" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="F18" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -1550,13 +1556,13 @@
         <v>104</v>
       </c>
       <c r="D19" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="E19" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="F19" t="s">
-        <v>259</v>
+        <v>263</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -1567,16 +1573,16 @@
         <v>23</v>
       </c>
       <c r="C20" t="s">
-        <v>23</v>
+        <v>105</v>
       </c>
       <c r="D20" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="E20" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="F20" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -1587,16 +1593,16 @@
         <v>24</v>
       </c>
       <c r="C21" t="s">
-        <v>105</v>
+        <v>24</v>
       </c>
       <c r="D21" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="E21" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="F21" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -1607,16 +1613,16 @@
         <v>25</v>
       </c>
       <c r="C22" t="s">
-        <v>25</v>
+        <v>106</v>
       </c>
       <c r="D22" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="E22" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="F22" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -1627,16 +1633,16 @@
         <v>26</v>
       </c>
       <c r="C23" t="s">
-        <v>106</v>
+        <v>26</v>
       </c>
       <c r="D23" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="E23" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="F23" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -1647,16 +1653,16 @@
         <v>27</v>
       </c>
       <c r="C24" t="s">
-        <v>27</v>
+        <v>107</v>
       </c>
       <c r="D24" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="E24" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="F24" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -1667,16 +1673,16 @@
         <v>28</v>
       </c>
       <c r="C25" t="s">
-        <v>107</v>
+        <v>28</v>
       </c>
       <c r="D25" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="E25" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="F25" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -1690,13 +1696,13 @@
         <v>108</v>
       </c>
       <c r="D26" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="E26" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="F26" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -1710,13 +1716,13 @@
         <v>109</v>
       </c>
       <c r="D27" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="E27" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="F27" t="s">
-        <v>259</v>
+        <v>263</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -1730,13 +1736,13 @@
         <v>110</v>
       </c>
       <c r="D28" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="E28" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="F28" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -1750,13 +1756,13 @@
         <v>111</v>
       </c>
       <c r="D29" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="E29" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="F29" t="s">
-        <v>256</v>
+        <v>260</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -1770,13 +1776,13 @@
         <v>112</v>
       </c>
       <c r="D30" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="E30" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="F30" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -1790,13 +1796,13 @@
         <v>113</v>
       </c>
       <c r="D31" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="E31" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="F31" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -1810,13 +1816,13 @@
         <v>114</v>
       </c>
       <c r="D32" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="E32" t="s">
-        <v>245</v>
+        <v>250</v>
       </c>
       <c r="F32" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -1830,13 +1836,13 @@
         <v>115</v>
       </c>
       <c r="D33" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="E33" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="F33" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -1850,13 +1856,13 @@
         <v>116</v>
       </c>
       <c r="D34" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="E34" t="s">
-        <v>244</v>
+        <v>251</v>
       </c>
       <c r="F34" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -1870,13 +1876,13 @@
         <v>117</v>
       </c>
       <c r="D35" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E35" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="F35" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -1890,13 +1896,13 @@
         <v>118</v>
       </c>
       <c r="D36" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="E36" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="F36" t="s">
-        <v>256</v>
+        <v>260</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -1910,13 +1916,13 @@
         <v>119</v>
       </c>
       <c r="D37" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="E37" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="F37" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -1930,13 +1936,13 @@
         <v>120</v>
       </c>
       <c r="D38" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="E38" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="F38" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -1950,13 +1956,13 @@
         <v>121</v>
       </c>
       <c r="D39" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="E39" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="F39" t="s">
-        <v>133</v>
+        <v>260</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -1970,13 +1976,13 @@
         <v>122</v>
       </c>
       <c r="D40" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="E40" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="F40" t="s">
-        <v>256</v>
+        <v>134</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -1990,13 +1996,13 @@
         <v>123</v>
       </c>
       <c r="D41" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="E41" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="F41" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -2010,13 +2016,13 @@
         <v>124</v>
       </c>
       <c r="D42" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="E42" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="F42" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -2030,10 +2036,10 @@
         <v>125</v>
       </c>
       <c r="D43" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="E43" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="F43" t="s">
         <v>259</v>
@@ -2050,13 +2056,13 @@
         <v>126</v>
       </c>
       <c r="D44" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="E44" t="s">
-        <v>244</v>
+        <v>252</v>
       </c>
       <c r="F44" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -2070,13 +2076,13 @@
         <v>127</v>
       </c>
       <c r="D45" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E45" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="F45" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="46" spans="1:6">
@@ -2090,13 +2096,13 @@
         <v>128</v>
       </c>
       <c r="D46" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="E46" t="s">
-        <v>245</v>
+        <v>253</v>
       </c>
       <c r="F46" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
     </row>
     <row r="47" spans="1:6">
@@ -2110,13 +2116,13 @@
         <v>129</v>
       </c>
       <c r="D47" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="E47" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="F47" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="48" spans="1:6">
@@ -2130,13 +2136,13 @@
         <v>130</v>
       </c>
       <c r="D48" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="E48" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="F48" t="s">
-        <v>259</v>
+        <v>264</v>
       </c>
     </row>
     <row r="49" spans="1:6">
@@ -2150,13 +2156,13 @@
         <v>131</v>
       </c>
       <c r="D49" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="E49" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="F49" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="50" spans="1:6">
@@ -2170,13 +2176,13 @@
         <v>132</v>
       </c>
       <c r="D50" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="E50" t="s">
-        <v>244</v>
+        <v>251</v>
       </c>
       <c r="F50" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="51" spans="1:6">
@@ -2190,13 +2196,13 @@
         <v>133</v>
       </c>
       <c r="D51" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="E51" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="F51" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
     </row>
     <row r="52" spans="1:6">
@@ -2210,13 +2216,13 @@
         <v>134</v>
       </c>
       <c r="D52" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E52" t="s">
-        <v>245</v>
+        <v>251</v>
       </c>
       <c r="F52" t="s">
-        <v>259</v>
+        <v>265</v>
       </c>
     </row>
     <row r="53" spans="1:6">
@@ -2230,13 +2236,13 @@
         <v>135</v>
       </c>
       <c r="D53" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="E53" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="F53" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="54" spans="1:6">
@@ -2250,13 +2256,13 @@
         <v>136</v>
       </c>
       <c r="D54" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="E54" t="s">
-        <v>244</v>
+        <v>251</v>
       </c>
       <c r="F54" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="55" spans="1:6">
@@ -2270,13 +2276,13 @@
         <v>137</v>
       </c>
       <c r="D55" t="s">
-        <v>206</v>
+        <v>216</v>
       </c>
       <c r="E55" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="F55" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
     </row>
     <row r="56" spans="1:6">
@@ -2290,13 +2296,13 @@
         <v>138</v>
       </c>
       <c r="D56" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="E56" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="F56" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
     </row>
     <row r="57" spans="1:6">
@@ -2310,13 +2316,13 @@
         <v>139</v>
       </c>
       <c r="D57" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="E57" t="s">
-        <v>244</v>
+        <v>254</v>
       </c>
       <c r="F57" t="s">
-        <v>256</v>
+        <v>266</v>
       </c>
     </row>
     <row r="58" spans="1:6">
@@ -2330,13 +2336,13 @@
         <v>140</v>
       </c>
       <c r="D58" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="E58" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="F58" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
     </row>
     <row r="59" spans="1:6">
@@ -2350,13 +2356,13 @@
         <v>141</v>
       </c>
       <c r="D59" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="E59" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="F59" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="60" spans="1:6">
@@ -2370,13 +2376,13 @@
         <v>142</v>
       </c>
       <c r="D60" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="E60" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="F60" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="61" spans="1:6">
@@ -2390,13 +2396,13 @@
         <v>143</v>
       </c>
       <c r="D61" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="E61" t="s">
-        <v>245</v>
+        <v>253</v>
       </c>
       <c r="F61" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="62" spans="1:6">
@@ -2410,13 +2416,13 @@
         <v>144</v>
       </c>
       <c r="D62" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="E62" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="F62" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="63" spans="1:6">
@@ -2430,13 +2436,13 @@
         <v>145</v>
       </c>
       <c r="D63" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="E63" t="s">
         <v>246</v>
       </c>
       <c r="F63" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
     </row>
     <row r="64" spans="1:6">
@@ -2450,10 +2456,10 @@
         <v>146</v>
       </c>
       <c r="D64" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="E64" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="F64" t="s">
         <v>259</v>
@@ -2467,16 +2473,16 @@
         <v>68</v>
       </c>
       <c r="C65" t="s">
-        <v>133</v>
+        <v>147</v>
       </c>
       <c r="D65" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="E65" t="s">
-        <v>245</v>
+        <v>251</v>
       </c>
       <c r="F65" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
     </row>
     <row r="66" spans="1:6">
@@ -2487,13 +2493,13 @@
         <v>69</v>
       </c>
       <c r="C66" t="s">
-        <v>147</v>
+        <v>134</v>
       </c>
       <c r="D66" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="E66" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="F66" t="s">
         <v>259</v>
@@ -2510,13 +2516,13 @@
         <v>148</v>
       </c>
       <c r="D67" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="E67" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="F67" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="68" spans="1:6">
@@ -2530,13 +2536,13 @@
         <v>149</v>
       </c>
       <c r="D68" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="E68" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="F68" t="s">
-        <v>256</v>
+        <v>260</v>
       </c>
     </row>
     <row r="69" spans="1:6">
@@ -2550,13 +2556,13 @@
         <v>150</v>
       </c>
       <c r="D69" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="E69" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="F69" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
     <row r="70" spans="1:6">
@@ -2570,13 +2576,13 @@
         <v>151</v>
       </c>
       <c r="D70" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="E70" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="F70" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="71" spans="1:6">
@@ -2590,13 +2596,13 @@
         <v>152</v>
       </c>
       <c r="D71" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="E71" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="F71" t="s">
-        <v>259</v>
+        <v>263</v>
       </c>
     </row>
     <row r="72" spans="1:6">
@@ -2610,13 +2616,13 @@
         <v>153</v>
       </c>
       <c r="D72" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="E72" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="F72" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="73" spans="1:6">
@@ -2630,13 +2636,13 @@
         <v>154</v>
       </c>
       <c r="D73" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="E73" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="F73" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="74" spans="1:6">
@@ -2650,13 +2656,13 @@
         <v>155</v>
       </c>
       <c r="D74" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="E74" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="F74" t="s">
-        <v>256</v>
+        <v>260</v>
       </c>
     </row>
     <row r="75" spans="1:6">
@@ -2667,16 +2673,16 @@
         <v>78</v>
       </c>
       <c r="C75" t="s">
-        <v>78</v>
+        <v>156</v>
       </c>
       <c r="D75" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="E75" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="F75" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
     </row>
     <row r="76" spans="1:6">
@@ -2690,13 +2696,13 @@
         <v>79</v>
       </c>
       <c r="D76" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="E76" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="F76" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="77" spans="1:6">
@@ -2707,16 +2713,16 @@
         <v>80</v>
       </c>
       <c r="C77" t="s">
-        <v>156</v>
+        <v>80</v>
       </c>
       <c r="D77" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="E77" t="s">
-        <v>246</v>
+        <v>256</v>
       </c>
       <c r="F77" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
     </row>
     <row r="78" spans="1:6">
@@ -2730,13 +2736,13 @@
         <v>157</v>
       </c>
       <c r="D78" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="E78" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="F78" t="s">
-        <v>259</v>
+        <v>267</v>
       </c>
     </row>
     <row r="79" spans="1:6">
@@ -2750,13 +2756,13 @@
         <v>158</v>
       </c>
       <c r="D79" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="E79" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="F79" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
     </row>
     <row r="80" spans="1:6">
@@ -2770,10 +2776,10 @@
         <v>159</v>
       </c>
       <c r="D80" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="E80" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="F80" t="s">
         <v>259</v>
@@ -2787,16 +2793,16 @@
         <v>84</v>
       </c>
       <c r="C81" t="s">
-        <v>111</v>
+        <v>160</v>
       </c>
       <c r="D81" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="E81" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="F81" t="s">
-        <v>256</v>
+        <v>260</v>
       </c>
     </row>
     <row r="82" spans="1:6">
@@ -2807,16 +2813,16 @@
         <v>85</v>
       </c>
       <c r="C82" t="s">
-        <v>160</v>
+        <v>112</v>
       </c>
       <c r="D82" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="E82" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="F82" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
     </row>
     <row r="83" spans="1:6">
@@ -2830,13 +2836,13 @@
         <v>161</v>
       </c>
       <c r="D83" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="E83" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="F83" t="s">
-        <v>265</v>
+        <v>258</v>
       </c>
     </row>
     <row r="84" spans="1:6">
@@ -2850,13 +2856,33 @@
         <v>162</v>
       </c>
       <c r="D84" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="E84" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="F84" t="s">
-        <v>256</v>
+        <v>267</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6">
+      <c r="A85" s="1">
+        <v>84</v>
+      </c>
+      <c r="B85" t="s">
+        <v>88</v>
+      </c>
+      <c r="C85" t="s">
+        <v>163</v>
+      </c>
+      <c r="D85" t="s">
+        <v>245</v>
+      </c>
+      <c r="E85" t="s">
+        <v>257</v>
+      </c>
+      <c r="F85" t="s">
+        <v>258</v>
       </c>
     </row>
   </sheetData>

</xml_diff>